<commit_message>
RDM-12681 - Fully populated fairweather XLS and JSON files
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D6FD54-F4F0-8E41-9540-9A233DB70960}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9773FC08-A4F2-2746-80FC-4BE49008C022}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="20500" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -51313,7 +51313,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -51339,7 +51339,7 @@
       <c r="G1" s="380"/>
       <c r="H1" s="380"/>
     </row>
-    <row r="2" spans="1:8" s="595" customFormat="1" ht="238">
+    <row r="2" spans="1:8" s="595" customFormat="1" ht="182">
       <c r="A2" s="593" t="s">
         <v>1253</v>
       </c>
@@ -51397,22 +51397,22 @@
       </c>
       <c r="B4" s="380"/>
       <c r="C4" s="597" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="D4" s="597" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
       <c r="E4" s="597" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
       <c r="F4" s="597" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
       <c r="G4" s="597" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
       <c r="H4" s="597" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -53175,8 +53175,8 @@
   <dimension ref="A1:IO194"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C50" sqref="C50:D56"/>
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C27:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>

</xml_diff>

<commit_message>
RDM-12681 - unhide all tabs in excel files
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9773FC08-A4F2-2746-80FC-4BE49008C022}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC1D7F2-495E-E34A-8529-45528C99A65F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -20,25 +20,25 @@
     <sheet name="Category" sheetId="23" r:id="rId5"/>
     <sheet name="CaseField" sheetId="3" r:id="rId6"/>
     <sheet name="ComplexTypes" sheetId="4" r:id="rId7"/>
-    <sheet name="AuthorisationComplexType" sheetId="21" state="hidden" r:id="rId8"/>
-    <sheet name="EventToComplexTypes" sheetId="20" state="hidden" r:id="rId9"/>
-    <sheet name="FixedLists" sheetId="5" state="hidden" r:id="rId10"/>
-    <sheet name="CaseTypeTab" sheetId="6" state="hidden" r:id="rId11"/>
-    <sheet name="State" sheetId="7" state="hidden" r:id="rId12"/>
-    <sheet name="CaseEvent" sheetId="8" state="hidden" r:id="rId13"/>
-    <sheet name="CaseEventToFields" sheetId="9" state="hidden" r:id="rId14"/>
-    <sheet name="SearchInputFields" sheetId="10" state="hidden" r:id="rId15"/>
-    <sheet name="SearchCasesResultFields" sheetId="25" state="hidden" r:id="rId16"/>
-    <sheet name="SearchResultFields" sheetId="11" state="hidden" r:id="rId17"/>
-    <sheet name="WorkBasketInputFields" sheetId="12" state="hidden" r:id="rId18"/>
-    <sheet name="WorkBasketResultFields" sheetId="13" state="hidden" r:id="rId19"/>
-    <sheet name="UserProfile" sheetId="14" state="hidden" r:id="rId20"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" state="hidden" r:id="rId21"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" state="hidden" r:id="rId22"/>
-    <sheet name="CaseRoles" sheetId="19" state="hidden" r:id="rId23"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" state="hidden" r:id="rId24"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" state="hidden" r:id="rId25"/>
-    <sheet name="RoleToAccessProfiles" sheetId="27" state="hidden" r:id="rId26"/>
+    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId8"/>
+    <sheet name="EventToComplexTypes" sheetId="20" r:id="rId9"/>
+    <sheet name="FixedLists" sheetId="5" r:id="rId10"/>
+    <sheet name="CaseTypeTab" sheetId="6" r:id="rId11"/>
+    <sheet name="State" sheetId="7" r:id="rId12"/>
+    <sheet name="CaseEvent" sheetId="8" r:id="rId13"/>
+    <sheet name="CaseEventToFields" sheetId="9" r:id="rId14"/>
+    <sheet name="SearchInputFields" sheetId="10" r:id="rId15"/>
+    <sheet name="SearchCasesResultFields" sheetId="25" r:id="rId16"/>
+    <sheet name="SearchResultFields" sheetId="11" r:id="rId17"/>
+    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId18"/>
+    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId19"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId20"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId21"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId22"/>
+    <sheet name="CaseRoles" sheetId="19" r:id="rId23"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId24"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId25"/>
+    <sheet name="RoleToAccessProfiles" sheetId="27" r:id="rId26"/>
     <sheet name="SearchParty" sheetId="30" r:id="rId27"/>
   </sheets>
   <externalReferences>
@@ -41200,7 +41200,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
@@ -41320,7 +41320,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -49212,7 +49212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:CF64"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
@@ -51312,8 +51312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B2520D-B5D1-6249-96E1-C392AB55B40B}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -51837,7 +51837,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -52555,7 +52555,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -52925,7 +52925,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -53176,7 +53176,8 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C27:G32"/>
+      <selection activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -61213,7 +61214,7 @@
   <dimension ref="A1:T90"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>

</xml_diff>

<commit_message>
RDM-12680 - Add valid and invalid test definitions. Add Search Criteria json
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC1D7F2-495E-E34A-8529-45528C99A65F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BAFC04-FC08-674C-BF15-64E8380C9354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24520" windowHeight="19060" firstSheet="22" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,10 @@
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId25"/>
     <sheet name="RoleToAccessProfiles" sheetId="27" r:id="rId26"/>
     <sheet name="SearchParty" sheetId="30" r:id="rId27"/>
+    <sheet name="SearchCriteria" sheetId="31" r:id="rId28"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId28"/>
+    <externalReference r:id="rId29"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">CaseEvent!$A$22:$V$22</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9853" uniqueCount="1266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9873" uniqueCount="1269">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3942,6 +3943,16 @@
   </si>
   <si>
     <t>AddressComplex1.AddressLine1</t>
+  </si>
+  <si>
+    <t>SearchCriteria</t>
+  </si>
+  <si>
+    <t>OtherCaseReference</t>
+  </si>
+  <si>
+    <t>A complex types that make up the Other Case Reference.
+Max Length: 200</t>
   </si>
 </sst>
 </file>
@@ -17258,8 +17269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:CR96"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G82" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -49212,7 +49223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:CF64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
@@ -51312,8 +51323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B2520D-B5D1-6249-96E1-C392AB55B40B}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -51829,6 +51840,248 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78534859-F064-B543-88B4-7FD2D061D929}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.6640625" customWidth="1"/>
+    <col min="5" max="8" width="26.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18">
+      <c r="A1" s="596" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B1" s="380"/>
+      <c r="C1" s="380"/>
+      <c r="D1" s="380"/>
+    </row>
+    <row r="2" spans="1:4" ht="84">
+      <c r="A2" s="593" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B2" s="594" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C2" s="593" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D2" s="594" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="598" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="598" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="598" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D3" s="598" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="109">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="380"/>
+      <c r="C4" s="597" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="597" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="109">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="380"/>
+      <c r="C5" s="597" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="597" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="109">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="380"/>
+      <c r="C6" s="597" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="597" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="109">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="380"/>
+      <c r="C7" s="597" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="597" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="109">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="380"/>
+      <c r="C8" s="597" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="555" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="109">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="380"/>
+      <c r="C9" s="597" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="380"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="109"/>
+      <c r="B10" s="380"/>
+      <c r="C10" s="597"/>
+      <c r="D10" s="380"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="109"/>
+      <c r="B11" s="380"/>
+      <c r="C11" s="597"/>
+      <c r="D11" s="380"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="109"/>
+      <c r="B12" s="380"/>
+      <c r="C12" s="597"/>
+      <c r="D12" s="380"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="120"/>
+      <c r="B13" s="601"/>
+      <c r="C13" s="601"/>
+      <c r="D13" s="380"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="109"/>
+      <c r="B14" s="380"/>
+      <c r="C14" s="597"/>
+      <c r="D14" s="380"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="109"/>
+      <c r="B15" s="380"/>
+      <c r="C15" s="597"/>
+      <c r="D15" s="380"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="109"/>
+      <c r="B16" s="380"/>
+      <c r="C16" s="597"/>
+      <c r="D16" s="380"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="109"/>
+      <c r="B17" s="380"/>
+      <c r="C17" s="380"/>
+      <c r="D17" s="380"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="380"/>
+      <c r="B18" s="380"/>
+      <c r="C18" s="380"/>
+      <c r="D18" s="380"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="380"/>
+      <c r="B19" s="380"/>
+      <c r="C19" s="380"/>
+      <c r="D19" s="380"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="380"/>
+      <c r="B20" s="380"/>
+      <c r="C20" s="380"/>
+      <c r="D20" s="380"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="380"/>
+      <c r="B21" s="380"/>
+      <c r="C21" s="380"/>
+      <c r="D21" s="380"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="380"/>
+      <c r="B22" s="380"/>
+      <c r="C22" s="380"/>
+      <c r="D22" s="380"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="380"/>
+      <c r="B23" s="380"/>
+      <c r="C23" s="380"/>
+      <c r="D23" s="380"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="380"/>
+      <c r="B24" s="380"/>
+      <c r="C24" s="380"/>
+      <c r="D24" s="380"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="380"/>
+      <c r="B25" s="380"/>
+      <c r="C25" s="380"/>
+      <c r="D25" s="380"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="380"/>
+      <c r="B26" s="380"/>
+      <c r="C26" s="380"/>
+      <c r="D26" s="380"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="380"/>
+      <c r="B27" s="380"/>
+      <c r="C27" s="380"/>
+      <c r="D27" s="380"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="380"/>
+      <c r="B28" s="380"/>
+      <c r="C28" s="380"/>
+      <c r="D28" s="380"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
RDM-12680 - Update spreadsheets with correct values for FTA tests
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BAFC04-FC08-674C-BF15-64E8380C9354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DE9958-82C2-B743-A977-E40D6F7A5BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24520" windowHeight="19060" firstSheet="22" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1760" yWindow="820" windowWidth="31120" windowHeight="18640" firstSheet="19" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9873" uniqueCount="1269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9875" uniqueCount="1269">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -51323,13 +51323,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B2520D-B5D1-6249-96E1-C392AB55B40B}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
     <col min="4" max="4" width="79.83203125" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
@@ -51848,7 +51848,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -51953,7 +51953,7 @@
         <v>61</v>
       </c>
       <c r="D8" s="555" t="s">
-        <v>165</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -51967,21 +51967,27 @@
       <c r="D9" s="380"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="109"/>
+      <c r="A10" s="109">
+        <v>42736</v>
+      </c>
       <c r="B10" s="380"/>
-      <c r="C10" s="597"/>
-      <c r="D10" s="380"/>
+      <c r="C10" s="597" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="597" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="109"/>
+      <c r="A11" s="380"/>
       <c r="B11" s="380"/>
-      <c r="C11" s="597"/>
+      <c r="C11" s="380"/>
       <c r="D11" s="380"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="109"/>
+      <c r="A12" s="380"/>
       <c r="B12" s="380"/>
-      <c r="C12" s="597"/>
+      <c r="C12" s="380"/>
       <c r="D12" s="380"/>
     </row>
     <row r="13" spans="1:4">
@@ -51991,25 +51997,25 @@
       <c r="D13" s="380"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="109"/>
+      <c r="A14" s="380"/>
       <c r="B14" s="380"/>
-      <c r="C14" s="597"/>
+      <c r="C14" s="380"/>
       <c r="D14" s="380"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="109"/>
+      <c r="A15" s="380"/>
       <c r="B15" s="380"/>
-      <c r="C15" s="597"/>
+      <c r="C15" s="380"/>
       <c r="D15" s="380"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="109"/>
+      <c r="A16" s="380"/>
       <c r="B16" s="380"/>
-      <c r="C16" s="597"/>
+      <c r="C16" s="380"/>
       <c r="D16" s="380"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="109"/>
+      <c r="A17" s="380"/>
       <c r="B17" s="380"/>
       <c r="C17" s="380"/>
       <c r="D17" s="380"/>
@@ -53428,9 +53434,9 @@
   <dimension ref="A1:IO194"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C5" sqref="C5"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -61466,8 +61472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T90"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -62003,7 +62009,7 @@
         <v>42736</v>
       </c>
       <c r="B15" s="53"/>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="57" t="s">
         <v>443</v>
       </c>
       <c r="D15" s="54" t="s">

</xml_diff>

<commit_message>
RDM-12828 - Update description for TTLIncrement
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE40734-46CB-6B4F-9422-22A5B478E729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928A2515-2273-B348-B4B9-02F469CA1BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9864" uniqueCount="1259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9864" uniqueCount="1260">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3923,6 +3923,10 @@
   </si>
   <si>
     <t>TTLIncrement</t>
+  </si>
+  <si>
+    <t>Integer value that if present identifies that the event is one that should set the TTL.SystemTTL (to today + the TTLIncrement)
+MaxLength: &lt;unlimited&gt;</t>
   </si>
 </sst>
 </file>
@@ -22104,8 +22108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y78" sqref="Y78"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -22131,7 +22135,7 @@
     <col min="19" max="20" width="18.5" style="6" customWidth="1"/>
     <col min="21" max="21" width="16.83203125" style="16" customWidth="1"/>
     <col min="22" max="22" width="16.83203125" style="6" customWidth="1"/>
-    <col min="23" max="23" width="16.83203125" style="16" customWidth="1"/>
+    <col min="23" max="23" width="20.83203125" style="16" customWidth="1"/>
     <col min="24" max="258" width="8.83203125" style="19" customWidth="1"/>
     <col min="259" max="16384" width="8.83203125" style="19"/>
   </cols>
@@ -22237,7 +22241,7 @@
         <v>908</v>
       </c>
       <c r="W2" s="482" t="s">
-        <v>908</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="333" customFormat="1" ht="20" customHeight="1">

</xml_diff>

<commit_message>
add dod to global search casetype
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleynoronha/code/ccd/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7A9505-0531-1140-A005-4A43731E8214}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4EA5CA-C132-0E45-B3C1-872404963541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="16" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="16" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10146" uniqueCount="1278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10162" uniqueCount="1280">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3980,6 +3980,12 @@
   <si>
     <t>A complex types that make up the Other Case Reference.
 Max Length: 200</t>
+  </si>
+  <si>
+    <t>DateOfDeath</t>
+  </si>
+  <si>
+    <t>SearchPartyDOD</t>
   </si>
 </sst>
 </file>
@@ -43290,10 +43296,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F283"/>
+  <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A266" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C288" sqref="C288"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A262" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D277" sqref="D277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -48286,10 +48292,10 @@
         <v>1252</v>
       </c>
       <c r="D277" s="57" t="s">
-        <v>1254</v>
-      </c>
-      <c r="E277" s="102" t="s">
-        <v>1200</v>
+        <v>1278</v>
+      </c>
+      <c r="E277" s="72" t="s">
+        <v>584</v>
       </c>
       <c r="F277" s="99" t="s">
         <v>583</v>
@@ -48304,7 +48310,7 @@
         <v>1252</v>
       </c>
       <c r="D278" s="57" t="s">
-        <v>445</v>
+        <v>1254</v>
       </c>
       <c r="E278" s="102" t="s">
         <v>1200</v>
@@ -48322,7 +48328,7 @@
         <v>1252</v>
       </c>
       <c r="D279" s="57" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E279" s="102" t="s">
         <v>1200</v>
@@ -48340,7 +48346,7 @@
         <v>1252</v>
       </c>
       <c r="D280" s="57" t="s">
-        <v>177</v>
+        <v>449</v>
       </c>
       <c r="E280" s="102" t="s">
         <v>1200</v>
@@ -48358,7 +48364,7 @@
         <v>1252</v>
       </c>
       <c r="D281" s="57" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
       <c r="E281" s="102" t="s">
         <v>1200</v>
@@ -48376,7 +48382,7 @@
         <v>1252</v>
       </c>
       <c r="D282" s="57" t="s">
-        <v>674</v>
+        <v>212</v>
       </c>
       <c r="E282" s="102" t="s">
         <v>1200</v>
@@ -48394,12 +48400,48 @@
         <v>1252</v>
       </c>
       <c r="D283" s="57" t="s">
-        <v>450</v>
+        <v>674</v>
       </c>
       <c r="E283" s="102" t="s">
         <v>1200</v>
       </c>
       <c r="F283" s="99" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" s="333" customFormat="1" ht="20" customHeight="1">
+      <c r="A284" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B284" s="53"/>
+      <c r="C284" s="57" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D284" s="57" t="s">
+        <v>450</v>
+      </c>
+      <c r="E284" s="102" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F284" s="99" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" s="333" customFormat="1" ht="20" customHeight="1">
+      <c r="A285" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B285" s="53"/>
+      <c r="C285" s="57" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D285" s="57" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E285" s="102" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F285" s="99" t="s">
         <v>583</v>
       </c>
     </row>
@@ -52986,10 +53028,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778BCCC1-48D7-FA41-814D-66E309A10BB8}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -53001,7 +53043,7 @@
     <col min="5" max="8" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="599" t="s">
         <v>1255</v>
       </c>
@@ -53013,7 +53055,7 @@
       <c r="G1" s="380"/>
       <c r="H1" s="380"/>
     </row>
-    <row r="2" spans="1:8" ht="126">
+    <row r="2" spans="1:9" ht="126">
       <c r="A2" s="600" t="s">
         <v>1256</v>
       </c>
@@ -53039,7 +53081,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="602" t="s">
         <v>9</v>
       </c>
@@ -53064,8 +53106,11 @@
       <c r="H3" s="602" t="s">
         <v>1269</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="602" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="556">
         <v>42736</v>
       </c>
@@ -53089,7 +53134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="556">
         <v>42736</v>
       </c>
@@ -53113,7 +53158,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="556">
         <v>42736</v>
       </c>
@@ -53137,7 +53182,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="556">
         <v>42736</v>
       </c>
@@ -53161,7 +53206,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="556">
         <v>42736</v>
       </c>
@@ -53185,7 +53230,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="556">
         <v>42736</v>
       </c>
@@ -53209,7 +53254,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="556">
         <v>42736</v>
       </c>
@@ -53233,7 +53278,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="556">
         <v>42736</v>
       </c>
@@ -53257,7 +53302,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="556">
         <v>42736</v>
       </c>
@@ -53281,7 +53326,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="598">
         <v>42736</v>
       </c>
@@ -53303,7 +53348,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="556">
         <v>42736</v>
       </c>
@@ -53325,7 +53370,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="556">
         <v>42736</v>
       </c>
@@ -53347,7 +53392,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="556">
         <v>42736</v>
       </c>
@@ -53369,7 +53414,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" s="556">
         <v>42736</v>
       </c>
@@ -53390,7 +53435,7 @@
       </c>
       <c r="H17" s="380"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="556">
         <v>42736</v>
       </c>
@@ -53411,6 +53456,9 @@
       </c>
       <c r="H18" s="380" t="s">
         <v>450</v>
+      </c>
+      <c r="I18" s="603" t="s">
+        <v>1278</v>
       </c>
     </row>
   </sheetData>
@@ -53422,8 +53470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662D18BA-BEA0-DA4A-8F67-416A693D549E}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -54562,11 +54610,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IO201"/>
+  <dimension ref="A1:IO202"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G196" sqref="G196"/>
+      <selection pane="bottomLeft" activeCell="D206" sqref="D205:D206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -62798,6 +62846,37 @@
       </c>
       <c r="O201" s="99"/>
     </row>
+    <row r="202" spans="1:15" s="333" customFormat="1" ht="20" customHeight="1">
+      <c r="A202" s="59">
+        <v>42736</v>
+      </c>
+      <c r="B202" s="53"/>
+      <c r="C202" s="270" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D202" s="73" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E202" s="73" t="s">
+        <v>450</v>
+      </c>
+      <c r="F202" s="72"/>
+      <c r="G202" s="554" t="s">
+        <v>167</v>
+      </c>
+      <c r="H202" s="54"/>
+      <c r="I202" s="61"/>
+      <c r="J202" s="61"/>
+      <c r="K202" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="L202" s="61"/>
+      <c r="M202" s="61"/>
+      <c r="N202" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="O202" s="99"/>
+    </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B138" xr:uid="{EB4CB59A-D663-4C4C-AAAC-D2AEAD1D4BBC}">

</xml_diff>

<commit_message>
RDM-12836: Update Case Definition Import to Allow Injected Show Conditions and Labels
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA38D6B-BED0-E84A-A5FF-0D866EE4039B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95778D8E-C273-734F-9E4D-1B25FC4094E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="25880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="25740" firstSheet="9" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9914" uniqueCount="1258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9929" uniqueCount="1258">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -20100,10 +20100,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:IQ54"/>
+  <dimension ref="A1:IQ55"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A35" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -22095,6 +22095,26 @@
       </c>
       <c r="H54" s="359"/>
     </row>
+    <row r="55" spans="1:8" s="333" customFormat="1" ht="20" customHeight="1">
+      <c r="A55" s="304">
+        <v>42736</v>
+      </c>
+      <c r="B55" s="304"/>
+      <c r="C55" s="65" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D55" s="305" t="s">
+        <v>848</v>
+      </c>
+      <c r="E55" s="305" t="s">
+        <v>849</v>
+      </c>
+      <c r="F55" s="359"/>
+      <c r="G55" s="391">
+        <v>1</v>
+      </c>
+      <c r="H55" s="359"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G26:G28" xr:uid="{4F2581EF-0318-6146-80A0-4232D55627A6}">
@@ -35648,10 +35668,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -37112,6 +37132,26 @@
         <v>1</v>
       </c>
       <c r="H69" s="69"/>
+    </row>
+    <row r="70" spans="1:8" s="327" customFormat="1" ht="20" customHeight="1">
+      <c r="A70" s="128">
+        <v>42736</v>
+      </c>
+      <c r="B70" s="128"/>
+      <c r="C70" s="69" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D70" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="E70" s="69"/>
+      <c r="F70" s="69" t="s">
+        <v>166</v>
+      </c>
+      <c r="G70" s="408">
+        <v>1</v>
+      </c>
+      <c r="H70" s="69"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -37367,10 +37407,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:DS59"/>
+  <dimension ref="A1:DS60"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -38882,6 +38922,27 @@
       <c r="H59" s="433"/>
       <c r="I59" s="433"/>
     </row>
+    <row r="60" spans="1:9" s="327" customFormat="1" ht="20" customHeight="1">
+      <c r="A60" s="120">
+        <v>42736</v>
+      </c>
+      <c r="B60" s="139"/>
+      <c r="C60" s="121" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D60" s="121" t="s">
+        <v>165</v>
+      </c>
+      <c r="E60" s="140" t="s">
+        <v>166</v>
+      </c>
+      <c r="F60" s="140"/>
+      <c r="G60" s="141">
+        <v>1</v>
+      </c>
+      <c r="H60" s="433"/>
+      <c r="I60" s="433"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G23:G24" xr:uid="{9850B61E-9DFD-1342-A596-EA5F0D31DB06}">
@@ -38901,10 +38962,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.75" customHeight="1"/>
@@ -40302,8 +40363,28 @@
       </c>
       <c r="H67" s="72"/>
     </row>
+    <row r="68" spans="1:8" s="333" customFormat="1" ht="20" customHeight="1">
+      <c r="A68" s="148">
+        <v>42736</v>
+      </c>
+      <c r="B68" s="139"/>
+      <c r="C68" s="140" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D68" s="121" t="s">
+        <v>165</v>
+      </c>
+      <c r="E68" s="121"/>
+      <c r="F68" s="121" t="s">
+        <v>166</v>
+      </c>
+      <c r="G68" s="141">
+        <v>1</v>
+      </c>
+      <c r="H68" s="72"/>
+    </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G36 G39 G42 G44:G45" xr:uid="{1466D592-8C51-1B42-9713-FF7D423B9DE0}">
       <formula1>0</formula1>
     </dataValidation>
@@ -40323,8 +40404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:BL75"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="H106" sqref="H106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -41973,14 +42054,24 @@
       <c r="H71" s="173"/>
       <c r="I71" s="173"/>
     </row>
-    <row r="72" spans="1:9" s="333" customFormat="1" ht="20" customHeight="1">
-      <c r="A72" s="178"/>
+    <row r="72" spans="1:9" ht="20" customHeight="1">
+      <c r="A72" s="178">
+        <v>42736</v>
+      </c>
       <c r="B72" s="179"/>
-      <c r="C72" s="173"/>
-      <c r="D72" s="173"/>
+      <c r="C72" s="173" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D72" s="173" t="s">
+        <v>165</v>
+      </c>
       <c r="E72" s="173"/>
-      <c r="F72" s="173"/>
-      <c r="G72" s="174"/>
+      <c r="F72" s="173" t="s">
+        <v>166</v>
+      </c>
+      <c r="G72" s="174">
+        <v>2</v>
+      </c>
       <c r="H72" s="173"/>
       <c r="I72" s="173"/>
     </row>
@@ -53111,7 +53202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E15BE1-896E-C94F-B2CD-122BE5CAB0E3}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+    <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding permissions for master-caseworker for all TTL events
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A656B101-A087-4130-91B9-E61F9C3818E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA4A05D0-9B1A-4B4D-9994-F1DB78D7740C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="23" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="23" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9995" uniqueCount="1281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10011" uniqueCount="1281">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -4759,7 +4759,7 @@
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="533">
+  <cellXfs count="532">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -6226,9 +6226,6 @@
     <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6238,16 +6235,16 @@
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Explanatory Text" xfId="14" builtinId="53"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
@@ -15192,7 +15189,7 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F81" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F85" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="26"/>
@@ -22018,8 +22015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K7:K8"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.35" customHeight="1"/>
@@ -25968,7 +25965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:T259"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -26838,7 +26835,7 @@
         <v>1077</v>
       </c>
       <c r="J24" s="49"/>
-      <c r="M24" s="530"/>
+      <c r="M24" s="39"/>
       <c r="P24" s="36" t="s">
         <v>250</v>
       </c>
@@ -26871,7 +26868,7 @@
         <v>1077</v>
       </c>
       <c r="J25" s="49"/>
-      <c r="M25" s="530"/>
+      <c r="M25" s="39"/>
       <c r="P25" s="36" t="s">
         <v>250</v>
       </c>
@@ -26904,7 +26901,7 @@
         <v>1077</v>
       </c>
       <c r="J26" s="49"/>
-      <c r="M26" s="530"/>
+      <c r="M26" s="39"/>
       <c r="P26" s="36" t="s">
         <v>250</v>
       </c>
@@ -26937,7 +26934,7 @@
         <v>1077</v>
       </c>
       <c r="J27" s="49"/>
-      <c r="M27" s="530"/>
+      <c r="M27" s="39"/>
       <c r="P27" s="36" t="s">
         <v>250</v>
       </c>
@@ -26970,7 +26967,7 @@
         <v>1077</v>
       </c>
       <c r="J28" s="49"/>
-      <c r="M28" s="530"/>
+      <c r="M28" s="39"/>
       <c r="P28" s="36" t="s">
         <v>250</v>
       </c>
@@ -27003,7 +27000,7 @@
         <v>1077</v>
       </c>
       <c r="J29" s="49"/>
-      <c r="M29" s="530"/>
+      <c r="M29" s="39"/>
       <c r="P29" s="36" t="s">
         <v>250</v>
       </c>
@@ -48590,10 +48587,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:EK97"/>
+  <dimension ref="A1:EK101"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.35" customHeight="1"/>
@@ -48808,14 +48805,14 @@
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="34">
-        <v>42736</v>
+        <v>42737</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>665</v>
+        <v>41</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>933</v>
       </c>
       <c r="E12" s="86" t="s">
         <v>586</v>
@@ -48826,14 +48823,14 @@
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="34">
-        <v>42736</v>
+        <v>42738</v>
       </c>
       <c r="B13" s="50"/>
       <c r="C13" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>949</v>
+        <v>41</v>
+      </c>
+      <c r="D13" s="489" t="s">
+        <v>936</v>
       </c>
       <c r="E13" s="86" t="s">
         <v>586</v>
@@ -48844,14 +48841,14 @@
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="34">
-        <v>42736</v>
+        <v>42739</v>
       </c>
       <c r="B14" s="50"/>
-      <c r="C14" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>665</v>
+      <c r="C14" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="489" t="s">
+        <v>940</v>
       </c>
       <c r="E14" s="86" t="s">
         <v>586</v>
@@ -48862,14 +48859,14 @@
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="34">
-        <v>42736</v>
+        <v>42740</v>
       </c>
       <c r="B15" s="50"/>
-      <c r="C15" s="76" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="76" t="s">
-        <v>667</v>
+      <c r="C15" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="489" t="s">
+        <v>944</v>
       </c>
       <c r="E15" s="86" t="s">
         <v>586</v>
@@ -48883,11 +48880,11 @@
         <v>42736</v>
       </c>
       <c r="B16" s="50"/>
-      <c r="C16" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="77" t="s">
-        <v>629</v>
+      <c r="C16" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>665</v>
       </c>
       <c r="E16" s="86" t="s">
         <v>586</v>
@@ -48901,11 +48898,11 @@
         <v>42736</v>
       </c>
       <c r="B17" s="50"/>
-      <c r="C17" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="77" t="s">
-        <v>956</v>
+      <c r="C17" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>949</v>
       </c>
       <c r="E17" s="86" t="s">
         <v>586</v>
@@ -48919,11 +48916,11 @@
         <v>42736</v>
       </c>
       <c r="B18" s="50"/>
-      <c r="C18" s="77" t="s">
+      <c r="C18" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="77" t="s">
-        <v>958</v>
+      <c r="D18" s="36" t="s">
+        <v>665</v>
       </c>
       <c r="E18" s="86" t="s">
         <v>586</v>
@@ -48937,11 +48934,11 @@
         <v>42736</v>
       </c>
       <c r="B19" s="50"/>
-      <c r="C19" s="77" t="s">
+      <c r="C19" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="77" t="s">
-        <v>960</v>
+      <c r="D19" s="76" t="s">
+        <v>667</v>
       </c>
       <c r="E19" s="86" t="s">
         <v>586</v>
@@ -48950,383 +48947,383 @@
         <v>585</v>
       </c>
     </row>
-    <row r="20" spans="1:141" s="192" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="190">
-        <v>42736</v>
-      </c>
-      <c r="B20" s="191"/>
-      <c r="C20" s="193" t="s">
+    <row r="20" spans="1:141" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="50"/>
+      <c r="C20" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="77" t="s">
+        <v>629</v>
+      </c>
+      <c r="E20" s="86" t="s">
+        <v>586</v>
+      </c>
+      <c r="F20" s="74" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="21" spans="1:141" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="77" t="s">
+        <v>956</v>
+      </c>
+      <c r="E21" s="86" t="s">
+        <v>586</v>
+      </c>
+      <c r="F21" s="74" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="22" spans="1:141" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B22" s="50"/>
+      <c r="C22" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="77" t="s">
+        <v>958</v>
+      </c>
+      <c r="E22" s="86" t="s">
+        <v>586</v>
+      </c>
+      <c r="F22" s="74" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="23" spans="1:141" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B23" s="50"/>
+      <c r="C23" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="77" t="s">
+        <v>960</v>
+      </c>
+      <c r="E23" s="86" t="s">
+        <v>586</v>
+      </c>
+      <c r="F23" s="74" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="24" spans="1:141" s="192" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="190">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="191"/>
+      <c r="C24" s="193" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="193" t="s">
+      <c r="D24" s="193" t="s">
         <v>662</v>
       </c>
-      <c r="E20" s="217" t="s">
+      <c r="E24" s="217" t="s">
         <v>586</v>
       </c>
-      <c r="F20" s="194" t="s">
+      <c r="F24" s="194" t="s">
         <v>585</v>
       </c>
-      <c r="G20" s="238"/>
-      <c r="H20" s="238"/>
-      <c r="I20" s="238"/>
-      <c r="J20" s="238"/>
-      <c r="K20" s="238"/>
-      <c r="L20" s="238"/>
-      <c r="M20" s="238"/>
-      <c r="N20" s="238"/>
-      <c r="O20" s="238"/>
-      <c r="P20" s="238"/>
-      <c r="Q20" s="238"/>
-      <c r="R20" s="238"/>
-      <c r="S20" s="238"/>
-      <c r="T20" s="238"/>
-      <c r="U20" s="238"/>
-      <c r="V20" s="238"/>
-      <c r="W20" s="238"/>
-      <c r="X20" s="238"/>
-      <c r="Y20" s="238"/>
-      <c r="Z20" s="238"/>
-      <c r="AA20" s="238"/>
-      <c r="AB20" s="238"/>
-      <c r="AC20" s="238"/>
-      <c r="AD20" s="238"/>
-      <c r="AE20" s="238"/>
-      <c r="AF20" s="238"/>
-      <c r="AG20" s="238"/>
-      <c r="AH20" s="238"/>
-      <c r="AI20" s="238"/>
-      <c r="AJ20" s="238"/>
-      <c r="AK20" s="238"/>
-      <c r="AL20" s="238"/>
-      <c r="AM20" s="238"/>
-      <c r="AN20" s="238"/>
-      <c r="AO20" s="238"/>
-      <c r="AP20" s="238"/>
-      <c r="AQ20" s="238"/>
-      <c r="AR20" s="238"/>
-      <c r="AS20" s="238"/>
-      <c r="AT20" s="238"/>
-      <c r="AU20" s="238"/>
-      <c r="AV20" s="238"/>
-      <c r="AW20" s="238"/>
-      <c r="AX20" s="238"/>
-      <c r="AY20" s="238"/>
-      <c r="AZ20" s="238"/>
-      <c r="BA20" s="238"/>
-      <c r="BB20" s="238"/>
-      <c r="BC20" s="238"/>
-      <c r="BD20" s="238"/>
-      <c r="BE20" s="238"/>
-      <c r="BF20" s="238"/>
-      <c r="BG20" s="238"/>
-      <c r="BH20" s="238"/>
-      <c r="BI20" s="238"/>
-      <c r="BJ20" s="238"/>
-      <c r="BK20" s="238"/>
-      <c r="BL20" s="238"/>
-      <c r="BM20" s="238"/>
-      <c r="BN20" s="238"/>
-      <c r="BO20" s="238"/>
-      <c r="BP20" s="238"/>
-      <c r="BQ20" s="238"/>
-      <c r="BR20" s="238"/>
-      <c r="BS20" s="238"/>
-      <c r="BT20" s="238"/>
-      <c r="BU20" s="238"/>
-      <c r="BV20" s="238"/>
-      <c r="BW20" s="238"/>
-      <c r="BX20" s="238"/>
-      <c r="BY20" s="238"/>
-      <c r="BZ20" s="238"/>
-      <c r="CA20" s="238"/>
-      <c r="CB20" s="238"/>
-      <c r="CC20" s="238"/>
-      <c r="CD20" s="238"/>
-      <c r="CE20" s="238"/>
-      <c r="CF20" s="238"/>
-      <c r="CG20" s="238"/>
-      <c r="CH20" s="238"/>
-      <c r="CI20" s="238"/>
-      <c r="CJ20" s="238"/>
-      <c r="CK20" s="238"/>
-      <c r="CL20" s="238"/>
-      <c r="CM20" s="238"/>
-      <c r="CN20" s="238"/>
-      <c r="CO20" s="238"/>
-      <c r="CP20" s="238"/>
-      <c r="CQ20" s="238"/>
-      <c r="CR20" s="238"/>
-      <c r="CS20" s="238"/>
-      <c r="CT20" s="238"/>
-      <c r="CU20" s="238"/>
-      <c r="CV20" s="238"/>
-      <c r="CW20" s="238"/>
-      <c r="CX20" s="238"/>
-      <c r="CY20" s="238"/>
-      <c r="CZ20" s="238"/>
-      <c r="DA20" s="238"/>
-      <c r="DB20" s="238"/>
-      <c r="DC20" s="238"/>
-      <c r="DD20" s="238"/>
-      <c r="DE20" s="238"/>
-      <c r="DF20" s="238"/>
-      <c r="DG20" s="238"/>
-      <c r="DH20" s="238"/>
-      <c r="DI20" s="238"/>
-      <c r="DJ20" s="238"/>
-      <c r="DK20" s="238"/>
-      <c r="DL20" s="238"/>
-      <c r="DM20" s="238"/>
-      <c r="DN20" s="238"/>
-      <c r="DO20" s="238"/>
-      <c r="DP20" s="238"/>
-      <c r="DQ20" s="238"/>
-      <c r="DR20" s="238"/>
-      <c r="DS20" s="238"/>
-      <c r="DT20" s="238"/>
-      <c r="DU20" s="238"/>
-      <c r="DV20" s="238"/>
-      <c r="DW20" s="238"/>
-      <c r="DX20" s="238"/>
-      <c r="DY20" s="238"/>
-      <c r="DZ20" s="238"/>
-      <c r="EA20" s="238"/>
-      <c r="EB20" s="238"/>
-      <c r="EC20" s="238"/>
-      <c r="ED20" s="238"/>
-      <c r="EE20" s="238"/>
-      <c r="EF20" s="238"/>
-      <c r="EG20" s="238"/>
-      <c r="EH20" s="238"/>
-      <c r="EI20" s="238"/>
-      <c r="EJ20" s="238"/>
-      <c r="EK20" s="238"/>
-    </row>
-    <row r="21" spans="1:141" s="192" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="190">
-        <v>42736</v>
-      </c>
-      <c r="B21" s="191"/>
-      <c r="C21" s="193" t="s">
+      <c r="G24" s="238"/>
+      <c r="H24" s="238"/>
+      <c r="I24" s="238"/>
+      <c r="J24" s="238"/>
+      <c r="K24" s="238"/>
+      <c r="L24" s="238"/>
+      <c r="M24" s="238"/>
+      <c r="N24" s="238"/>
+      <c r="O24" s="238"/>
+      <c r="P24" s="238"/>
+      <c r="Q24" s="238"/>
+      <c r="R24" s="238"/>
+      <c r="S24" s="238"/>
+      <c r="T24" s="238"/>
+      <c r="U24" s="238"/>
+      <c r="V24" s="238"/>
+      <c r="W24" s="238"/>
+      <c r="X24" s="238"/>
+      <c r="Y24" s="238"/>
+      <c r="Z24" s="238"/>
+      <c r="AA24" s="238"/>
+      <c r="AB24" s="238"/>
+      <c r="AC24" s="238"/>
+      <c r="AD24" s="238"/>
+      <c r="AE24" s="238"/>
+      <c r="AF24" s="238"/>
+      <c r="AG24" s="238"/>
+      <c r="AH24" s="238"/>
+      <c r="AI24" s="238"/>
+      <c r="AJ24" s="238"/>
+      <c r="AK24" s="238"/>
+      <c r="AL24" s="238"/>
+      <c r="AM24" s="238"/>
+      <c r="AN24" s="238"/>
+      <c r="AO24" s="238"/>
+      <c r="AP24" s="238"/>
+      <c r="AQ24" s="238"/>
+      <c r="AR24" s="238"/>
+      <c r="AS24" s="238"/>
+      <c r="AT24" s="238"/>
+      <c r="AU24" s="238"/>
+      <c r="AV24" s="238"/>
+      <c r="AW24" s="238"/>
+      <c r="AX24" s="238"/>
+      <c r="AY24" s="238"/>
+      <c r="AZ24" s="238"/>
+      <c r="BA24" s="238"/>
+      <c r="BB24" s="238"/>
+      <c r="BC24" s="238"/>
+      <c r="BD24" s="238"/>
+      <c r="BE24" s="238"/>
+      <c r="BF24" s="238"/>
+      <c r="BG24" s="238"/>
+      <c r="BH24" s="238"/>
+      <c r="BI24" s="238"/>
+      <c r="BJ24" s="238"/>
+      <c r="BK24" s="238"/>
+      <c r="BL24" s="238"/>
+      <c r="BM24" s="238"/>
+      <c r="BN24" s="238"/>
+      <c r="BO24" s="238"/>
+      <c r="BP24" s="238"/>
+      <c r="BQ24" s="238"/>
+      <c r="BR24" s="238"/>
+      <c r="BS24" s="238"/>
+      <c r="BT24" s="238"/>
+      <c r="BU24" s="238"/>
+      <c r="BV24" s="238"/>
+      <c r="BW24" s="238"/>
+      <c r="BX24" s="238"/>
+      <c r="BY24" s="238"/>
+      <c r="BZ24" s="238"/>
+      <c r="CA24" s="238"/>
+      <c r="CB24" s="238"/>
+      <c r="CC24" s="238"/>
+      <c r="CD24" s="238"/>
+      <c r="CE24" s="238"/>
+      <c r="CF24" s="238"/>
+      <c r="CG24" s="238"/>
+      <c r="CH24" s="238"/>
+      <c r="CI24" s="238"/>
+      <c r="CJ24" s="238"/>
+      <c r="CK24" s="238"/>
+      <c r="CL24" s="238"/>
+      <c r="CM24" s="238"/>
+      <c r="CN24" s="238"/>
+      <c r="CO24" s="238"/>
+      <c r="CP24" s="238"/>
+      <c r="CQ24" s="238"/>
+      <c r="CR24" s="238"/>
+      <c r="CS24" s="238"/>
+      <c r="CT24" s="238"/>
+      <c r="CU24" s="238"/>
+      <c r="CV24" s="238"/>
+      <c r="CW24" s="238"/>
+      <c r="CX24" s="238"/>
+      <c r="CY24" s="238"/>
+      <c r="CZ24" s="238"/>
+      <c r="DA24" s="238"/>
+      <c r="DB24" s="238"/>
+      <c r="DC24" s="238"/>
+      <c r="DD24" s="238"/>
+      <c r="DE24" s="238"/>
+      <c r="DF24" s="238"/>
+      <c r="DG24" s="238"/>
+      <c r="DH24" s="238"/>
+      <c r="DI24" s="238"/>
+      <c r="DJ24" s="238"/>
+      <c r="DK24" s="238"/>
+      <c r="DL24" s="238"/>
+      <c r="DM24" s="238"/>
+      <c r="DN24" s="238"/>
+      <c r="DO24" s="238"/>
+      <c r="DP24" s="238"/>
+      <c r="DQ24" s="238"/>
+      <c r="DR24" s="238"/>
+      <c r="DS24" s="238"/>
+      <c r="DT24" s="238"/>
+      <c r="DU24" s="238"/>
+      <c r="DV24" s="238"/>
+      <c r="DW24" s="238"/>
+      <c r="DX24" s="238"/>
+      <c r="DY24" s="238"/>
+      <c r="DZ24" s="238"/>
+      <c r="EA24" s="238"/>
+      <c r="EB24" s="238"/>
+      <c r="EC24" s="238"/>
+      <c r="ED24" s="238"/>
+      <c r="EE24" s="238"/>
+      <c r="EF24" s="238"/>
+      <c r="EG24" s="238"/>
+      <c r="EH24" s="238"/>
+      <c r="EI24" s="238"/>
+      <c r="EJ24" s="238"/>
+      <c r="EK24" s="238"/>
+    </row>
+    <row r="25" spans="1:141" s="192" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="190">
+        <v>42736</v>
+      </c>
+      <c r="B25" s="191"/>
+      <c r="C25" s="193" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="193" t="s">
+      <c r="D25" s="193" t="s">
         <v>645</v>
       </c>
-      <c r="E21" s="217" t="s">
+      <c r="E25" s="217" t="s">
         <v>586</v>
       </c>
-      <c r="F21" s="194" t="s">
+      <c r="F25" s="194" t="s">
         <v>585</v>
       </c>
-      <c r="G21" s="238"/>
-      <c r="H21" s="238"/>
-      <c r="I21" s="238"/>
-      <c r="J21" s="238"/>
-      <c r="K21" s="238"/>
-      <c r="L21" s="238"/>
-      <c r="M21" s="238"/>
-      <c r="N21" s="238"/>
-      <c r="O21" s="238"/>
-      <c r="P21" s="238"/>
-      <c r="Q21" s="238"/>
-      <c r="R21" s="238"/>
-      <c r="S21" s="238"/>
-      <c r="T21" s="238"/>
-      <c r="U21" s="238"/>
-      <c r="V21" s="238"/>
-      <c r="W21" s="238"/>
-      <c r="X21" s="238"/>
-      <c r="Y21" s="238"/>
-      <c r="Z21" s="238"/>
-      <c r="AA21" s="238"/>
-      <c r="AB21" s="238"/>
-      <c r="AC21" s="238"/>
-      <c r="AD21" s="238"/>
-      <c r="AE21" s="238"/>
-      <c r="AF21" s="238"/>
-      <c r="AG21" s="238"/>
-      <c r="AH21" s="238"/>
-      <c r="AI21" s="238"/>
-      <c r="AJ21" s="238"/>
-      <c r="AK21" s="238"/>
-      <c r="AL21" s="238"/>
-      <c r="AM21" s="238"/>
-      <c r="AN21" s="238"/>
-      <c r="AO21" s="238"/>
-      <c r="AP21" s="238"/>
-      <c r="AQ21" s="238"/>
-      <c r="AR21" s="238"/>
-      <c r="AS21" s="238"/>
-      <c r="AT21" s="238"/>
-      <c r="AU21" s="238"/>
-      <c r="AV21" s="238"/>
-      <c r="AW21" s="238"/>
-      <c r="AX21" s="238"/>
-      <c r="AY21" s="238"/>
-      <c r="AZ21" s="238"/>
-      <c r="BA21" s="238"/>
-      <c r="BB21" s="238"/>
-      <c r="BC21" s="238"/>
-      <c r="BD21" s="238"/>
-      <c r="BE21" s="238"/>
-      <c r="BF21" s="238"/>
-      <c r="BG21" s="238"/>
-      <c r="BH21" s="238"/>
-      <c r="BI21" s="238"/>
-      <c r="BJ21" s="238"/>
-      <c r="BK21" s="238"/>
-      <c r="BL21" s="238"/>
-      <c r="BM21" s="238"/>
-      <c r="BN21" s="238"/>
-      <c r="BO21" s="238"/>
-      <c r="BP21" s="238"/>
-      <c r="BQ21" s="238"/>
-      <c r="BR21" s="238"/>
-      <c r="BS21" s="238"/>
-      <c r="BT21" s="238"/>
-      <c r="BU21" s="238"/>
-      <c r="BV21" s="238"/>
-      <c r="BW21" s="238"/>
-      <c r="BX21" s="238"/>
-      <c r="BY21" s="238"/>
-      <c r="BZ21" s="238"/>
-      <c r="CA21" s="238"/>
-      <c r="CB21" s="238"/>
-      <c r="CC21" s="238"/>
-      <c r="CD21" s="238"/>
-      <c r="CE21" s="238"/>
-      <c r="CF21" s="238"/>
-      <c r="CG21" s="238"/>
-      <c r="CH21" s="238"/>
-      <c r="CI21" s="238"/>
-      <c r="CJ21" s="238"/>
-      <c r="CK21" s="238"/>
-      <c r="CL21" s="238"/>
-      <c r="CM21" s="238"/>
-      <c r="CN21" s="238"/>
-      <c r="CO21" s="238"/>
-      <c r="CP21" s="238"/>
-      <c r="CQ21" s="238"/>
-      <c r="CR21" s="238"/>
-      <c r="CS21" s="238"/>
-      <c r="CT21" s="238"/>
-      <c r="CU21" s="238"/>
-      <c r="CV21" s="238"/>
-      <c r="CW21" s="238"/>
-      <c r="CX21" s="238"/>
-      <c r="CY21" s="238"/>
-      <c r="CZ21" s="238"/>
-      <c r="DA21" s="238"/>
-      <c r="DB21" s="238"/>
-      <c r="DC21" s="238"/>
-      <c r="DD21" s="238"/>
-      <c r="DE21" s="238"/>
-      <c r="DF21" s="238"/>
-      <c r="DG21" s="238"/>
-      <c r="DH21" s="238"/>
-      <c r="DI21" s="238"/>
-      <c r="DJ21" s="238"/>
-      <c r="DK21" s="238"/>
-      <c r="DL21" s="238"/>
-      <c r="DM21" s="238"/>
-      <c r="DN21" s="238"/>
-      <c r="DO21" s="238"/>
-      <c r="DP21" s="238"/>
-      <c r="DQ21" s="238"/>
-      <c r="DR21" s="238"/>
-      <c r="DS21" s="238"/>
-      <c r="DT21" s="238"/>
-      <c r="DU21" s="238"/>
-      <c r="DV21" s="238"/>
-      <c r="DW21" s="238"/>
-      <c r="DX21" s="238"/>
-      <c r="DY21" s="238"/>
-      <c r="DZ21" s="238"/>
-      <c r="EA21" s="238"/>
-      <c r="EB21" s="238"/>
-      <c r="EC21" s="238"/>
-      <c r="ED21" s="238"/>
-      <c r="EE21" s="238"/>
-      <c r="EF21" s="238"/>
-      <c r="EG21" s="238"/>
-      <c r="EH21" s="238"/>
-      <c r="EI21" s="238"/>
-      <c r="EJ21" s="238"/>
-      <c r="EK21" s="238"/>
-    </row>
-    <row r="22" spans="1:141" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="266">
-        <v>42736</v>
-      </c>
-      <c r="B22" s="233"/>
-      <c r="C22" s="248" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="234" t="s">
-        <v>1018</v>
-      </c>
-      <c r="E22" s="268" t="s">
-        <v>586</v>
-      </c>
-      <c r="F22" s="252" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="23" spans="1:141" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="266">
-        <v>42736</v>
-      </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="248" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="234" t="s">
-        <v>673</v>
-      </c>
-      <c r="E23" s="268" t="s">
-        <v>586</v>
-      </c>
-      <c r="F23" s="252" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="24" spans="1:141" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="266">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="233"/>
-      <c r="C24" s="248" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="234" t="s">
-        <v>674</v>
-      </c>
-      <c r="E24" s="268" t="s">
-        <v>586</v>
-      </c>
-      <c r="F24" s="252" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="25" spans="1:141" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="266">
-        <v>42736</v>
-      </c>
-      <c r="B25" s="233"/>
-      <c r="C25" s="248" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="234" t="s">
-        <v>675</v>
-      </c>
-      <c r="E25" s="268" t="s">
-        <v>586</v>
-      </c>
-      <c r="F25" s="252" t="s">
-        <v>585</v>
-      </c>
+      <c r="G25" s="238"/>
+      <c r="H25" s="238"/>
+      <c r="I25" s="238"/>
+      <c r="J25" s="238"/>
+      <c r="K25" s="238"/>
+      <c r="L25" s="238"/>
+      <c r="M25" s="238"/>
+      <c r="N25" s="238"/>
+      <c r="O25" s="238"/>
+      <c r="P25" s="238"/>
+      <c r="Q25" s="238"/>
+      <c r="R25" s="238"/>
+      <c r="S25" s="238"/>
+      <c r="T25" s="238"/>
+      <c r="U25" s="238"/>
+      <c r="V25" s="238"/>
+      <c r="W25" s="238"/>
+      <c r="X25" s="238"/>
+      <c r="Y25" s="238"/>
+      <c r="Z25" s="238"/>
+      <c r="AA25" s="238"/>
+      <c r="AB25" s="238"/>
+      <c r="AC25" s="238"/>
+      <c r="AD25" s="238"/>
+      <c r="AE25" s="238"/>
+      <c r="AF25" s="238"/>
+      <c r="AG25" s="238"/>
+      <c r="AH25" s="238"/>
+      <c r="AI25" s="238"/>
+      <c r="AJ25" s="238"/>
+      <c r="AK25" s="238"/>
+      <c r="AL25" s="238"/>
+      <c r="AM25" s="238"/>
+      <c r="AN25" s="238"/>
+      <c r="AO25" s="238"/>
+      <c r="AP25" s="238"/>
+      <c r="AQ25" s="238"/>
+      <c r="AR25" s="238"/>
+      <c r="AS25" s="238"/>
+      <c r="AT25" s="238"/>
+      <c r="AU25" s="238"/>
+      <c r="AV25" s="238"/>
+      <c r="AW25" s="238"/>
+      <c r="AX25" s="238"/>
+      <c r="AY25" s="238"/>
+      <c r="AZ25" s="238"/>
+      <c r="BA25" s="238"/>
+      <c r="BB25" s="238"/>
+      <c r="BC25" s="238"/>
+      <c r="BD25" s="238"/>
+      <c r="BE25" s="238"/>
+      <c r="BF25" s="238"/>
+      <c r="BG25" s="238"/>
+      <c r="BH25" s="238"/>
+      <c r="BI25" s="238"/>
+      <c r="BJ25" s="238"/>
+      <c r="BK25" s="238"/>
+      <c r="BL25" s="238"/>
+      <c r="BM25" s="238"/>
+      <c r="BN25" s="238"/>
+      <c r="BO25" s="238"/>
+      <c r="BP25" s="238"/>
+      <c r="BQ25" s="238"/>
+      <c r="BR25" s="238"/>
+      <c r="BS25" s="238"/>
+      <c r="BT25" s="238"/>
+      <c r="BU25" s="238"/>
+      <c r="BV25" s="238"/>
+      <c r="BW25" s="238"/>
+      <c r="BX25" s="238"/>
+      <c r="BY25" s="238"/>
+      <c r="BZ25" s="238"/>
+      <c r="CA25" s="238"/>
+      <c r="CB25" s="238"/>
+      <c r="CC25" s="238"/>
+      <c r="CD25" s="238"/>
+      <c r="CE25" s="238"/>
+      <c r="CF25" s="238"/>
+      <c r="CG25" s="238"/>
+      <c r="CH25" s="238"/>
+      <c r="CI25" s="238"/>
+      <c r="CJ25" s="238"/>
+      <c r="CK25" s="238"/>
+      <c r="CL25" s="238"/>
+      <c r="CM25" s="238"/>
+      <c r="CN25" s="238"/>
+      <c r="CO25" s="238"/>
+      <c r="CP25" s="238"/>
+      <c r="CQ25" s="238"/>
+      <c r="CR25" s="238"/>
+      <c r="CS25" s="238"/>
+      <c r="CT25" s="238"/>
+      <c r="CU25" s="238"/>
+      <c r="CV25" s="238"/>
+      <c r="CW25" s="238"/>
+      <c r="CX25" s="238"/>
+      <c r="CY25" s="238"/>
+      <c r="CZ25" s="238"/>
+      <c r="DA25" s="238"/>
+      <c r="DB25" s="238"/>
+      <c r="DC25" s="238"/>
+      <c r="DD25" s="238"/>
+      <c r="DE25" s="238"/>
+      <c r="DF25" s="238"/>
+      <c r="DG25" s="238"/>
+      <c r="DH25" s="238"/>
+      <c r="DI25" s="238"/>
+      <c r="DJ25" s="238"/>
+      <c r="DK25" s="238"/>
+      <c r="DL25" s="238"/>
+      <c r="DM25" s="238"/>
+      <c r="DN25" s="238"/>
+      <c r="DO25" s="238"/>
+      <c r="DP25" s="238"/>
+      <c r="DQ25" s="238"/>
+      <c r="DR25" s="238"/>
+      <c r="DS25" s="238"/>
+      <c r="DT25" s="238"/>
+      <c r="DU25" s="238"/>
+      <c r="DV25" s="238"/>
+      <c r="DW25" s="238"/>
+      <c r="DX25" s="238"/>
+      <c r="DY25" s="238"/>
+      <c r="DZ25" s="238"/>
+      <c r="EA25" s="238"/>
+      <c r="EB25" s="238"/>
+      <c r="EC25" s="238"/>
+      <c r="ED25" s="238"/>
+      <c r="EE25" s="238"/>
+      <c r="EF25" s="238"/>
+      <c r="EG25" s="238"/>
+      <c r="EH25" s="238"/>
+      <c r="EI25" s="238"/>
+      <c r="EJ25" s="238"/>
+      <c r="EK25" s="238"/>
     </row>
     <row r="26" spans="1:141" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="266">
@@ -49337,7 +49334,7 @@
         <v>85</v>
       </c>
       <c r="D26" s="234" t="s">
-        <v>1023</v>
+        <v>1018</v>
       </c>
       <c r="E26" s="268" t="s">
         <v>586</v>
@@ -49355,7 +49352,7 @@
         <v>85</v>
       </c>
       <c r="D27" s="234" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="E27" s="268" t="s">
         <v>586</v>
@@ -49373,7 +49370,7 @@
         <v>85</v>
       </c>
       <c r="D28" s="234" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="E28" s="268" t="s">
         <v>586</v>
@@ -49383,74 +49380,74 @@
       </c>
     </row>
     <row r="29" spans="1:141" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>665</v>
-      </c>
-      <c r="E29" s="86" t="s">
+      <c r="A29" s="266">
+        <v>42736</v>
+      </c>
+      <c r="B29" s="233"/>
+      <c r="C29" s="248" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="234" t="s">
+        <v>675</v>
+      </c>
+      <c r="E29" s="268" t="s">
         <v>586</v>
       </c>
-      <c r="F29" s="74" t="s">
+      <c r="F29" s="252" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="30" spans="1:141" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="36" t="s">
-        <v>665</v>
-      </c>
-      <c r="E30" s="86" t="s">
+      <c r="A30" s="266">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="233"/>
+      <c r="C30" s="248" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="234" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E30" s="268" t="s">
         <v>586</v>
       </c>
-      <c r="F30" s="74" t="s">
+      <c r="F30" s="252" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="31" spans="1:141" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="36" t="s">
-        <v>963</v>
-      </c>
-      <c r="E31" s="86" t="s">
+      <c r="A31" s="266">
+        <v>42736</v>
+      </c>
+      <c r="B31" s="233"/>
+      <c r="C31" s="248" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="234" t="s">
+        <v>677</v>
+      </c>
+      <c r="E31" s="268" t="s">
         <v>586</v>
       </c>
-      <c r="F31" s="74" t="s">
+      <c r="F31" s="252" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="32" spans="1:141" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="36" t="s">
-        <v>965</v>
-      </c>
-      <c r="E32" s="86" t="s">
+      <c r="A32" s="266">
+        <v>42736</v>
+      </c>
+      <c r="B32" s="233"/>
+      <c r="C32" s="248" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="234" t="s">
+        <v>682</v>
+      </c>
+      <c r="E32" s="268" t="s">
         <v>586</v>
       </c>
-      <c r="F32" s="74" t="s">
+      <c r="F32" s="252" t="s">
         <v>585</v>
       </c>
     </row>
@@ -49460,10 +49457,10 @@
       </c>
       <c r="B33" s="50"/>
       <c r="C33" s="38" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>967</v>
+        <v>665</v>
       </c>
       <c r="E33" s="86" t="s">
         <v>586</v>
@@ -49481,7 +49478,7 @@
         <v>55</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>969</v>
+        <v>665</v>
       </c>
       <c r="E34" s="86" t="s">
         <v>586</v>
@@ -49495,11 +49492,11 @@
         <v>42736</v>
       </c>
       <c r="B35" s="50"/>
-      <c r="C35" s="36" t="s">
-        <v>58</v>
+      <c r="C35" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>665</v>
+        <v>963</v>
       </c>
       <c r="E35" s="86" t="s">
         <v>586</v>
@@ -49513,11 +49510,11 @@
         <v>42736</v>
       </c>
       <c r="B36" s="50"/>
-      <c r="C36" s="36" t="s">
-        <v>61</v>
+      <c r="C36" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>665</v>
+        <v>965</v>
       </c>
       <c r="E36" s="86" t="s">
         <v>586</v>
@@ -49531,11 +49528,11 @@
         <v>42736</v>
       </c>
       <c r="B37" s="50"/>
-      <c r="C37" s="36" t="s">
-        <v>61</v>
+      <c r="C37" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>972</v>
+        <v>967</v>
       </c>
       <c r="E37" s="86" t="s">
         <v>586</v>
@@ -49549,11 +49546,11 @@
         <v>42736</v>
       </c>
       <c r="B38" s="50"/>
-      <c r="C38" s="36" t="s">
-        <v>61</v>
+      <c r="C38" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>976</v>
+        <v>969</v>
       </c>
       <c r="E38" s="86" t="s">
         <v>586</v>
@@ -49568,10 +49565,10 @@
       </c>
       <c r="B39" s="50"/>
       <c r="C39" s="36" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>974</v>
+        <v>665</v>
       </c>
       <c r="E39" s="86" t="s">
         <v>586</v>
@@ -49589,7 +49586,7 @@
         <v>61</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>978</v>
+        <v>665</v>
       </c>
       <c r="E40" s="86" t="s">
         <v>586</v>
@@ -49604,16 +49601,16 @@
       </c>
       <c r="B41" s="50"/>
       <c r="C41" s="36" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>665</v>
+        <v>972</v>
       </c>
       <c r="E41" s="86" t="s">
         <v>586</v>
       </c>
       <c r="F41" s="74" t="s">
-        <v>603</v>
+        <v>585</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -49621,11 +49618,11 @@
         <v>42736</v>
       </c>
       <c r="B42" s="50"/>
-      <c r="C42" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="38" t="s">
-        <v>665</v>
+      <c r="C42" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>976</v>
       </c>
       <c r="E42" s="86" t="s">
         <v>586</v>
@@ -49639,11 +49636,11 @@
         <v>42736</v>
       </c>
       <c r="B43" s="50"/>
-      <c r="C43" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="76" t="s">
-        <v>980</v>
+      <c r="C43" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>974</v>
       </c>
       <c r="E43" s="86" t="s">
         <v>586</v>
@@ -49657,11 +49654,11 @@
         <v>42736</v>
       </c>
       <c r="B44" s="50"/>
-      <c r="C44" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="76" t="s">
-        <v>984</v>
+      <c r="C44" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>978</v>
       </c>
       <c r="E44" s="86" t="s">
         <v>586</v>
@@ -49675,8 +49672,8 @@
         <v>42736</v>
       </c>
       <c r="B45" s="50"/>
-      <c r="C45" s="38" t="s">
-        <v>70</v>
+      <c r="C45" s="36" t="s">
+        <v>67</v>
       </c>
       <c r="D45" s="36" t="s">
         <v>665</v>
@@ -49685,7 +49682,7 @@
         <v>586</v>
       </c>
       <c r="F45" s="74" t="s">
-        <v>585</v>
+        <v>603</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -49693,14 +49690,14 @@
         <v>42736</v>
       </c>
       <c r="B46" s="50"/>
-      <c r="C46" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="D46" s="51" t="s">
+      <c r="C46" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="38" t="s">
         <v>665</v>
       </c>
-      <c r="E46" s="50" t="s">
-        <v>602</v>
+      <c r="E46" s="86" t="s">
+        <v>586</v>
       </c>
       <c r="F46" s="74" t="s">
         <v>585</v>
@@ -49711,17 +49708,17 @@
         <v>42736</v>
       </c>
       <c r="B47" s="50"/>
-      <c r="C47" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="51" t="s">
-        <v>671</v>
-      </c>
-      <c r="E47" s="50" t="s">
-        <v>602</v>
+      <c r="C47" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" s="76" t="s">
+        <v>980</v>
+      </c>
+      <c r="E47" s="86" t="s">
+        <v>586</v>
       </c>
       <c r="F47" s="74" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -49729,14 +49726,14 @@
         <v>42736</v>
       </c>
       <c r="B48" s="50"/>
-      <c r="C48" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="D48" s="51" t="s">
-        <v>665</v>
-      </c>
-      <c r="E48" s="50" t="s">
-        <v>600</v>
+      <c r="C48" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="76" t="s">
+        <v>984</v>
+      </c>
+      <c r="E48" s="86" t="s">
+        <v>586</v>
       </c>
       <c r="F48" s="74" t="s">
         <v>585</v>
@@ -49747,17 +49744,17 @@
         <v>42736</v>
       </c>
       <c r="B49" s="50"/>
-      <c r="C49" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="51" t="s">
-        <v>671</v>
-      </c>
-      <c r="E49" s="50" t="s">
-        <v>600</v>
+      <c r="C49" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="36" t="s">
+        <v>665</v>
+      </c>
+      <c r="E49" s="86" t="s">
+        <v>586</v>
       </c>
       <c r="F49" s="74" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -49768,14 +49765,14 @@
       <c r="C50" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="D50" s="36" t="s">
-        <v>672</v>
+      <c r="D50" s="51" t="s">
+        <v>665</v>
       </c>
       <c r="E50" s="50" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="F50" s="74" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -49786,14 +49783,14 @@
       <c r="C51" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="36" t="s">
-        <v>672</v>
+      <c r="D51" s="51" t="s">
+        <v>671</v>
       </c>
       <c r="E51" s="50" t="s">
         <v>602</v>
       </c>
       <c r="F51" s="74" t="s">
-        <v>587</v>
+        <v>599</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -49802,13 +49799,13 @@
       </c>
       <c r="B52" s="50"/>
       <c r="C52" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="51" t="s">
         <v>665</v>
       </c>
       <c r="E52" s="50" t="s">
-        <v>586</v>
+        <v>600</v>
       </c>
       <c r="F52" s="74" t="s">
         <v>585</v>
@@ -49820,16 +49817,16 @@
       </c>
       <c r="B53" s="50"/>
       <c r="C53" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="D53" s="36" t="s">
-        <v>666</v>
+        <v>73</v>
+      </c>
+      <c r="D53" s="51" t="s">
+        <v>671</v>
       </c>
       <c r="E53" s="50" t="s">
-        <v>586</v>
+        <v>600</v>
       </c>
       <c r="F53" s="74" t="s">
-        <v>585</v>
+        <v>599</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -49838,16 +49835,16 @@
       </c>
       <c r="B54" s="50"/>
       <c r="C54" s="36" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>1014</v>
+        <v>672</v>
       </c>
       <c r="E54" s="50" t="s">
-        <v>586</v>
+        <v>600</v>
       </c>
       <c r="F54" s="74" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -49855,17 +49852,17 @@
         <v>42736</v>
       </c>
       <c r="B55" s="50"/>
-      <c r="C55" s="38" t="s">
-        <v>76</v>
+      <c r="C55" s="36" t="s">
+        <v>73</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>665</v>
-      </c>
-      <c r="E55" s="86" t="s">
-        <v>586</v>
+        <v>672</v>
+      </c>
+      <c r="E55" s="50" t="s">
+        <v>602</v>
       </c>
       <c r="F55" s="74" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -49873,13 +49870,13 @@
         <v>42736</v>
       </c>
       <c r="B56" s="50"/>
-      <c r="C56" s="38" t="s">
-        <v>76</v>
+      <c r="C56" s="36" t="s">
+        <v>88</v>
       </c>
       <c r="D56" s="36" t="s">
-        <v>992</v>
-      </c>
-      <c r="E56" s="86" t="s">
+        <v>665</v>
+      </c>
+      <c r="E56" s="50" t="s">
         <v>586</v>
       </c>
       <c r="F56" s="74" t="s">
@@ -49887,74 +49884,74 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A57" s="41">
-        <v>42736</v>
-      </c>
-      <c r="B57" s="55"/>
-      <c r="C57" s="43" t="s">
+      <c r="A57" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B57" s="50"/>
+      <c r="C57" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" s="36" t="s">
+        <v>666</v>
+      </c>
+      <c r="E57" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="F57" s="74" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A58" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B58" s="50"/>
+      <c r="C58" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" s="36" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E58" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="F58" s="74" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A59" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B59" s="50"/>
+      <c r="C59" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D57" s="53" t="s">
-        <v>995</v>
-      </c>
-      <c r="E57" s="127" t="s">
+      <c r="D59" s="36" t="s">
+        <v>665</v>
+      </c>
+      <c r="E59" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F57" s="79" t="s">
+      <c r="F59" s="74" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A58" s="41">
-        <v>42736</v>
-      </c>
-      <c r="B58" s="39"/>
-      <c r="C58" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D58" s="51" t="s">
-        <v>999</v>
-      </c>
-      <c r="E58" s="127" t="s">
+    <row r="60" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A60" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B60" s="50"/>
+      <c r="C60" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" s="36" t="s">
+        <v>992</v>
+      </c>
+      <c r="E60" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F58" s="79" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A59" s="41">
-        <v>42736</v>
-      </c>
-      <c r="B59" s="39"/>
-      <c r="C59" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D59" s="51" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E59" s="127" t="s">
-        <v>586</v>
-      </c>
-      <c r="F59" s="79" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A60" s="41">
-        <v>42736</v>
-      </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D60" s="51" t="s">
-        <v>1004</v>
-      </c>
-      <c r="E60" s="127" t="s">
-        <v>586</v>
-      </c>
-      <c r="F60" s="79" t="s">
+      <c r="F60" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -49962,12 +49959,12 @@
       <c r="A61" s="41">
         <v>42736</v>
       </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D61" s="54" t="s">
-        <v>1006</v>
+      <c r="B61" s="55"/>
+      <c r="C61" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="53" t="s">
+        <v>995</v>
       </c>
       <c r="E61" s="127" t="s">
         <v>586</v>
@@ -49980,105 +49977,105 @@
       <c r="A62" s="41">
         <v>42736</v>
       </c>
-      <c r="B62" s="55"/>
-      <c r="C62" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="D62" s="53" t="s">
-        <v>665</v>
-      </c>
-      <c r="E62" s="246" t="s">
-        <v>1229</v>
+      <c r="B62" s="39"/>
+      <c r="C62" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="51" t="s">
+        <v>999</v>
+      </c>
+      <c r="E62" s="127" t="s">
+        <v>586</v>
       </c>
       <c r="F62" s="79" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A63" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B63" s="50"/>
-      <c r="C63" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D63" s="38" t="s">
-        <v>666</v>
-      </c>
-      <c r="E63" s="246" t="s">
-        <v>1229</v>
-      </c>
-      <c r="F63" s="74" t="s">
+      <c r="A63" s="41">
+        <v>42736</v>
+      </c>
+      <c r="B63" s="39"/>
+      <c r="C63" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="51" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E63" s="127" t="s">
+        <v>586</v>
+      </c>
+      <c r="F63" s="79" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="290" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A64" s="34">
+    <row r="64" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A64" s="41">
         <v>42736</v>
       </c>
       <c r="B64" s="39"/>
       <c r="C64" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D64" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" s="51" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E64" s="127" t="s">
+        <v>586</v>
+      </c>
+      <c r="F64" s="79" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A65" s="41">
+        <v>42736</v>
+      </c>
+      <c r="B65" s="42"/>
+      <c r="C65" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D65" s="54" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E65" s="127" t="s">
+        <v>586</v>
+      </c>
+      <c r="F65" s="79" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A66" s="41">
+        <v>42736</v>
+      </c>
+      <c r="B66" s="55"/>
+      <c r="C66" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" s="53" t="s">
         <v>665</v>
       </c>
-      <c r="E64" s="387" t="s">
-        <v>1228</v>
-      </c>
-      <c r="F64" s="74" t="s">
+      <c r="E66" s="246" t="s">
+        <v>1229</v>
+      </c>
+      <c r="F66" s="79" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="290" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A65" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B65" s="39"/>
-      <c r="C65" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D65" s="36" t="s">
-        <v>692</v>
-      </c>
-      <c r="E65" s="387" t="s">
-        <v>1227</v>
-      </c>
-      <c r="F65" s="74" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="290" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A66" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B66" s="39"/>
-      <c r="C66" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D66" s="36" t="s">
-        <v>665</v>
-      </c>
-      <c r="E66" s="387" t="s">
-        <v>586</v>
-      </c>
-      <c r="F66" s="74" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="290" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="67" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="34">
         <v>42736</v>
       </c>
-      <c r="B67" s="39"/>
-      <c r="C67" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D67" s="36" t="s">
-        <v>692</v>
-      </c>
-      <c r="E67" s="387" t="s">
-        <v>586</v>
+      <c r="B67" s="50"/>
+      <c r="C67" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="38" t="s">
+        <v>666</v>
+      </c>
+      <c r="E67" s="246" t="s">
+        <v>1229</v>
       </c>
       <c r="F67" s="74" t="s">
         <v>585</v>
@@ -50093,10 +50090,10 @@
         <v>91</v>
       </c>
       <c r="D68" s="36" t="s">
-        <v>693</v>
+        <v>665</v>
       </c>
       <c r="E68" s="387" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="F68" s="74" t="s">
         <v>585</v>
@@ -50111,16 +50108,16 @@
         <v>91</v>
       </c>
       <c r="D69" s="36" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E69" s="387" t="s">
-        <v>586</v>
+        <v>1227</v>
       </c>
       <c r="F69" s="74" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="13.35" customHeight="1">
+    <row r="70" spans="1:6" s="290" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="34">
         <v>42736</v>
       </c>
@@ -50128,8 +50125,8 @@
       <c r="C70" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D70" s="404" t="s">
-        <v>689</v>
+      <c r="D70" s="36" t="s">
+        <v>665</v>
       </c>
       <c r="E70" s="387" t="s">
         <v>586</v>
@@ -50144,13 +50141,13 @@
       </c>
       <c r="B71" s="39"/>
       <c r="C71" s="38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D71" s="36" t="s">
-        <v>665</v>
+        <v>692</v>
       </c>
       <c r="E71" s="387" t="s">
-        <v>1228</v>
+        <v>586</v>
       </c>
       <c r="F71" s="74" t="s">
         <v>585</v>
@@ -50162,13 +50159,13 @@
       </c>
       <c r="B72" s="39"/>
       <c r="C72" s="38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D72" s="36" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E72" s="387" t="s">
-        <v>1227</v>
+        <v>1230</v>
       </c>
       <c r="F72" s="74" t="s">
         <v>585</v>
@@ -50180,10 +50177,10 @@
       </c>
       <c r="B73" s="39"/>
       <c r="C73" s="38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>665</v>
+        <v>693</v>
       </c>
       <c r="E73" s="387" t="s">
         <v>586</v>
@@ -50192,16 +50189,16 @@
         <v>585</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="290" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="74" spans="1:6" ht="13.35" customHeight="1">
       <c r="A74" s="34">
         <v>42736</v>
       </c>
       <c r="B74" s="39"/>
       <c r="C74" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D74" s="36" t="s">
-        <v>694</v>
+        <v>91</v>
+      </c>
+      <c r="D74" s="404" t="s">
+        <v>689</v>
       </c>
       <c r="E74" s="387" t="s">
         <v>586</v>
@@ -50219,10 +50216,10 @@
         <v>94</v>
       </c>
       <c r="D75" s="36" t="s">
-        <v>693</v>
+        <v>665</v>
       </c>
       <c r="E75" s="387" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="F75" s="74" t="s">
         <v>585</v>
@@ -50232,17 +50229,17 @@
       <c r="A76" s="34">
         <v>42736</v>
       </c>
-      <c r="B76" s="42"/>
-      <c r="C76" s="43" t="s">
+      <c r="B76" s="39"/>
+      <c r="C76" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="D76" s="53" t="s">
-        <v>693</v>
-      </c>
-      <c r="E76" s="246" t="s">
-        <v>586</v>
-      </c>
-      <c r="F76" s="79" t="s">
+      <c r="D76" s="36" t="s">
+        <v>694</v>
+      </c>
+      <c r="E76" s="387" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F76" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50252,7 +50249,7 @@
       </c>
       <c r="B77" s="39"/>
       <c r="C77" s="38" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D77" s="36" t="s">
         <v>665</v>
@@ -50270,15 +50267,15 @@
       </c>
       <c r="B78" s="39"/>
       <c r="C78" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="D78" s="38" t="s">
-        <v>1018</v>
-      </c>
-      <c r="E78" s="246" t="s">
+        <v>94</v>
+      </c>
+      <c r="D78" s="36" t="s">
+        <v>694</v>
+      </c>
+      <c r="E78" s="387" t="s">
         <v>586</v>
       </c>
-      <c r="F78" s="79" t="s">
+      <c r="F78" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50287,14 +50284,14 @@
         <v>42736</v>
       </c>
       <c r="B79" s="39"/>
-      <c r="C79" s="428" t="s">
-        <v>100</v>
-      </c>
-      <c r="D79" s="428" t="s">
-        <v>673</v>
+      <c r="C79" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79" s="36" t="s">
+        <v>693</v>
       </c>
       <c r="E79" s="387" t="s">
-        <v>586</v>
+        <v>1230</v>
       </c>
       <c r="F79" s="74" t="s">
         <v>585</v>
@@ -50304,12 +50301,12 @@
       <c r="A80" s="34">
         <v>42736</v>
       </c>
-      <c r="B80" s="39"/>
-      <c r="C80" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="D80" s="38" t="s">
-        <v>674</v>
+      <c r="B80" s="42"/>
+      <c r="C80" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="D80" s="53" t="s">
+        <v>693</v>
       </c>
       <c r="E80" s="246" t="s">
         <v>586</v>
@@ -50318,111 +50315,111 @@
         <v>585</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A81" s="440">
-        <v>42736</v>
-      </c>
-      <c r="B81" s="434"/>
-      <c r="C81" s="472" t="s">
-        <v>103</v>
-      </c>
-      <c r="D81" s="433" t="s">
+    <row r="81" spans="1:6" s="290" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A81" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B81" s="39"/>
+      <c r="C81" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D81" s="36" t="s">
         <v>665</v>
       </c>
-      <c r="E81" s="434" t="s">
+      <c r="E81" s="387" t="s">
         <v>586</v>
       </c>
-      <c r="F81" s="471" t="s">
+      <c r="F81" s="74" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A82" s="440">
-        <v>42736</v>
-      </c>
-      <c r="B82" s="434"/>
-      <c r="C82" s="472" t="s">
-        <v>103</v>
-      </c>
-      <c r="D82" s="433" t="s">
-        <v>666</v>
-      </c>
-      <c r="E82" s="434" t="s">
+    <row r="82" spans="1:6" s="290" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A82" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B82" s="39"/>
+      <c r="C82" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D82" s="38" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E82" s="246" t="s">
         <v>586</v>
       </c>
-      <c r="F82" s="471" t="s">
+      <c r="F82" s="79" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="20.100000000000001" customHeight="1">
+    <row r="83" spans="1:6" s="290" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A83" s="34">
         <v>42736</v>
       </c>
-      <c r="B83" s="50"/>
-      <c r="C83" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D83" s="36" t="s">
-        <v>665</v>
-      </c>
-      <c r="E83" s="86" t="s">
+      <c r="B83" s="39"/>
+      <c r="C83" s="428" t="s">
+        <v>100</v>
+      </c>
+      <c r="D83" s="428" t="s">
+        <v>673</v>
+      </c>
+      <c r="E83" s="387" t="s">
         <v>586</v>
       </c>
       <c r="F83" s="74" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="20.100000000000001" customHeight="1">
+    <row r="84" spans="1:6" s="290" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A84" s="34">
         <v>42736</v>
       </c>
-      <c r="B84" s="50"/>
-      <c r="C84" s="36" t="s">
-        <v>106</v>
+      <c r="B84" s="39"/>
+      <c r="C84" s="38" t="s">
+        <v>100</v>
       </c>
       <c r="D84" s="38" t="s">
-        <v>1036</v>
-      </c>
-      <c r="E84" s="86" t="s">
+        <v>674</v>
+      </c>
+      <c r="E84" s="246" t="s">
         <v>586</v>
       </c>
-      <c r="F84" s="188" t="s">
-        <v>587</v>
+      <c r="F84" s="79" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A85" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B85" s="50"/>
-      <c r="C85" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D85" s="38" t="s">
-        <v>1038</v>
-      </c>
-      <c r="E85" s="86" t="s">
+      <c r="A85" s="440">
+        <v>42736</v>
+      </c>
+      <c r="B85" s="434"/>
+      <c r="C85" s="472" t="s">
+        <v>103</v>
+      </c>
+      <c r="D85" s="433" t="s">
+        <v>665</v>
+      </c>
+      <c r="E85" s="434" t="s">
         <v>586</v>
       </c>
-      <c r="F85" s="74" t="s">
+      <c r="F85" s="471" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A86" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B86" s="50"/>
-      <c r="C86" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D86" s="38" t="s">
-        <v>1040</v>
-      </c>
-      <c r="E86" s="86" t="s">
+      <c r="A86" s="440">
+        <v>42736</v>
+      </c>
+      <c r="B86" s="434"/>
+      <c r="C86" s="472" t="s">
+        <v>103</v>
+      </c>
+      <c r="D86" s="433" t="s">
+        <v>666</v>
+      </c>
+      <c r="E86" s="434" t="s">
         <v>586</v>
       </c>
-      <c r="F86" s="74" t="s">
+      <c r="F86" s="471" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50434,8 +50431,8 @@
       <c r="C87" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D87" s="38" t="s">
-        <v>1044</v>
+      <c r="D87" s="36" t="s">
+        <v>665</v>
       </c>
       <c r="E87" s="86" t="s">
         <v>586</v>
@@ -50452,14 +50449,14 @@
       <c r="C88" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>1042</v>
+      <c r="D88" s="38" t="s">
+        <v>1036</v>
       </c>
       <c r="E88" s="86" t="s">
         <v>586</v>
       </c>
       <c r="F88" s="188" t="s">
-        <v>1231</v>
+        <v>587</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -50471,13 +50468,13 @@
         <v>106</v>
       </c>
       <c r="D89" s="38" t="s">
-        <v>1047</v>
+        <v>1038</v>
       </c>
       <c r="E89" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F89" s="188" t="s">
-        <v>1231</v>
+      <c r="F89" s="74" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -50489,7 +50486,7 @@
         <v>106</v>
       </c>
       <c r="D90" s="38" t="s">
-        <v>1052</v>
+        <v>1040</v>
       </c>
       <c r="E90" s="86" t="s">
         <v>586</v>
@@ -50506,50 +50503,50 @@
       <c r="C91" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>1050</v>
+      <c r="D91" s="38" t="s">
+        <v>1044</v>
       </c>
       <c r="E91" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F91" s="188" t="s">
+      <c r="F91" s="74" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="92" spans="1:6" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A92" s="485">
-        <v>42736</v>
-      </c>
-      <c r="B92" s="531"/>
-      <c r="C92" s="483" t="s">
-        <v>109</v>
-      </c>
-      <c r="D92" s="483" t="s">
-        <v>665</v>
-      </c>
-      <c r="E92" s="517" t="s">
+    <row r="92" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A92" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B92" s="50"/>
+      <c r="C92" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E92" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F92" s="532" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A93" s="485">
-        <v>42736</v>
-      </c>
-      <c r="B93" s="531"/>
-      <c r="C93" s="483" t="s">
-        <v>109</v>
-      </c>
-      <c r="D93" s="483" t="s">
-        <v>665</v>
-      </c>
-      <c r="E93" s="517" t="s">
-        <v>1227</v>
-      </c>
-      <c r="F93" s="532" t="s">
-        <v>585</v>
+      <c r="F92" s="188" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A93" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B93" s="50"/>
+      <c r="C93" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D93" s="38" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E93" s="86" t="s">
+        <v>586</v>
+      </c>
+      <c r="F93" s="188" t="s">
+        <v>1231</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -50557,11 +50554,11 @@
         <v>42736</v>
       </c>
       <c r="B94" s="50"/>
-      <c r="C94" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D94" s="36" t="s">
-        <v>665</v>
+      <c r="C94" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D94" s="38" t="s">
+        <v>1052</v>
       </c>
       <c r="E94" s="86" t="s">
         <v>586</v>
@@ -50575,16 +50572,16 @@
         <v>42736</v>
       </c>
       <c r="B95" s="50"/>
-      <c r="C95" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D95" s="38" t="s">
-        <v>1036</v>
+      <c r="C95" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>1050</v>
       </c>
       <c r="E95" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F95" s="74" t="s">
+      <c r="F95" s="188" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50592,9 +50589,9 @@
       <c r="A96" s="485">
         <v>42736</v>
       </c>
-      <c r="B96" s="531"/>
+      <c r="B96" s="530"/>
       <c r="C96" s="483" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D96" s="483" t="s">
         <v>665</v>
@@ -50602,7 +50599,7 @@
       <c r="E96" s="517" t="s">
         <v>586</v>
       </c>
-      <c r="F96" s="532" t="s">
+      <c r="F96" s="531" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50610,17 +50607,89 @@
       <c r="A97" s="485">
         <v>42736</v>
       </c>
-      <c r="B97" s="531"/>
+      <c r="B97" s="530"/>
       <c r="C97" s="483" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D97" s="483" t="s">
         <v>665</v>
       </c>
       <c r="E97" s="517" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F97" s="531" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A98" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B98" s="50"/>
+      <c r="C98" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D98" s="36" t="s">
+        <v>665</v>
+      </c>
+      <c r="E98" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F97" s="532" t="s">
+      <c r="F98" s="74" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A99" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B99" s="50"/>
+      <c r="C99" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D99" s="38" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E99" s="86" t="s">
+        <v>586</v>
+      </c>
+      <c r="F99" s="74" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A100" s="485">
+        <v>42736</v>
+      </c>
+      <c r="B100" s="530"/>
+      <c r="C100" s="483" t="s">
+        <v>115</v>
+      </c>
+      <c r="D100" s="483" t="s">
+        <v>665</v>
+      </c>
+      <c r="E100" s="517" t="s">
+        <v>586</v>
+      </c>
+      <c r="F100" s="531" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A101" s="485">
+        <v>42736</v>
+      </c>
+      <c r="B101" s="530"/>
+      <c r="C101" s="483" t="s">
+        <v>118</v>
+      </c>
+      <c r="D101" s="483" t="s">
+        <v>665</v>
+      </c>
+      <c r="E101" s="517" t="s">
+        <v>586</v>
+      </c>
+      <c r="F101" s="531" t="s">
         <v>587</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RDM-12846 - remove duplicate AuthorisationCaseEvent.json
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C1E43-262F-9C49-A97F-0D44D296496C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F9CE50-407F-9341-9B30-B7755BDA0301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20480" firstSheet="13" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20480" firstSheet="16" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10024" uniqueCount="1284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10020" uniqueCount="1284">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -15198,7 +15198,7 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F86" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F85" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="26"/>
@@ -26023,7 +26023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:T259"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -26045,7 +26045,7 @@
     <col min="15" max="15" width="42.5" style="1" customWidth="1"/>
     <col min="16" max="16" width="28.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="54" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.83203125" style="2"/>
+    <col min="18" max="18" width="25.5" style="2" customWidth="1"/>
     <col min="19" max="19" width="15.33203125" style="2" customWidth="1"/>
     <col min="20" max="20" width="23.1640625" style="2" customWidth="1"/>
     <col min="21" max="16384" width="8.83203125" style="2"/>
@@ -48645,10 +48645,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:EK102"/>
+  <dimension ref="A1:EK101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -48737,14 +48737,14 @@
     </row>
     <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" s="34">
-        <v>42739</v>
+        <v>42736</v>
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>665</v>
+      <c r="D5" s="38" t="s">
+        <v>926</v>
       </c>
       <c r="E5" s="86" t="s">
         <v>586</v>
@@ -48765,7 +48765,7 @@
         <v>926</v>
       </c>
       <c r="E6" s="86" t="s">
-        <v>586</v>
+        <v>1228</v>
       </c>
       <c r="F6" s="74" t="s">
         <v>585</v>
@@ -48779,11 +48779,11 @@
       <c r="C7" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="38" t="s">
-        <v>926</v>
-      </c>
-      <c r="E7" s="86" t="s">
-        <v>1228</v>
+      <c r="D7" s="36" t="s">
+        <v>665</v>
+      </c>
+      <c r="E7" s="136" t="s">
+        <v>1244</v>
       </c>
       <c r="F7" s="74" t="s">
         <v>585</v>
@@ -48797,11 +48797,11 @@
       <c r="C8" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="36" t="s">
-        <v>665</v>
-      </c>
-      <c r="E8" s="136" t="s">
-        <v>1244</v>
+      <c r="D8" s="38" t="s">
+        <v>666</v>
+      </c>
+      <c r="E8" s="86" t="s">
+        <v>586</v>
       </c>
       <c r="F8" s="74" t="s">
         <v>585</v>
@@ -48819,7 +48819,7 @@
         <v>666</v>
       </c>
       <c r="E9" s="86" t="s">
-        <v>586</v>
+        <v>1227</v>
       </c>
       <c r="F9" s="74" t="s">
         <v>585</v>
@@ -48834,10 +48834,10 @@
         <v>41</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>666</v>
+        <v>928</v>
       </c>
       <c r="E10" s="86" t="s">
-        <v>1227</v>
+        <v>586</v>
       </c>
       <c r="F10" s="74" t="s">
         <v>585</v>
@@ -48855,7 +48855,7 @@
         <v>928</v>
       </c>
       <c r="E11" s="86" t="s">
-        <v>586</v>
+        <v>1228</v>
       </c>
       <c r="F11" s="74" t="s">
         <v>585</v>
@@ -48863,17 +48863,17 @@
     </row>
     <row r="12" spans="1:6" ht="20" customHeight="1">
       <c r="A12" s="34">
-        <v>42736</v>
+        <v>42737</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="36" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>928</v>
+        <v>933</v>
       </c>
       <c r="E12" s="86" t="s">
-        <v>1228</v>
+        <v>586</v>
       </c>
       <c r="F12" s="74" t="s">
         <v>585</v>
@@ -48881,14 +48881,14 @@
     </row>
     <row r="13" spans="1:6" ht="20" customHeight="1">
       <c r="A13" s="34">
-        <v>42737</v>
+        <v>42738</v>
       </c>
       <c r="B13" s="50"/>
       <c r="C13" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="38" t="s">
-        <v>933</v>
+      <c r="D13" s="489" t="s">
+        <v>936</v>
       </c>
       <c r="E13" s="86" t="s">
         <v>586</v>
@@ -48899,14 +48899,14 @@
     </row>
     <row r="14" spans="1:6" ht="20" customHeight="1">
       <c r="A14" s="34">
-        <v>42738</v>
+        <v>42739</v>
       </c>
       <c r="B14" s="50"/>
       <c r="C14" s="36" t="s">
         <v>41</v>
       </c>
       <c r="D14" s="489" t="s">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c r="E14" s="86" t="s">
         <v>586</v>
@@ -48917,14 +48917,14 @@
     </row>
     <row r="15" spans="1:6" ht="20" customHeight="1">
       <c r="A15" s="34">
-        <v>42739</v>
+        <v>42740</v>
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="36" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="489" t="s">
-        <v>940</v>
+        <v>944</v>
       </c>
       <c r="E15" s="86" t="s">
         <v>586</v>
@@ -48935,14 +48935,14 @@
     </row>
     <row r="16" spans="1:6" ht="20" customHeight="1">
       <c r="A16" s="34">
-        <v>42740</v>
+        <v>42736</v>
       </c>
       <c r="B16" s="50"/>
       <c r="C16" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="489" t="s">
-        <v>944</v>
+        <v>46</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>665</v>
       </c>
       <c r="E16" s="86" t="s">
         <v>586</v>
@@ -48959,8 +48959,8 @@
       <c r="C17" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="36" t="s">
-        <v>665</v>
+      <c r="D17" s="38" t="s">
+        <v>949</v>
       </c>
       <c r="E17" s="86" t="s">
         <v>586</v>
@@ -48974,11 +48974,11 @@
         <v>42736</v>
       </c>
       <c r="B18" s="50"/>
-      <c r="C18" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>949</v>
+      <c r="C18" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>665</v>
       </c>
       <c r="E18" s="86" t="s">
         <v>586</v>
@@ -48992,11 +48992,11 @@
         <v>42736</v>
       </c>
       <c r="B19" s="50"/>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="36" t="s">
-        <v>665</v>
+      <c r="D19" s="76" t="s">
+        <v>667</v>
       </c>
       <c r="E19" s="86" t="s">
         <v>586</v>
@@ -49010,11 +49010,11 @@
         <v>42736</v>
       </c>
       <c r="B20" s="50"/>
-      <c r="C20" s="76" t="s">
+      <c r="C20" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="76" t="s">
-        <v>667</v>
+      <c r="D20" s="77" t="s">
+        <v>629</v>
       </c>
       <c r="E20" s="86" t="s">
         <v>586</v>
@@ -49032,7 +49032,7 @@
         <v>49</v>
       </c>
       <c r="D21" s="77" t="s">
-        <v>629</v>
+        <v>956</v>
       </c>
       <c r="E21" s="86" t="s">
         <v>586</v>
@@ -49050,7 +49050,7 @@
         <v>49</v>
       </c>
       <c r="D22" s="77" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E22" s="86" t="s">
         <v>586</v>
@@ -49068,7 +49068,7 @@
         <v>49</v>
       </c>
       <c r="D23" s="77" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="E23" s="86" t="s">
         <v>586</v>
@@ -49077,23 +49077,158 @@
         <v>585</v>
       </c>
     </row>
-    <row r="24" spans="1:141" ht="20" customHeight="1">
-      <c r="A24" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="77" t="s">
-        <v>960</v>
-      </c>
-      <c r="E24" s="86" t="s">
+    <row r="24" spans="1:141" s="192" customFormat="1" ht="20" customHeight="1">
+      <c r="A24" s="190">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="191"/>
+      <c r="C24" s="193" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="193" t="s">
+        <v>662</v>
+      </c>
+      <c r="E24" s="217" t="s">
         <v>586</v>
       </c>
-      <c r="F24" s="74" t="s">
+      <c r="F24" s="194" t="s">
         <v>585</v>
       </c>
+      <c r="G24" s="238"/>
+      <c r="H24" s="238"/>
+      <c r="I24" s="238"/>
+      <c r="J24" s="238"/>
+      <c r="K24" s="238"/>
+      <c r="L24" s="238"/>
+      <c r="M24" s="238"/>
+      <c r="N24" s="238"/>
+      <c r="O24" s="238"/>
+      <c r="P24" s="238"/>
+      <c r="Q24" s="238"/>
+      <c r="R24" s="238"/>
+      <c r="S24" s="238"/>
+      <c r="T24" s="238"/>
+      <c r="U24" s="238"/>
+      <c r="V24" s="238"/>
+      <c r="W24" s="238"/>
+      <c r="X24" s="238"/>
+      <c r="Y24" s="238"/>
+      <c r="Z24" s="238"/>
+      <c r="AA24" s="238"/>
+      <c r="AB24" s="238"/>
+      <c r="AC24" s="238"/>
+      <c r="AD24" s="238"/>
+      <c r="AE24" s="238"/>
+      <c r="AF24" s="238"/>
+      <c r="AG24" s="238"/>
+      <c r="AH24" s="238"/>
+      <c r="AI24" s="238"/>
+      <c r="AJ24" s="238"/>
+      <c r="AK24" s="238"/>
+      <c r="AL24" s="238"/>
+      <c r="AM24" s="238"/>
+      <c r="AN24" s="238"/>
+      <c r="AO24" s="238"/>
+      <c r="AP24" s="238"/>
+      <c r="AQ24" s="238"/>
+      <c r="AR24" s="238"/>
+      <c r="AS24" s="238"/>
+      <c r="AT24" s="238"/>
+      <c r="AU24" s="238"/>
+      <c r="AV24" s="238"/>
+      <c r="AW24" s="238"/>
+      <c r="AX24" s="238"/>
+      <c r="AY24" s="238"/>
+      <c r="AZ24" s="238"/>
+      <c r="BA24" s="238"/>
+      <c r="BB24" s="238"/>
+      <c r="BC24" s="238"/>
+      <c r="BD24" s="238"/>
+      <c r="BE24" s="238"/>
+      <c r="BF24" s="238"/>
+      <c r="BG24" s="238"/>
+      <c r="BH24" s="238"/>
+      <c r="BI24" s="238"/>
+      <c r="BJ24" s="238"/>
+      <c r="BK24" s="238"/>
+      <c r="BL24" s="238"/>
+      <c r="BM24" s="238"/>
+      <c r="BN24" s="238"/>
+      <c r="BO24" s="238"/>
+      <c r="BP24" s="238"/>
+      <c r="BQ24" s="238"/>
+      <c r="BR24" s="238"/>
+      <c r="BS24" s="238"/>
+      <c r="BT24" s="238"/>
+      <c r="BU24" s="238"/>
+      <c r="BV24" s="238"/>
+      <c r="BW24" s="238"/>
+      <c r="BX24" s="238"/>
+      <c r="BY24" s="238"/>
+      <c r="BZ24" s="238"/>
+      <c r="CA24" s="238"/>
+      <c r="CB24" s="238"/>
+      <c r="CC24" s="238"/>
+      <c r="CD24" s="238"/>
+      <c r="CE24" s="238"/>
+      <c r="CF24" s="238"/>
+      <c r="CG24" s="238"/>
+      <c r="CH24" s="238"/>
+      <c r="CI24" s="238"/>
+      <c r="CJ24" s="238"/>
+      <c r="CK24" s="238"/>
+      <c r="CL24" s="238"/>
+      <c r="CM24" s="238"/>
+      <c r="CN24" s="238"/>
+      <c r="CO24" s="238"/>
+      <c r="CP24" s="238"/>
+      <c r="CQ24" s="238"/>
+      <c r="CR24" s="238"/>
+      <c r="CS24" s="238"/>
+      <c r="CT24" s="238"/>
+      <c r="CU24" s="238"/>
+      <c r="CV24" s="238"/>
+      <c r="CW24" s="238"/>
+      <c r="CX24" s="238"/>
+      <c r="CY24" s="238"/>
+      <c r="CZ24" s="238"/>
+      <c r="DA24" s="238"/>
+      <c r="DB24" s="238"/>
+      <c r="DC24" s="238"/>
+      <c r="DD24" s="238"/>
+      <c r="DE24" s="238"/>
+      <c r="DF24" s="238"/>
+      <c r="DG24" s="238"/>
+      <c r="DH24" s="238"/>
+      <c r="DI24" s="238"/>
+      <c r="DJ24" s="238"/>
+      <c r="DK24" s="238"/>
+      <c r="DL24" s="238"/>
+      <c r="DM24" s="238"/>
+      <c r="DN24" s="238"/>
+      <c r="DO24" s="238"/>
+      <c r="DP24" s="238"/>
+      <c r="DQ24" s="238"/>
+      <c r="DR24" s="238"/>
+      <c r="DS24" s="238"/>
+      <c r="DT24" s="238"/>
+      <c r="DU24" s="238"/>
+      <c r="DV24" s="238"/>
+      <c r="DW24" s="238"/>
+      <c r="DX24" s="238"/>
+      <c r="DY24" s="238"/>
+      <c r="DZ24" s="238"/>
+      <c r="EA24" s="238"/>
+      <c r="EB24" s="238"/>
+      <c r="EC24" s="238"/>
+      <c r="ED24" s="238"/>
+      <c r="EE24" s="238"/>
+      <c r="EF24" s="238"/>
+      <c r="EG24" s="238"/>
+      <c r="EH24" s="238"/>
+      <c r="EI24" s="238"/>
+      <c r="EJ24" s="238"/>
+      <c r="EK24" s="238"/>
     </row>
     <row r="25" spans="1:141" s="192" customFormat="1" ht="20" customHeight="1">
       <c r="A25" s="190">
@@ -49104,7 +49239,7 @@
         <v>82</v>
       </c>
       <c r="D25" s="193" t="s">
-        <v>662</v>
+        <v>645</v>
       </c>
       <c r="E25" s="217" t="s">
         <v>586</v>
@@ -49248,158 +49383,23 @@
       <c r="EJ25" s="238"/>
       <c r="EK25" s="238"/>
     </row>
-    <row r="26" spans="1:141" s="192" customFormat="1" ht="20" customHeight="1">
-      <c r="A26" s="190">
-        <v>42736</v>
-      </c>
-      <c r="B26" s="191"/>
-      <c r="C26" s="193" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="193" t="s">
-        <v>645</v>
-      </c>
-      <c r="E26" s="217" t="s">
+    <row r="26" spans="1:141" ht="20" customHeight="1">
+      <c r="A26" s="266">
+        <v>42736</v>
+      </c>
+      <c r="B26" s="233"/>
+      <c r="C26" s="248" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="234" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E26" s="268" t="s">
         <v>586</v>
       </c>
-      <c r="F26" s="194" t="s">
+      <c r="F26" s="252" t="s">
         <v>585</v>
       </c>
-      <c r="G26" s="238"/>
-      <c r="H26" s="238"/>
-      <c r="I26" s="238"/>
-      <c r="J26" s="238"/>
-      <c r="K26" s="238"/>
-      <c r="L26" s="238"/>
-      <c r="M26" s="238"/>
-      <c r="N26" s="238"/>
-      <c r="O26" s="238"/>
-      <c r="P26" s="238"/>
-      <c r="Q26" s="238"/>
-      <c r="R26" s="238"/>
-      <c r="S26" s="238"/>
-      <c r="T26" s="238"/>
-      <c r="U26" s="238"/>
-      <c r="V26" s="238"/>
-      <c r="W26" s="238"/>
-      <c r="X26" s="238"/>
-      <c r="Y26" s="238"/>
-      <c r="Z26" s="238"/>
-      <c r="AA26" s="238"/>
-      <c r="AB26" s="238"/>
-      <c r="AC26" s="238"/>
-      <c r="AD26" s="238"/>
-      <c r="AE26" s="238"/>
-      <c r="AF26" s="238"/>
-      <c r="AG26" s="238"/>
-      <c r="AH26" s="238"/>
-      <c r="AI26" s="238"/>
-      <c r="AJ26" s="238"/>
-      <c r="AK26" s="238"/>
-      <c r="AL26" s="238"/>
-      <c r="AM26" s="238"/>
-      <c r="AN26" s="238"/>
-      <c r="AO26" s="238"/>
-      <c r="AP26" s="238"/>
-      <c r="AQ26" s="238"/>
-      <c r="AR26" s="238"/>
-      <c r="AS26" s="238"/>
-      <c r="AT26" s="238"/>
-      <c r="AU26" s="238"/>
-      <c r="AV26" s="238"/>
-      <c r="AW26" s="238"/>
-      <c r="AX26" s="238"/>
-      <c r="AY26" s="238"/>
-      <c r="AZ26" s="238"/>
-      <c r="BA26" s="238"/>
-      <c r="BB26" s="238"/>
-      <c r="BC26" s="238"/>
-      <c r="BD26" s="238"/>
-      <c r="BE26" s="238"/>
-      <c r="BF26" s="238"/>
-      <c r="BG26" s="238"/>
-      <c r="BH26" s="238"/>
-      <c r="BI26" s="238"/>
-      <c r="BJ26" s="238"/>
-      <c r="BK26" s="238"/>
-      <c r="BL26" s="238"/>
-      <c r="BM26" s="238"/>
-      <c r="BN26" s="238"/>
-      <c r="BO26" s="238"/>
-      <c r="BP26" s="238"/>
-      <c r="BQ26" s="238"/>
-      <c r="BR26" s="238"/>
-      <c r="BS26" s="238"/>
-      <c r="BT26" s="238"/>
-      <c r="BU26" s="238"/>
-      <c r="BV26" s="238"/>
-      <c r="BW26" s="238"/>
-      <c r="BX26" s="238"/>
-      <c r="BY26" s="238"/>
-      <c r="BZ26" s="238"/>
-      <c r="CA26" s="238"/>
-      <c r="CB26" s="238"/>
-      <c r="CC26" s="238"/>
-      <c r="CD26" s="238"/>
-      <c r="CE26" s="238"/>
-      <c r="CF26" s="238"/>
-      <c r="CG26" s="238"/>
-      <c r="CH26" s="238"/>
-      <c r="CI26" s="238"/>
-      <c r="CJ26" s="238"/>
-      <c r="CK26" s="238"/>
-      <c r="CL26" s="238"/>
-      <c r="CM26" s="238"/>
-      <c r="CN26" s="238"/>
-      <c r="CO26" s="238"/>
-      <c r="CP26" s="238"/>
-      <c r="CQ26" s="238"/>
-      <c r="CR26" s="238"/>
-      <c r="CS26" s="238"/>
-      <c r="CT26" s="238"/>
-      <c r="CU26" s="238"/>
-      <c r="CV26" s="238"/>
-      <c r="CW26" s="238"/>
-      <c r="CX26" s="238"/>
-      <c r="CY26" s="238"/>
-      <c r="CZ26" s="238"/>
-      <c r="DA26" s="238"/>
-      <c r="DB26" s="238"/>
-      <c r="DC26" s="238"/>
-      <c r="DD26" s="238"/>
-      <c r="DE26" s="238"/>
-      <c r="DF26" s="238"/>
-      <c r="DG26" s="238"/>
-      <c r="DH26" s="238"/>
-      <c r="DI26" s="238"/>
-      <c r="DJ26" s="238"/>
-      <c r="DK26" s="238"/>
-      <c r="DL26" s="238"/>
-      <c r="DM26" s="238"/>
-      <c r="DN26" s="238"/>
-      <c r="DO26" s="238"/>
-      <c r="DP26" s="238"/>
-      <c r="DQ26" s="238"/>
-      <c r="DR26" s="238"/>
-      <c r="DS26" s="238"/>
-      <c r="DT26" s="238"/>
-      <c r="DU26" s="238"/>
-      <c r="DV26" s="238"/>
-      <c r="DW26" s="238"/>
-      <c r="DX26" s="238"/>
-      <c r="DY26" s="238"/>
-      <c r="DZ26" s="238"/>
-      <c r="EA26" s="238"/>
-      <c r="EB26" s="238"/>
-      <c r="EC26" s="238"/>
-      <c r="ED26" s="238"/>
-      <c r="EE26" s="238"/>
-      <c r="EF26" s="238"/>
-      <c r="EG26" s="238"/>
-      <c r="EH26" s="238"/>
-      <c r="EI26" s="238"/>
-      <c r="EJ26" s="238"/>
-      <c r="EK26" s="238"/>
     </row>
     <row r="27" spans="1:141" ht="20" customHeight="1">
       <c r="A27" s="266">
@@ -49410,7 +49410,7 @@
         <v>85</v>
       </c>
       <c r="D27" s="234" t="s">
-        <v>1018</v>
+        <v>673</v>
       </c>
       <c r="E27" s="268" t="s">
         <v>586</v>
@@ -49428,7 +49428,7 @@
         <v>85</v>
       </c>
       <c r="D28" s="234" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="E28" s="268" t="s">
         <v>586</v>
@@ -49446,7 +49446,7 @@
         <v>85</v>
       </c>
       <c r="D29" s="234" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E29" s="268" t="s">
         <v>586</v>
@@ -49464,7 +49464,7 @@
         <v>85</v>
       </c>
       <c r="D30" s="234" t="s">
-        <v>675</v>
+        <v>1023</v>
       </c>
       <c r="E30" s="268" t="s">
         <v>586</v>
@@ -49482,7 +49482,7 @@
         <v>85</v>
       </c>
       <c r="D31" s="234" t="s">
-        <v>1023</v>
+        <v>677</v>
       </c>
       <c r="E31" s="268" t="s">
         <v>586</v>
@@ -49500,7 +49500,7 @@
         <v>85</v>
       </c>
       <c r="D32" s="234" t="s">
-        <v>677</v>
+        <v>682</v>
       </c>
       <c r="E32" s="268" t="s">
         <v>586</v>
@@ -49510,20 +49510,20 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="20" customHeight="1">
-      <c r="A33" s="266">
-        <v>42736</v>
-      </c>
-      <c r="B33" s="233"/>
-      <c r="C33" s="248" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="234" t="s">
-        <v>682</v>
-      </c>
-      <c r="E33" s="268" t="s">
+      <c r="A33" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B33" s="50"/>
+      <c r="C33" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>665</v>
+      </c>
+      <c r="E33" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F33" s="252" t="s">
+      <c r="F33" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -49533,7 +49533,7 @@
       </c>
       <c r="B34" s="50"/>
       <c r="C34" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D34" s="36" t="s">
         <v>665</v>
@@ -49554,7 +49554,7 @@
         <v>55</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>665</v>
+        <v>963</v>
       </c>
       <c r="E35" s="86" t="s">
         <v>586</v>
@@ -49572,7 +49572,7 @@
         <v>55</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="E36" s="86" t="s">
         <v>586</v>
@@ -49590,7 +49590,7 @@
         <v>55</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="E37" s="86" t="s">
         <v>586</v>
@@ -49608,7 +49608,7 @@
         <v>55</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="E38" s="86" t="s">
         <v>586</v>
@@ -49622,11 +49622,11 @@
         <v>42736</v>
       </c>
       <c r="B39" s="50"/>
-      <c r="C39" s="38" t="s">
-        <v>55</v>
+      <c r="C39" s="36" t="s">
+        <v>58</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>969</v>
+        <v>665</v>
       </c>
       <c r="E39" s="86" t="s">
         <v>586</v>
@@ -49641,7 +49641,7 @@
       </c>
       <c r="B40" s="50"/>
       <c r="C40" s="36" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D40" s="36" t="s">
         <v>665</v>
@@ -49662,7 +49662,7 @@
         <v>61</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>665</v>
+        <v>972</v>
       </c>
       <c r="E41" s="86" t="s">
         <v>586</v>
@@ -49680,7 +49680,7 @@
         <v>61</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>972</v>
+        <v>976</v>
       </c>
       <c r="E42" s="86" t="s">
         <v>586</v>
@@ -49698,7 +49698,7 @@
         <v>61</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="E43" s="86" t="s">
         <v>586</v>
@@ -49716,7 +49716,7 @@
         <v>61</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>974</v>
+        <v>978</v>
       </c>
       <c r="E44" s="86" t="s">
         <v>586</v>
@@ -49731,16 +49731,16 @@
       </c>
       <c r="B45" s="50"/>
       <c r="C45" s="36" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>978</v>
+        <v>665</v>
       </c>
       <c r="E45" s="86" t="s">
         <v>586</v>
       </c>
       <c r="F45" s="74" t="s">
-        <v>585</v>
+        <v>603</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="20" customHeight="1">
@@ -49748,17 +49748,17 @@
         <v>42736</v>
       </c>
       <c r="B46" s="50"/>
-      <c r="C46" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46" s="36" t="s">
+      <c r="C46" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="38" t="s">
         <v>665</v>
       </c>
       <c r="E46" s="86" t="s">
         <v>586</v>
       </c>
       <c r="F46" s="74" t="s">
-        <v>603</v>
+        <v>585</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="20" customHeight="1">
@@ -49769,8 +49769,8 @@
       <c r="C47" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="D47" s="38" t="s">
-        <v>665</v>
+      <c r="D47" s="76" t="s">
+        <v>980</v>
       </c>
       <c r="E47" s="86" t="s">
         <v>586</v>
@@ -49788,7 +49788,7 @@
         <v>64</v>
       </c>
       <c r="D48" s="76" t="s">
-        <v>980</v>
+        <v>984</v>
       </c>
       <c r="E48" s="86" t="s">
         <v>586</v>
@@ -49802,11 +49802,11 @@
         <v>42736</v>
       </c>
       <c r="B49" s="50"/>
-      <c r="C49" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="D49" s="76" t="s">
-        <v>984</v>
+      <c r="C49" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="36" t="s">
+        <v>665</v>
       </c>
       <c r="E49" s="86" t="s">
         <v>586</v>
@@ -49820,14 +49820,14 @@
         <v>42736</v>
       </c>
       <c r="B50" s="50"/>
-      <c r="C50" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="D50" s="36" t="s">
+      <c r="C50" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="51" t="s">
         <v>665</v>
       </c>
-      <c r="E50" s="86" t="s">
-        <v>586</v>
+      <c r="E50" s="50" t="s">
+        <v>602</v>
       </c>
       <c r="F50" s="74" t="s">
         <v>585</v>
@@ -49842,13 +49842,13 @@
         <v>73</v>
       </c>
       <c r="D51" s="51" t="s">
-        <v>665</v>
+        <v>671</v>
       </c>
       <c r="E51" s="50" t="s">
         <v>602</v>
       </c>
       <c r="F51" s="74" t="s">
-        <v>585</v>
+        <v>599</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="20" customHeight="1">
@@ -49860,13 +49860,13 @@
         <v>73</v>
       </c>
       <c r="D52" s="51" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="E52" s="50" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="F52" s="74" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="20" customHeight="1">
@@ -49878,13 +49878,13 @@
         <v>73</v>
       </c>
       <c r="D53" s="51" t="s">
-        <v>665</v>
+        <v>671</v>
       </c>
       <c r="E53" s="50" t="s">
         <v>600</v>
       </c>
       <c r="F53" s="74" t="s">
-        <v>585</v>
+        <v>599</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="20" customHeight="1">
@@ -49895,14 +49895,14 @@
       <c r="C54" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="D54" s="51" t="s">
-        <v>671</v>
+      <c r="D54" s="36" t="s">
+        <v>672</v>
       </c>
       <c r="E54" s="50" t="s">
         <v>600</v>
       </c>
       <c r="F54" s="74" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="20" customHeight="1">
@@ -49917,7 +49917,7 @@
         <v>672</v>
       </c>
       <c r="E55" s="50" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="F55" s="74" t="s">
         <v>587</v>
@@ -49929,16 +49929,16 @@
       </c>
       <c r="B56" s="50"/>
       <c r="C56" s="36" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D56" s="36" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="E56" s="50" t="s">
-        <v>602</v>
+        <v>586</v>
       </c>
       <c r="F56" s="74" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="20" customHeight="1">
@@ -49950,7 +49950,7 @@
         <v>88</v>
       </c>
       <c r="D57" s="36" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="E57" s="50" t="s">
         <v>586</v>
@@ -49968,7 +49968,7 @@
         <v>88</v>
       </c>
       <c r="D58" s="36" t="s">
-        <v>666</v>
+        <v>1014</v>
       </c>
       <c r="E58" s="50" t="s">
         <v>586</v>
@@ -49982,13 +49982,13 @@
         <v>42736</v>
       </c>
       <c r="B59" s="50"/>
-      <c r="C59" s="36" t="s">
-        <v>88</v>
+      <c r="C59" s="38" t="s">
+        <v>76</v>
       </c>
       <c r="D59" s="36" t="s">
-        <v>1014</v>
-      </c>
-      <c r="E59" s="50" t="s">
+        <v>665</v>
+      </c>
+      <c r="E59" s="86" t="s">
         <v>586</v>
       </c>
       <c r="F59" s="74" t="s">
@@ -50004,7 +50004,7 @@
         <v>76</v>
       </c>
       <c r="D60" s="36" t="s">
-        <v>665</v>
+        <v>992</v>
       </c>
       <c r="E60" s="86" t="s">
         <v>586</v>
@@ -50014,20 +50014,20 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="20" customHeight="1">
-      <c r="A61" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B61" s="50"/>
-      <c r="C61" s="38" t="s">
+      <c r="A61" s="41">
+        <v>42736</v>
+      </c>
+      <c r="B61" s="55"/>
+      <c r="C61" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D61" s="36" t="s">
-        <v>992</v>
-      </c>
-      <c r="E61" s="86" t="s">
+      <c r="D61" s="53" t="s">
+        <v>995</v>
+      </c>
+      <c r="E61" s="127" t="s">
         <v>586</v>
       </c>
-      <c r="F61" s="74" t="s">
+      <c r="F61" s="79" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50035,12 +50035,12 @@
       <c r="A62" s="41">
         <v>42736</v>
       </c>
-      <c r="B62" s="55"/>
-      <c r="C62" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="D62" s="53" t="s">
-        <v>995</v>
+      <c r="B62" s="39"/>
+      <c r="C62" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="51" t="s">
+        <v>999</v>
       </c>
       <c r="E62" s="127" t="s">
         <v>586</v>
@@ -50058,7 +50058,7 @@
         <v>79</v>
       </c>
       <c r="D63" s="51" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E63" s="127" t="s">
         <v>586</v>
@@ -50076,7 +50076,7 @@
         <v>79</v>
       </c>
       <c r="D64" s="51" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="E64" s="127" t="s">
         <v>586</v>
@@ -50089,12 +50089,12 @@
       <c r="A65" s="41">
         <v>42736</v>
       </c>
-      <c r="B65" s="39"/>
+      <c r="B65" s="42"/>
       <c r="C65" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="D65" s="51" t="s">
-        <v>1004</v>
+      <c r="D65" s="54" t="s">
+        <v>1006</v>
       </c>
       <c r="E65" s="127" t="s">
         <v>586</v>
@@ -50107,51 +50107,51 @@
       <c r="A66" s="41">
         <v>42736</v>
       </c>
-      <c r="B66" s="42"/>
-      <c r="C66" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D66" s="54" t="s">
-        <v>1006</v>
-      </c>
-      <c r="E66" s="127" t="s">
-        <v>586</v>
+      <c r="B66" s="55"/>
+      <c r="C66" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" s="53" t="s">
+        <v>665</v>
+      </c>
+      <c r="E66" s="246" t="s">
+        <v>1229</v>
       </c>
       <c r="F66" s="79" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="20" customHeight="1">
-      <c r="A67" s="41">
-        <v>42736</v>
-      </c>
-      <c r="B67" s="55"/>
-      <c r="C67" s="43" t="s">
+      <c r="A67" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B67" s="50"/>
+      <c r="C67" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D67" s="53" t="s">
-        <v>665</v>
+      <c r="D67" s="38" t="s">
+        <v>666</v>
       </c>
       <c r="E67" s="246" t="s">
         <v>1229</v>
       </c>
-      <c r="F67" s="79" t="s">
+      <c r="F67" s="74" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="20" customHeight="1">
+    <row r="68" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
       <c r="A68" s="34">
         <v>42736</v>
       </c>
-      <c r="B68" s="50"/>
-      <c r="C68" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D68" s="38" t="s">
-        <v>666</v>
-      </c>
-      <c r="E68" s="246" t="s">
-        <v>1229</v>
+      <c r="B68" s="39"/>
+      <c r="C68" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" s="36" t="s">
+        <v>665</v>
+      </c>
+      <c r="E68" s="387" t="s">
+        <v>1228</v>
       </c>
       <c r="F68" s="74" t="s">
         <v>585</v>
@@ -50166,10 +50166,10 @@
         <v>91</v>
       </c>
       <c r="D69" s="36" t="s">
-        <v>665</v>
+        <v>692</v>
       </c>
       <c r="E69" s="387" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="F69" s="74" t="s">
         <v>585</v>
@@ -50184,10 +50184,10 @@
         <v>91</v>
       </c>
       <c r="D70" s="36" t="s">
-        <v>692</v>
+        <v>665</v>
       </c>
       <c r="E70" s="387" t="s">
-        <v>1227</v>
+        <v>586</v>
       </c>
       <c r="F70" s="74" t="s">
         <v>585</v>
@@ -50202,7 +50202,7 @@
         <v>91</v>
       </c>
       <c r="D71" s="36" t="s">
-        <v>665</v>
+        <v>692</v>
       </c>
       <c r="E71" s="387" t="s">
         <v>586</v>
@@ -50220,10 +50220,10 @@
         <v>91</v>
       </c>
       <c r="D72" s="36" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="E72" s="387" t="s">
-        <v>586</v>
+        <v>1230</v>
       </c>
       <c r="F72" s="74" t="s">
         <v>585</v>
@@ -50241,13 +50241,13 @@
         <v>693</v>
       </c>
       <c r="E73" s="387" t="s">
-        <v>1230</v>
+        <v>586</v>
       </c>
       <c r="F73" s="74" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
+    <row r="74" spans="1:6" ht="13.25" customHeight="1">
       <c r="A74" s="34">
         <v>42736</v>
       </c>
@@ -50255,8 +50255,8 @@
       <c r="C74" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D74" s="36" t="s">
-        <v>693</v>
+      <c r="D74" s="404" t="s">
+        <v>689</v>
       </c>
       <c r="E74" s="387" t="s">
         <v>586</v>
@@ -50265,19 +50265,19 @@
         <v>585</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="13.25" customHeight="1">
+    <row r="75" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
       <c r="A75" s="34">
         <v>42736</v>
       </c>
       <c r="B75" s="39"/>
       <c r="C75" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D75" s="404" t="s">
-        <v>689</v>
+        <v>94</v>
+      </c>
+      <c r="D75" s="36" t="s">
+        <v>665</v>
       </c>
       <c r="E75" s="387" t="s">
-        <v>586</v>
+        <v>1228</v>
       </c>
       <c r="F75" s="74" t="s">
         <v>585</v>
@@ -50292,10 +50292,10 @@
         <v>94</v>
       </c>
       <c r="D76" s="36" t="s">
-        <v>665</v>
+        <v>694</v>
       </c>
       <c r="E76" s="387" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="F76" s="74" t="s">
         <v>585</v>
@@ -50310,10 +50310,10 @@
         <v>94</v>
       </c>
       <c r="D77" s="36" t="s">
-        <v>694</v>
+        <v>665</v>
       </c>
       <c r="E77" s="387" t="s">
-        <v>1227</v>
+        <v>586</v>
       </c>
       <c r="F77" s="74" t="s">
         <v>585</v>
@@ -50328,7 +50328,7 @@
         <v>94</v>
       </c>
       <c r="D78" s="36" t="s">
-        <v>665</v>
+        <v>694</v>
       </c>
       <c r="E78" s="387" t="s">
         <v>586</v>
@@ -50346,10 +50346,10 @@
         <v>94</v>
       </c>
       <c r="D79" s="36" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E79" s="387" t="s">
-        <v>586</v>
+        <v>1230</v>
       </c>
       <c r="F79" s="74" t="s">
         <v>585</v>
@@ -50359,17 +50359,17 @@
       <c r="A80" s="34">
         <v>42736</v>
       </c>
-      <c r="B80" s="39"/>
-      <c r="C80" s="38" t="s">
+      <c r="B80" s="42"/>
+      <c r="C80" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="D80" s="36" t="s">
+      <c r="D80" s="53" t="s">
         <v>693</v>
       </c>
-      <c r="E80" s="387" t="s">
-        <v>1230</v>
-      </c>
-      <c r="F80" s="74" t="s">
+      <c r="E80" s="246" t="s">
+        <v>586</v>
+      </c>
+      <c r="F80" s="79" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50377,17 +50377,17 @@
       <c r="A81" s="34">
         <v>42736</v>
       </c>
-      <c r="B81" s="42"/>
-      <c r="C81" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="D81" s="53" t="s">
-        <v>693</v>
-      </c>
-      <c r="E81" s="246" t="s">
+      <c r="B81" s="39"/>
+      <c r="C81" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D81" s="36" t="s">
+        <v>665</v>
+      </c>
+      <c r="E81" s="387" t="s">
         <v>586</v>
       </c>
-      <c r="F81" s="79" t="s">
+      <c r="F81" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50397,15 +50397,15 @@
       </c>
       <c r="B82" s="39"/>
       <c r="C82" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="D82" s="36" t="s">
-        <v>665</v>
-      </c>
-      <c r="E82" s="387" t="s">
+        <v>100</v>
+      </c>
+      <c r="D82" s="38" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E82" s="246" t="s">
         <v>586</v>
       </c>
-      <c r="F82" s="74" t="s">
+      <c r="F82" s="79" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50414,16 +50414,16 @@
         <v>42736</v>
       </c>
       <c r="B83" s="39"/>
-      <c r="C83" s="38" t="s">
+      <c r="C83" s="428" t="s">
         <v>100</v>
       </c>
-      <c r="D83" s="38" t="s">
-        <v>1018</v>
-      </c>
-      <c r="E83" s="246" t="s">
+      <c r="D83" s="428" t="s">
+        <v>673</v>
+      </c>
+      <c r="E83" s="387" t="s">
         <v>586</v>
       </c>
-      <c r="F83" s="79" t="s">
+      <c r="F83" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50432,34 +50432,34 @@
         <v>42736</v>
       </c>
       <c r="B84" s="39"/>
-      <c r="C84" s="428" t="s">
+      <c r="C84" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="D84" s="428" t="s">
-        <v>673</v>
-      </c>
-      <c r="E84" s="387" t="s">
+      <c r="D84" s="38" t="s">
+        <v>674</v>
+      </c>
+      <c r="E84" s="246" t="s">
         <v>586</v>
       </c>
-      <c r="F84" s="74" t="s">
+      <c r="F84" s="79" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
-      <c r="A85" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B85" s="39"/>
-      <c r="C85" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="D85" s="38" t="s">
-        <v>674</v>
-      </c>
-      <c r="E85" s="246" t="s">
+    <row r="85" spans="1:6" ht="20" customHeight="1">
+      <c r="A85" s="440">
+        <v>42736</v>
+      </c>
+      <c r="B85" s="434"/>
+      <c r="C85" s="472" t="s">
+        <v>103</v>
+      </c>
+      <c r="D85" s="433" t="s">
+        <v>665</v>
+      </c>
+      <c r="E85" s="434" t="s">
         <v>586</v>
       </c>
-      <c r="F85" s="79" t="s">
+      <c r="F85" s="471" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50472,7 +50472,7 @@
         <v>103</v>
       </c>
       <c r="D86" s="433" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="E86" s="434" t="s">
         <v>586</v>
@@ -50482,20 +50482,20 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="20" customHeight="1">
-      <c r="A87" s="440">
-        <v>42736</v>
-      </c>
-      <c r="B87" s="434"/>
-      <c r="C87" s="472" t="s">
-        <v>103</v>
-      </c>
-      <c r="D87" s="433" t="s">
-        <v>666</v>
-      </c>
-      <c r="E87" s="434" t="s">
+      <c r="A87" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B87" s="50"/>
+      <c r="C87" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D87" s="36" t="s">
+        <v>665</v>
+      </c>
+      <c r="E87" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F87" s="471" t="s">
+      <c r="F87" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50507,14 +50507,14 @@
       <c r="C88" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D88" s="36" t="s">
-        <v>665</v>
+      <c r="D88" s="38" t="s">
+        <v>1036</v>
       </c>
       <c r="E88" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F88" s="74" t="s">
-        <v>585</v>
+      <c r="F88" s="188" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="20" customHeight="1">
@@ -50526,13 +50526,13 @@
         <v>106</v>
       </c>
       <c r="D89" s="38" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="E89" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F89" s="188" t="s">
-        <v>587</v>
+      <c r="F89" s="74" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="20" customHeight="1">
@@ -50544,7 +50544,7 @@
         <v>106</v>
       </c>
       <c r="D90" s="38" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="E90" s="86" t="s">
         <v>586</v>
@@ -50562,7 +50562,7 @@
         <v>106</v>
       </c>
       <c r="D91" s="38" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
       <c r="E91" s="86" t="s">
         <v>586</v>
@@ -50579,14 +50579,14 @@
       <c r="C92" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D92" s="38" t="s">
-        <v>1044</v>
+      <c r="D92" s="1" t="s">
+        <v>1042</v>
       </c>
       <c r="E92" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F92" s="74" t="s">
-        <v>585</v>
+      <c r="F92" s="188" t="s">
+        <v>1231</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="20" customHeight="1">
@@ -50597,8 +50597,8 @@
       <c r="C93" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>1042</v>
+      <c r="D93" s="38" t="s">
+        <v>1047</v>
       </c>
       <c r="E93" s="86" t="s">
         <v>586</v>
@@ -50616,13 +50616,13 @@
         <v>106</v>
       </c>
       <c r="D94" s="38" t="s">
-        <v>1047</v>
+        <v>1052</v>
       </c>
       <c r="E94" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F94" s="188" t="s">
-        <v>1231</v>
+      <c r="F94" s="74" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="20" customHeight="1">
@@ -50633,31 +50633,31 @@
       <c r="C95" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D95" s="38" t="s">
-        <v>1052</v>
+      <c r="D95" s="1" t="s">
+        <v>1050</v>
       </c>
       <c r="E95" s="86" t="s">
         <v>586</v>
       </c>
-      <c r="F95" s="74" t="s">
+      <c r="F95" s="188" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="20" customHeight="1">
-      <c r="A96" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B96" s="50"/>
-      <c r="C96" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>1050</v>
-      </c>
-      <c r="E96" s="86" t="s">
+    <row r="96" spans="1:6" customFormat="1" ht="20" customHeight="1">
+      <c r="A96" s="485">
+        <v>42736</v>
+      </c>
+      <c r="B96" s="530"/>
+      <c r="C96" s="483" t="s">
+        <v>109</v>
+      </c>
+      <c r="D96" s="483" t="s">
+        <v>665</v>
+      </c>
+      <c r="E96" s="517" t="s">
         <v>586</v>
       </c>
-      <c r="F96" s="188" t="s">
+      <c r="F96" s="531" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50673,27 +50673,27 @@
         <v>665</v>
       </c>
       <c r="E97" s="517" t="s">
-        <v>586</v>
+        <v>1227</v>
       </c>
       <c r="F97" s="531" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="98" spans="1:6" customFormat="1" ht="20" customHeight="1">
-      <c r="A98" s="485">
-        <v>42736</v>
-      </c>
-      <c r="B98" s="530"/>
-      <c r="C98" s="483" t="s">
-        <v>109</v>
-      </c>
-      <c r="D98" s="483" t="s">
+    <row r="98" spans="1:6" ht="20" customHeight="1">
+      <c r="A98" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B98" s="50"/>
+      <c r="C98" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D98" s="36" t="s">
         <v>665</v>
       </c>
-      <c r="E98" s="517" t="s">
-        <v>1227</v>
-      </c>
-      <c r="F98" s="531" t="s">
+      <c r="E98" s="86" t="s">
+        <v>586</v>
+      </c>
+      <c r="F98" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50705,8 +50705,8 @@
       <c r="C99" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D99" s="36" t="s">
-        <v>665</v>
+      <c r="D99" s="38" t="s">
+        <v>1036</v>
       </c>
       <c r="E99" s="86" t="s">
         <v>586</v>
@@ -50715,21 +50715,21 @@
         <v>585</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="20" customHeight="1">
-      <c r="A100" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B100" s="50"/>
-      <c r="C100" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D100" s="38" t="s">
-        <v>1036</v>
-      </c>
-      <c r="E100" s="86" t="s">
+    <row r="100" spans="1:6" customFormat="1" ht="20" customHeight="1">
+      <c r="A100" s="485">
+        <v>42736</v>
+      </c>
+      <c r="B100" s="530"/>
+      <c r="C100" s="483" t="s">
+        <v>115</v>
+      </c>
+      <c r="D100" s="483" t="s">
+        <v>665</v>
+      </c>
+      <c r="E100" s="517" t="s">
         <v>586</v>
       </c>
-      <c r="F100" s="74" t="s">
+      <c r="F100" s="531" t="s">
         <v>585</v>
       </c>
     </row>
@@ -50739,7 +50739,7 @@
       </c>
       <c r="B101" s="530"/>
       <c r="C101" s="483" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D101" s="483" t="s">
         <v>665</v>
@@ -50748,24 +50748,6 @@
         <v>586</v>
       </c>
       <c r="F101" s="531" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" customFormat="1" ht="20" customHeight="1">
-      <c r="A102" s="485">
-        <v>42736</v>
-      </c>
-      <c r="B102" s="530"/>
-      <c r="C102" s="483" t="s">
-        <v>118</v>
-      </c>
-      <c r="D102" s="483" t="s">
-        <v>665</v>
-      </c>
-      <c r="E102" s="517" t="s">
-        <v>586</v>
-      </c>
-      <c r="F102" s="531" t="s">
         <v>587</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RDM-12851 - add CaseLinkCollection for citizen
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DC6FBD-6704-5049-ABB7-F4A5C7BCF3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58173BA8-4BB5-F44F-9715-FD2DA4DE9A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="580" windowWidth="33600" windowHeight="20480" firstSheet="13" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10188" uniqueCount="1296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10192" uniqueCount="1296">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -15215,7 +15215,7 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F256" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F257" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="46"/>
     <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="45"/>
@@ -43895,10 +43895,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F274"/>
+  <dimension ref="A1:F275"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -44458,15 +44458,15 @@
       <c r="A31" s="34">
         <v>42736</v>
       </c>
-      <c r="B31" s="50"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="38" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>586</v>
+        <v>1238</v>
       </c>
       <c r="F31" s="74" t="s">
         <v>585</v>
@@ -44484,7 +44484,7 @@
         <v>232</v>
       </c>
       <c r="E32" s="50" t="s">
-        <v>1238</v>
+        <v>586</v>
       </c>
       <c r="F32" s="74" t="s">
         <v>585</v>
@@ -44495,14 +44495,14 @@
         <v>42736</v>
       </c>
       <c r="B33" s="50"/>
-      <c r="C33" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="36" t="s">
-        <v>234</v>
+      <c r="C33" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>232</v>
       </c>
       <c r="E33" s="50" t="s">
-        <v>586</v>
+        <v>1238</v>
       </c>
       <c r="F33" s="74" t="s">
         <v>585</v>
@@ -44512,12 +44512,12 @@
       <c r="A34" s="34">
         <v>42736</v>
       </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="38" t="s">
+      <c r="B34" s="50"/>
+      <c r="C34" s="36" t="s">
         <v>46</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E34" s="50" t="s">
         <v>586</v>
@@ -44531,11 +44531,11 @@
         <v>42736</v>
       </c>
       <c r="B35" s="35"/>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="38" t="s">
         <v>46</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E35" s="50" t="s">
         <v>586</v>
@@ -44552,8 +44552,8 @@
       <c r="C36" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="38" t="s">
-        <v>240</v>
+      <c r="D36" s="36" t="s">
+        <v>238</v>
       </c>
       <c r="E36" s="50" t="s">
         <v>586</v>
@@ -44566,12 +44566,12 @@
       <c r="A37" s="34">
         <v>42736</v>
       </c>
-      <c r="B37" s="50"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="36" t="s">
-        <v>217</v>
+      <c r="D37" s="38" t="s">
+        <v>240</v>
       </c>
       <c r="E37" s="50" t="s">
         <v>586</v>
@@ -44584,12 +44584,12 @@
       <c r="A38" s="34">
         <v>42736</v>
       </c>
-      <c r="B38" s="35"/>
+      <c r="B38" s="50"/>
       <c r="C38" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="38" t="s">
-        <v>222</v>
+      <c r="D38" s="36" t="s">
+        <v>217</v>
       </c>
       <c r="E38" s="50" t="s">
         <v>586</v>
@@ -44603,11 +44603,11 @@
         <v>42736</v>
       </c>
       <c r="B39" s="35"/>
-      <c r="C39" s="128" t="s">
-        <v>49</v>
+      <c r="C39" s="36" t="s">
+        <v>46</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="E39" s="50" t="s">
         <v>586</v>
@@ -44625,7 +44625,7 @@
         <v>49</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E40" s="50" t="s">
         <v>586</v>
@@ -44643,7 +44643,7 @@
         <v>49</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E41" s="50" t="s">
         <v>586</v>
@@ -44656,12 +44656,12 @@
       <c r="A42" s="34">
         <v>42736</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="35"/>
       <c r="C42" s="128" t="s">
         <v>49</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="E42" s="50" t="s">
         <v>586</v>
@@ -44678,8 +44678,8 @@
       <c r="C43" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="86" t="s">
-        <v>251</v>
+      <c r="D43" s="38" t="s">
+        <v>253</v>
       </c>
       <c r="E43" s="50" t="s">
         <v>586</v>
@@ -44692,12 +44692,12 @@
       <c r="A44" s="34">
         <v>42736</v>
       </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="121" t="s">
+      <c r="B44" s="50"/>
+      <c r="C44" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="36" t="s">
-        <v>217</v>
+      <c r="D44" s="86" t="s">
+        <v>251</v>
       </c>
       <c r="E44" s="50" t="s">
         <v>586</v>
@@ -44710,12 +44710,12 @@
       <c r="A45" s="34">
         <v>42736</v>
       </c>
-      <c r="B45" s="50"/>
+      <c r="B45" s="39"/>
       <c r="C45" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="51" t="s">
-        <v>256</v>
+      <c r="D45" s="36" t="s">
+        <v>217</v>
       </c>
       <c r="E45" s="50" t="s">
         <v>586</v>
@@ -44732,8 +44732,8 @@
       <c r="C46" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="38" t="s">
-        <v>259</v>
+      <c r="D46" s="51" t="s">
+        <v>256</v>
       </c>
       <c r="E46" s="50" t="s">
         <v>586</v>
@@ -44751,7 +44751,7 @@
         <v>49</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E47" s="50" t="s">
         <v>586</v>
@@ -44769,7 +44769,7 @@
         <v>49</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E48" s="50" t="s">
         <v>586</v>
@@ -44784,10 +44784,10 @@
       </c>
       <c r="B49" s="50"/>
       <c r="C49" s="121" t="s">
-        <v>82</v>
-      </c>
-      <c r="D49" s="36" t="s">
-        <v>266</v>
+        <v>49</v>
+      </c>
+      <c r="D49" s="38" t="s">
+        <v>264</v>
       </c>
       <c r="E49" s="50" t="s">
         <v>586</v>
@@ -44804,8 +44804,8 @@
       <c r="C50" s="121" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="38" t="s">
-        <v>269</v>
+      <c r="D50" s="36" t="s">
+        <v>266</v>
       </c>
       <c r="E50" s="50" t="s">
         <v>586</v>
@@ -44823,7 +44823,7 @@
         <v>82</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E51" s="50" t="s">
         <v>586</v>
@@ -44836,12 +44836,12 @@
       <c r="A52" s="34">
         <v>42736</v>
       </c>
-      <c r="B52" s="35"/>
-      <c r="C52" s="248" t="s">
-        <v>85</v>
-      </c>
-      <c r="D52" s="235" t="s">
-        <v>273</v>
+      <c r="B52" s="50"/>
+      <c r="C52" s="121" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="38" t="s">
+        <v>270</v>
       </c>
       <c r="E52" s="50" t="s">
         <v>586</v>
@@ -44858,8 +44858,8 @@
       <c r="C53" s="248" t="s">
         <v>85</v>
       </c>
-      <c r="D53" s="234" t="s">
-        <v>275</v>
+      <c r="D53" s="235" t="s">
+        <v>273</v>
       </c>
       <c r="E53" s="50" t="s">
         <v>586</v>
@@ -44877,7 +44877,7 @@
         <v>85</v>
       </c>
       <c r="D54" s="234" t="s">
-        <v>12</v>
+        <v>275</v>
       </c>
       <c r="E54" s="50" t="s">
         <v>586</v>
@@ -44895,7 +44895,7 @@
         <v>85</v>
       </c>
       <c r="D55" s="234" t="s">
-        <v>277</v>
+        <v>12</v>
       </c>
       <c r="E55" s="50" t="s">
         <v>586</v>
@@ -44908,12 +44908,12 @@
       <c r="A56" s="34">
         <v>42736</v>
       </c>
-      <c r="B56" s="50"/>
-      <c r="C56" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="D56" s="38" t="s">
-        <v>280</v>
+      <c r="B56" s="35"/>
+      <c r="C56" s="248" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" s="234" t="s">
+        <v>277</v>
       </c>
       <c r="E56" s="50" t="s">
         <v>586</v>
@@ -44926,12 +44926,12 @@
       <c r="A57" s="34">
         <v>42736</v>
       </c>
-      <c r="B57" s="35"/>
+      <c r="B57" s="50"/>
       <c r="C57" s="38" t="s">
         <v>52</v>
       </c>
       <c r="D57" s="38" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E57" s="50" t="s">
         <v>586</v>
@@ -44949,7 +44949,7 @@
         <v>52</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E58" s="50" t="s">
         <v>586</v>
@@ -44967,7 +44967,7 @@
         <v>52</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E59" s="50" t="s">
         <v>586</v>
@@ -44985,7 +44985,7 @@
         <v>52</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E60" s="50" t="s">
         <v>586</v>
@@ -45003,7 +45003,7 @@
         <v>52</v>
       </c>
       <c r="D61" s="38" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E61" s="50" t="s">
         <v>586</v>
@@ -45021,7 +45021,7 @@
         <v>52</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E62" s="50" t="s">
         <v>586</v>
@@ -45039,7 +45039,7 @@
         <v>52</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E63" s="50" t="s">
         <v>586</v>
@@ -45057,7 +45057,7 @@
         <v>52</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E64" s="50" t="s">
         <v>586</v>
@@ -45075,7 +45075,7 @@
         <v>52</v>
       </c>
       <c r="D65" s="38" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E65" s="50" t="s">
         <v>586</v>
@@ -45092,8 +45092,8 @@
       <c r="C66" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D66" s="36" t="s">
-        <v>217</v>
+      <c r="D66" s="38" t="s">
+        <v>300</v>
       </c>
       <c r="E66" s="50" t="s">
         <v>586</v>
@@ -45108,10 +45108,10 @@
       </c>
       <c r="B67" s="35"/>
       <c r="C67" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D67" s="38" t="s">
-        <v>280</v>
+        <v>52</v>
+      </c>
+      <c r="D67" s="36" t="s">
+        <v>217</v>
       </c>
       <c r="E67" s="50" t="s">
         <v>586</v>
@@ -45129,7 +45129,7 @@
         <v>55</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E68" s="50" t="s">
         <v>586</v>
@@ -45147,7 +45147,7 @@
         <v>55</v>
       </c>
       <c r="D69" s="38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E69" s="50" t="s">
         <v>586</v>
@@ -45165,7 +45165,7 @@
         <v>55</v>
       </c>
       <c r="D70" s="38" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="E70" s="50" t="s">
         <v>586</v>
@@ -45182,8 +45182,8 @@
       <c r="C71" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="D71" s="36" t="s">
-        <v>217</v>
+      <c r="D71" s="38" t="s">
+        <v>302</v>
       </c>
       <c r="E71" s="50" t="s">
         <v>586</v>
@@ -45197,11 +45197,11 @@
         <v>42736</v>
       </c>
       <c r="B72" s="35"/>
-      <c r="C72" s="36" t="s">
-        <v>58</v>
+      <c r="C72" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="D72" s="36" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
       <c r="E72" s="50" t="s">
         <v>586</v>
@@ -45219,7 +45219,7 @@
         <v>58</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>217</v>
+        <v>165</v>
       </c>
       <c r="E73" s="50" t="s">
         <v>586</v>
@@ -45234,10 +45234,10 @@
       </c>
       <c r="B74" s="35"/>
       <c r="C74" s="36" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D74" s="36" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
       <c r="E74" s="50" t="s">
         <v>586</v>
@@ -45255,7 +45255,7 @@
         <v>61</v>
       </c>
       <c r="D75" s="36" t="s">
-        <v>305</v>
+        <v>165</v>
       </c>
       <c r="E75" s="50" t="s">
         <v>586</v>
@@ -45272,8 +45272,8 @@
       <c r="C76" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D76" s="38" t="s">
-        <v>282</v>
+      <c r="D76" s="36" t="s">
+        <v>305</v>
       </c>
       <c r="E76" s="50" t="s">
         <v>586</v>
@@ -45291,7 +45291,7 @@
         <v>61</v>
       </c>
       <c r="D77" s="38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E77" s="50" t="s">
         <v>586</v>
@@ -45308,8 +45308,8 @@
       <c r="C78" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D78" s="36" t="s">
-        <v>192</v>
+      <c r="D78" s="38" t="s">
+        <v>284</v>
       </c>
       <c r="E78" s="50" t="s">
         <v>586</v>
@@ -45327,7 +45327,7 @@
         <v>61</v>
       </c>
       <c r="D79" s="36" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="E79" s="50" t="s">
         <v>586</v>
@@ -45345,7 +45345,7 @@
         <v>61</v>
       </c>
       <c r="D80" s="36" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E80" s="50" t="s">
         <v>586</v>
@@ -45363,7 +45363,7 @@
         <v>61</v>
       </c>
       <c r="D81" s="36" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="E81" s="50" t="s">
         <v>586</v>
@@ -45381,7 +45381,7 @@
         <v>61</v>
       </c>
       <c r="D82" s="36" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E82" s="50" t="s">
         <v>586</v>
@@ -45399,7 +45399,7 @@
         <v>61</v>
       </c>
       <c r="D83" s="36" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E83" s="50" t="s">
         <v>586</v>
@@ -45417,7 +45417,7 @@
         <v>61</v>
       </c>
       <c r="D84" s="36" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E84" s="50" t="s">
         <v>586</v>
@@ -45434,8 +45434,8 @@
       <c r="C85" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D85" s="38" t="s">
-        <v>334</v>
+      <c r="D85" s="36" t="s">
+        <v>217</v>
       </c>
       <c r="E85" s="50" t="s">
         <v>586</v>
@@ -45453,7 +45453,7 @@
         <v>61</v>
       </c>
       <c r="D86" s="38" t="s">
-        <v>184</v>
+        <v>334</v>
       </c>
       <c r="E86" s="50" t="s">
         <v>586</v>
@@ -45471,7 +45471,7 @@
         <v>61</v>
       </c>
       <c r="D87" s="38" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="E87" s="50" t="s">
         <v>586</v>
@@ -45489,7 +45489,7 @@
         <v>61</v>
       </c>
       <c r="D88" s="38" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E88" s="50" t="s">
         <v>586</v>
@@ -45507,7 +45507,7 @@
         <v>61</v>
       </c>
       <c r="D89" s="38" t="s">
-        <v>307</v>
+        <v>169</v>
       </c>
       <c r="E89" s="50" t="s">
         <v>586</v>
@@ -45525,7 +45525,7 @@
         <v>61</v>
       </c>
       <c r="D90" s="38" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E90" s="50" t="s">
         <v>586</v>
@@ -45543,7 +45543,7 @@
         <v>61</v>
       </c>
       <c r="D91" s="38" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E91" s="50" t="s">
         <v>586</v>
@@ -45561,7 +45561,7 @@
         <v>61</v>
       </c>
       <c r="D92" s="38" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E92" s="50" t="s">
         <v>586</v>
@@ -45579,7 +45579,7 @@
         <v>61</v>
       </c>
       <c r="D93" s="38" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E93" s="50" t="s">
         <v>586</v>
@@ -45597,7 +45597,7 @@
         <v>61</v>
       </c>
       <c r="D94" s="38" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E94" s="50" t="s">
         <v>586</v>
@@ -45615,7 +45615,7 @@
         <v>61</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E95" s="50" t="s">
         <v>586</v>
@@ -45633,7 +45633,7 @@
         <v>61</v>
       </c>
       <c r="D96" s="38" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E96" s="50" t="s">
         <v>586</v>
@@ -45651,7 +45651,7 @@
         <v>61</v>
       </c>
       <c r="D97" s="38" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E97" s="50" t="s">
         <v>586</v>
@@ -45669,7 +45669,7 @@
         <v>61</v>
       </c>
       <c r="D98" s="38" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E98" s="50" t="s">
         <v>586</v>
@@ -45687,7 +45687,7 @@
         <v>61</v>
       </c>
       <c r="D99" s="38" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E99" s="50" t="s">
         <v>586</v>
@@ -45705,7 +45705,7 @@
         <v>61</v>
       </c>
       <c r="D100" s="38" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E100" s="50" t="s">
         <v>586</v>
@@ -45723,7 +45723,7 @@
         <v>61</v>
       </c>
       <c r="D101" s="38" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="E101" s="50" t="s">
         <v>586</v>
@@ -45741,7 +45741,7 @@
         <v>61</v>
       </c>
       <c r="D102" s="38" t="s">
-        <v>259</v>
+        <v>339</v>
       </c>
       <c r="E102" s="50" t="s">
         <v>586</v>
@@ -45758,8 +45758,8 @@
       <c r="C103" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D103" s="36" t="s">
-        <v>286</v>
+      <c r="D103" s="38" t="s">
+        <v>259</v>
       </c>
       <c r="E103" s="50" t="s">
         <v>586</v>
@@ -45777,7 +45777,7 @@
         <v>61</v>
       </c>
       <c r="D104" s="36" t="s">
-        <v>343</v>
+        <v>286</v>
       </c>
       <c r="E104" s="50" t="s">
         <v>586</v>
@@ -45795,7 +45795,7 @@
         <v>61</v>
       </c>
       <c r="D105" s="36" t="s">
-        <v>290</v>
+        <v>343</v>
       </c>
       <c r="E105" s="50" t="s">
         <v>586</v>
@@ -45813,7 +45813,7 @@
         <v>61</v>
       </c>
       <c r="D106" s="36" t="s">
-        <v>345</v>
+        <v>290</v>
       </c>
       <c r="E106" s="50" t="s">
         <v>586</v>
@@ -45830,8 +45830,8 @@
       <c r="C107" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D107" s="38" t="s">
-        <v>292</v>
+      <c r="D107" s="36" t="s">
+        <v>345</v>
       </c>
       <c r="E107" s="50" t="s">
         <v>586</v>
@@ -45849,7 +45849,7 @@
         <v>61</v>
       </c>
       <c r="D108" s="38" t="s">
-        <v>347</v>
+        <v>292</v>
       </c>
       <c r="E108" s="50" t="s">
         <v>586</v>
@@ -45867,7 +45867,7 @@
         <v>61</v>
       </c>
       <c r="D109" s="38" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E109" s="50" t="s">
         <v>586</v>
@@ -45885,7 +45885,7 @@
         <v>61</v>
       </c>
       <c r="D110" s="38" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E110" s="50" t="s">
         <v>586</v>
@@ -45903,7 +45903,7 @@
         <v>61</v>
       </c>
       <c r="D111" s="38" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E111" s="50" t="s">
         <v>586</v>
@@ -45921,7 +45921,7 @@
         <v>61</v>
       </c>
       <c r="D112" s="38" t="s">
-        <v>331</v>
+        <v>353</v>
       </c>
       <c r="E112" s="50" t="s">
         <v>586</v>
@@ -45938,8 +45938,8 @@
       <c r="C113" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D113" s="36" t="s">
-        <v>355</v>
+      <c r="D113" s="38" t="s">
+        <v>331</v>
       </c>
       <c r="E113" s="50" t="s">
         <v>586</v>
@@ -45957,7 +45957,7 @@
         <v>61</v>
       </c>
       <c r="D114" s="36" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E114" s="50" t="s">
         <v>586</v>
@@ -45971,11 +45971,11 @@
         <v>42736</v>
       </c>
       <c r="B115" s="35"/>
-      <c r="C115" s="128" t="s">
-        <v>64</v>
-      </c>
-      <c r="D115" s="38" t="s">
-        <v>247</v>
+      <c r="C115" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D115" s="36" t="s">
+        <v>357</v>
       </c>
       <c r="E115" s="50" t="s">
         <v>586</v>
@@ -45993,7 +45993,7 @@
         <v>64</v>
       </c>
       <c r="D116" s="38" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E116" s="50" t="s">
         <v>586</v>
@@ -46011,7 +46011,7 @@
         <v>64</v>
       </c>
       <c r="D117" s="38" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E117" s="50" t="s">
         <v>586</v>
@@ -46024,12 +46024,12 @@
       <c r="A118" s="34">
         <v>42736</v>
       </c>
-      <c r="B118" s="50"/>
+      <c r="B118" s="35"/>
       <c r="C118" s="128" t="s">
         <v>64</v>
       </c>
       <c r="D118" s="38" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="E118" s="50" t="s">
         <v>586</v>
@@ -46042,12 +46042,12 @@
       <c r="A119" s="34">
         <v>42736</v>
       </c>
-      <c r="B119" s="39"/>
+      <c r="B119" s="50"/>
       <c r="C119" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="D119" s="128" t="s">
-        <v>217</v>
+      <c r="D119" s="38" t="s">
+        <v>253</v>
       </c>
       <c r="E119" s="50" t="s">
         <v>586</v>
@@ -46060,12 +46060,12 @@
       <c r="A120" s="34">
         <v>42736</v>
       </c>
-      <c r="B120" s="50"/>
+      <c r="B120" s="39"/>
       <c r="C120" s="128" t="s">
         <v>64</v>
       </c>
       <c r="D120" s="128" t="s">
-        <v>256</v>
+        <v>217</v>
       </c>
       <c r="E120" s="50" t="s">
         <v>586</v>
@@ -46083,7 +46083,7 @@
         <v>64</v>
       </c>
       <c r="D121" s="128" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E121" s="50" t="s">
         <v>586</v>
@@ -46096,12 +46096,12 @@
       <c r="A122" s="34">
         <v>42736</v>
       </c>
-      <c r="B122" s="35"/>
-      <c r="C122" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D122" s="36" t="s">
-        <v>165</v>
+      <c r="B122" s="50"/>
+      <c r="C122" s="128" t="s">
+        <v>64</v>
+      </c>
+      <c r="D122" s="128" t="s">
+        <v>259</v>
       </c>
       <c r="E122" s="50" t="s">
         <v>586</v>
@@ -46115,8 +46115,8 @@
         <v>42736</v>
       </c>
       <c r="B123" s="35"/>
-      <c r="C123" s="38" t="s">
-        <v>70</v>
+      <c r="C123" s="36" t="s">
+        <v>67</v>
       </c>
       <c r="D123" s="36" t="s">
         <v>165</v>
@@ -46137,7 +46137,7 @@
         <v>70</v>
       </c>
       <c r="D124" s="36" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E124" s="50" t="s">
         <v>586</v>
@@ -46151,14 +46151,14 @@
         <v>42736</v>
       </c>
       <c r="B125" s="35"/>
-      <c r="C125" s="36" t="s">
-        <v>73</v>
+      <c r="C125" s="38" t="s">
+        <v>70</v>
       </c>
       <c r="D125" s="36" t="s">
-        <v>363</v>
+        <v>172</v>
       </c>
       <c r="E125" s="50" t="s">
-        <v>600</v>
+        <v>586</v>
       </c>
       <c r="F125" s="74" t="s">
         <v>585</v>
@@ -46176,10 +46176,10 @@
         <v>363</v>
       </c>
       <c r="E126" s="50" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="F126" s="74" t="s">
-        <v>603</v>
+        <v>585</v>
       </c>
     </row>
     <row r="127" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
@@ -46187,17 +46187,17 @@
         <v>42736</v>
       </c>
       <c r="B127" s="35"/>
-      <c r="C127" s="38" t="s">
+      <c r="C127" s="36" t="s">
         <v>73</v>
       </c>
       <c r="D127" s="36" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="E127" s="50" t="s">
         <v>602</v>
       </c>
       <c r="F127" s="74" t="s">
-        <v>585</v>
+        <v>603</v>
       </c>
     </row>
     <row r="128" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
@@ -46209,7 +46209,7 @@
         <v>73</v>
       </c>
       <c r="D128" s="36" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E128" s="50" t="s">
         <v>602</v>
@@ -46227,10 +46227,10 @@
         <v>73</v>
       </c>
       <c r="D129" s="36" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="E129" s="50" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="F129" s="74" t="s">
         <v>585</v>
@@ -46245,7 +46245,7 @@
         <v>73</v>
       </c>
       <c r="D130" s="36" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E130" s="50" t="s">
         <v>600</v>
@@ -46260,13 +46260,13 @@
       </c>
       <c r="B131" s="35"/>
       <c r="C131" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D131" s="38" t="s">
-        <v>302</v>
+        <v>73</v>
+      </c>
+      <c r="D131" s="36" t="s">
+        <v>362</v>
       </c>
       <c r="E131" s="50" t="s">
-        <v>586</v>
+        <v>600</v>
       </c>
       <c r="F131" s="74" t="s">
         <v>585</v>
@@ -46281,7 +46281,7 @@
         <v>76</v>
       </c>
       <c r="D132" s="38" t="s">
-        <v>280</v>
+        <v>302</v>
       </c>
       <c r="E132" s="50" t="s">
         <v>586</v>
@@ -46291,20 +46291,20 @@
       </c>
     </row>
     <row r="133" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
-      <c r="A133" s="41">
-        <v>42736</v>
-      </c>
-      <c r="B133" s="52"/>
-      <c r="C133" s="43" t="s">
+      <c r="A133" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B133" s="35"/>
+      <c r="C133" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D133" s="43" t="s">
-        <v>217</v>
-      </c>
-      <c r="E133" s="55" t="s">
+      <c r="D133" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="E133" s="50" t="s">
         <v>586</v>
       </c>
-      <c r="F133" s="79" t="s">
+      <c r="F133" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -46314,10 +46314,10 @@
       </c>
       <c r="B134" s="52"/>
       <c r="C134" s="43" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D134" s="43" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
       <c r="E134" s="55" t="s">
         <v>586</v>
@@ -46335,7 +46335,7 @@
         <v>88</v>
       </c>
       <c r="D135" s="43" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E135" s="55" t="s">
         <v>586</v>
@@ -46353,7 +46353,7 @@
         <v>88</v>
       </c>
       <c r="D136" s="43" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E136" s="55" t="s">
         <v>586</v>
@@ -46371,7 +46371,7 @@
         <v>88</v>
       </c>
       <c r="D137" s="43" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E137" s="55" t="s">
         <v>586</v>
@@ -46389,7 +46389,7 @@
         <v>88</v>
       </c>
       <c r="D138" s="43" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E138" s="55" t="s">
         <v>586</v>
@@ -46407,7 +46407,7 @@
         <v>88</v>
       </c>
       <c r="D139" s="43" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E139" s="55" t="s">
         <v>586</v>
@@ -46425,7 +46425,7 @@
         <v>88</v>
       </c>
       <c r="D140" s="43" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E140" s="55" t="s">
         <v>586</v>
@@ -46443,7 +46443,7 @@
         <v>88</v>
       </c>
       <c r="D141" s="43" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="E141" s="55" t="s">
         <v>586</v>
@@ -46461,7 +46461,7 @@
         <v>88</v>
       </c>
       <c r="D142" s="43" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E142" s="55" t="s">
         <v>586</v>
@@ -46479,7 +46479,7 @@
         <v>88</v>
       </c>
       <c r="D143" s="43" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E143" s="55" t="s">
         <v>586</v>
@@ -46497,7 +46497,7 @@
         <v>88</v>
       </c>
       <c r="D144" s="43" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E144" s="55" t="s">
         <v>586</v>
@@ -46510,12 +46510,12 @@
       <c r="A145" s="41">
         <v>42736</v>
       </c>
-      <c r="B145" s="35"/>
-      <c r="C145" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D145" s="38" t="s">
-        <v>366</v>
+      <c r="B145" s="52"/>
+      <c r="C145" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D145" s="43" t="s">
+        <v>213</v>
       </c>
       <c r="E145" s="55" t="s">
         <v>586</v>
@@ -46533,7 +46533,7 @@
         <v>79</v>
       </c>
       <c r="D146" s="38" t="s">
-        <v>172</v>
+        <v>366</v>
       </c>
       <c r="E146" s="55" t="s">
         <v>586</v>
@@ -46551,7 +46551,7 @@
         <v>79</v>
       </c>
       <c r="D147" s="38" t="s">
-        <v>370</v>
+        <v>172</v>
       </c>
       <c r="E147" s="55" t="s">
         <v>586</v>
@@ -46569,7 +46569,7 @@
         <v>79</v>
       </c>
       <c r="D148" s="38" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E148" s="55" t="s">
         <v>586</v>
@@ -46587,7 +46587,7 @@
         <v>79</v>
       </c>
       <c r="D149" s="38" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E149" s="55" t="s">
         <v>586</v>
@@ -46605,7 +46605,7 @@
         <v>79</v>
       </c>
       <c r="D150" s="38" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E150" s="55" t="s">
         <v>586</v>
@@ -46623,7 +46623,7 @@
         <v>79</v>
       </c>
       <c r="D151" s="38" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E151" s="55" t="s">
         <v>586</v>
@@ -46641,7 +46641,7 @@
         <v>79</v>
       </c>
       <c r="D152" s="38" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E152" s="55" t="s">
         <v>586</v>
@@ -46659,7 +46659,7 @@
         <v>79</v>
       </c>
       <c r="D153" s="38" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E153" s="55" t="s">
         <v>586</v>
@@ -46672,12 +46672,12 @@
       <c r="A154" s="41">
         <v>42736</v>
       </c>
-      <c r="B154" s="52"/>
+      <c r="B154" s="35"/>
       <c r="C154" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="D154" s="43" t="s">
-        <v>387</v>
+      <c r="D154" s="38" t="s">
+        <v>385</v>
       </c>
       <c r="E154" s="55" t="s">
         <v>586</v>
@@ -46687,20 +46687,20 @@
       </c>
     </row>
     <row r="155" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
-      <c r="A155" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B155" s="35"/>
+      <c r="A155" s="41">
+        <v>42736</v>
+      </c>
+      <c r="B155" s="52"/>
       <c r="C155" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D155" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="E155" s="50" t="s">
-        <v>1239</v>
-      </c>
-      <c r="F155" s="74" t="s">
+        <v>79</v>
+      </c>
+      <c r="D155" s="43" t="s">
+        <v>387</v>
+      </c>
+      <c r="E155" s="55" t="s">
+        <v>586</v>
+      </c>
+      <c r="F155" s="79" t="s">
         <v>585</v>
       </c>
     </row>
@@ -46713,7 +46713,7 @@
         <v>41</v>
       </c>
       <c r="D156" s="38" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E156" s="50" t="s">
         <v>1239</v>
@@ -46731,7 +46731,7 @@
         <v>41</v>
       </c>
       <c r="D157" s="38" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E157" s="50" t="s">
         <v>1239</v>
@@ -46749,7 +46749,7 @@
         <v>41</v>
       </c>
       <c r="D158" s="38" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E158" s="50" t="s">
         <v>1239</v>
@@ -46767,7 +46767,7 @@
         <v>41</v>
       </c>
       <c r="D159" s="38" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E159" s="50" t="s">
         <v>1239</v>
@@ -46785,7 +46785,7 @@
         <v>41</v>
       </c>
       <c r="D160" s="38" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E160" s="50" t="s">
         <v>1239</v>
@@ -46803,7 +46803,7 @@
         <v>41</v>
       </c>
       <c r="D161" s="38" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="E161" s="50" t="s">
         <v>1239</v>
@@ -46821,7 +46821,7 @@
         <v>41</v>
       </c>
       <c r="D162" s="38" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E162" s="50" t="s">
         <v>1239</v>
@@ -46839,7 +46839,7 @@
         <v>41</v>
       </c>
       <c r="D163" s="38" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E163" s="50" t="s">
         <v>1239</v>
@@ -46857,7 +46857,7 @@
         <v>41</v>
       </c>
       <c r="D164" s="38" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E164" s="50" t="s">
         <v>1239</v>
@@ -46875,7 +46875,7 @@
         <v>41</v>
       </c>
       <c r="D165" s="38" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E165" s="50" t="s">
         <v>1239</v>
@@ -46893,7 +46893,7 @@
         <v>41</v>
       </c>
       <c r="D166" s="38" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="E166" s="50" t="s">
         <v>1239</v>
@@ -46903,38 +46903,38 @@
       </c>
     </row>
     <row r="167" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
-      <c r="A167" s="95">
-        <v>42737</v>
-      </c>
-      <c r="B167" s="81"/>
+      <c r="A167" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B167" s="35"/>
       <c r="C167" s="38" t="s">
         <v>41</v>
       </c>
       <c r="D167" s="38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E167" s="50" t="s">
         <v>1239</v>
       </c>
-      <c r="F167" s="130" t="s">
+      <c r="F167" s="74" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="168" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
-      <c r="A168" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B168" s="35"/>
+      <c r="A168" s="95">
+        <v>42737</v>
+      </c>
+      <c r="B168" s="81"/>
       <c r="C168" s="38" t="s">
         <v>41</v>
       </c>
       <c r="D168" s="38" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="E168" s="50" t="s">
         <v>1239</v>
       </c>
-      <c r="F168" s="74" t="s">
+      <c r="F168" s="130" t="s">
         <v>585</v>
       </c>
     </row>
@@ -46947,7 +46947,7 @@
         <v>41</v>
       </c>
       <c r="D169" s="38" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E169" s="50" t="s">
         <v>1239</v>
@@ -46965,7 +46965,7 @@
         <v>41</v>
       </c>
       <c r="D170" s="38" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E170" s="50" t="s">
         <v>1239</v>
@@ -46983,7 +46983,7 @@
         <v>41</v>
       </c>
       <c r="D171" s="38" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E171" s="50" t="s">
         <v>1239</v>
@@ -47001,7 +47001,7 @@
         <v>41</v>
       </c>
       <c r="D172" s="38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E172" s="50" t="s">
         <v>1239</v>
@@ -47019,7 +47019,7 @@
         <v>41</v>
       </c>
       <c r="D173" s="38" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E173" s="50" t="s">
         <v>1239</v>
@@ -47029,20 +47029,20 @@
       </c>
     </row>
     <row r="174" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
-      <c r="A174" s="41">
-        <v>42736</v>
-      </c>
-      <c r="B174" s="52"/>
-      <c r="C174" s="43" t="s">
+      <c r="A174" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B174" s="35"/>
+      <c r="C174" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D174" s="43" t="s">
-        <v>227</v>
+      <c r="D174" s="38" t="s">
+        <v>224</v>
       </c>
       <c r="E174" s="50" t="s">
         <v>1239</v>
       </c>
-      <c r="F174" s="79" t="s">
+      <c r="F174" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -47050,17 +47050,17 @@
       <c r="A175" s="41">
         <v>42736</v>
       </c>
-      <c r="B175" s="35"/>
-      <c r="C175" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D175" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="E175" s="39" t="s">
-        <v>1238</v>
-      </c>
-      <c r="F175" s="74" t="s">
+      <c r="B175" s="52"/>
+      <c r="C175" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D175" s="43" t="s">
+        <v>227</v>
+      </c>
+      <c r="E175" s="50" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F175" s="79" t="s">
         <v>585</v>
       </c>
     </row>
@@ -47073,7 +47073,7 @@
         <v>91</v>
       </c>
       <c r="D176" s="38" t="s">
-        <v>390</v>
+        <v>217</v>
       </c>
       <c r="E176" s="39" t="s">
         <v>1238</v>
@@ -47091,7 +47091,7 @@
         <v>91</v>
       </c>
       <c r="D177" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E177" s="39" t="s">
         <v>1238</v>
@@ -47109,7 +47109,7 @@
         <v>91</v>
       </c>
       <c r="D178" s="38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E178" s="39" t="s">
         <v>1238</v>
@@ -47127,7 +47127,7 @@
         <v>91</v>
       </c>
       <c r="D179" s="38" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E179" s="39" t="s">
         <v>1238</v>
@@ -47145,7 +47145,7 @@
         <v>91</v>
       </c>
       <c r="D180" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E180" s="39" t="s">
         <v>1238</v>
@@ -47158,17 +47158,17 @@
       <c r="A181" s="41">
         <v>42736</v>
       </c>
-      <c r="B181" s="52"/>
-      <c r="C181" s="43" t="s">
+      <c r="B181" s="35"/>
+      <c r="C181" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D181" s="43" t="s">
-        <v>401</v>
-      </c>
-      <c r="E181" s="42" t="s">
+      <c r="D181" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="E181" s="39" t="s">
         <v>1238</v>
       </c>
-      <c r="F181" s="79" t="s">
+      <c r="F181" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -47180,8 +47180,8 @@
       <c r="C182" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="D182" s="38" t="s">
-        <v>403</v>
+      <c r="D182" s="43" t="s">
+        <v>401</v>
       </c>
       <c r="E182" s="42" t="s">
         <v>1238</v>
@@ -47190,21 +47190,21 @@
         <v>585</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="20" customHeight="1">
+    <row r="183" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
       <c r="A183" s="41">
         <v>42736</v>
       </c>
-      <c r="B183" s="35"/>
-      <c r="C183" s="38" t="s">
+      <c r="B183" s="52"/>
+      <c r="C183" s="43" t="s">
         <v>91</v>
       </c>
       <c r="D183" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="E183" s="39" t="s">
-        <v>1237</v>
-      </c>
-      <c r="F183" s="74" t="s">
+        <v>403</v>
+      </c>
+      <c r="E183" s="42" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F183" s="79" t="s">
         <v>585</v>
       </c>
     </row>
@@ -47217,7 +47217,7 @@
         <v>91</v>
       </c>
       <c r="D184" s="38" t="s">
-        <v>390</v>
+        <v>217</v>
       </c>
       <c r="E184" s="39" t="s">
         <v>1237</v>
@@ -47235,7 +47235,7 @@
         <v>91</v>
       </c>
       <c r="D185" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E185" s="39" t="s">
         <v>1237</v>
@@ -47253,7 +47253,7 @@
         <v>91</v>
       </c>
       <c r="D186" s="38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E186" s="39" t="s">
         <v>1237</v>
@@ -47271,7 +47271,7 @@
         <v>91</v>
       </c>
       <c r="D187" s="38" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E187" s="39" t="s">
         <v>1237</v>
@@ -47289,7 +47289,7 @@
         <v>91</v>
       </c>
       <c r="D188" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E188" s="39" t="s">
         <v>1237</v>
@@ -47307,7 +47307,7 @@
         <v>91</v>
       </c>
       <c r="D189" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E189" s="39" t="s">
         <v>1237</v>
@@ -47325,7 +47325,7 @@
         <v>91</v>
       </c>
       <c r="D190" s="38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E190" s="39" t="s">
         <v>1237</v>
@@ -47343,10 +47343,10 @@
         <v>91</v>
       </c>
       <c r="D191" s="38" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="E191" s="39" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="F191" s="74" t="s">
         <v>585</v>
@@ -47361,7 +47361,7 @@
         <v>91</v>
       </c>
       <c r="D192" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E192" s="39" t="s">
         <v>1240</v>
@@ -47379,7 +47379,7 @@
         <v>91</v>
       </c>
       <c r="D193" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E193" s="39" t="s">
         <v>1240</v>
@@ -47397,7 +47397,7 @@
         <v>91</v>
       </c>
       <c r="D194" s="38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E194" s="39" t="s">
         <v>1240</v>
@@ -47415,10 +47415,10 @@
         <v>91</v>
       </c>
       <c r="D195" s="38" t="s">
-        <v>217</v>
+        <v>403</v>
       </c>
       <c r="E195" s="39" t="s">
-        <v>586</v>
+        <v>1240</v>
       </c>
       <c r="F195" s="74" t="s">
         <v>585</v>
@@ -47433,7 +47433,7 @@
         <v>91</v>
       </c>
       <c r="D196" s="38" t="s">
-        <v>390</v>
+        <v>217</v>
       </c>
       <c r="E196" s="39" t="s">
         <v>586</v>
@@ -47451,7 +47451,7 @@
         <v>91</v>
       </c>
       <c r="D197" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E197" s="39" t="s">
         <v>586</v>
@@ -47469,7 +47469,7 @@
         <v>91</v>
       </c>
       <c r="D198" s="38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E198" s="39" t="s">
         <v>586</v>
@@ -47487,7 +47487,7 @@
         <v>91</v>
       </c>
       <c r="D199" s="38" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E199" s="39" t="s">
         <v>586</v>
@@ -47505,7 +47505,7 @@
         <v>91</v>
       </c>
       <c r="D200" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E200" s="39" t="s">
         <v>586</v>
@@ -47523,7 +47523,7 @@
         <v>91</v>
       </c>
       <c r="D201" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E201" s="39" t="s">
         <v>586</v>
@@ -47541,7 +47541,7 @@
         <v>91</v>
       </c>
       <c r="D202" s="38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E202" s="39" t="s">
         <v>586</v>
@@ -47556,13 +47556,13 @@
       </c>
       <c r="B203" s="35"/>
       <c r="C203" s="38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D203" s="38" t="s">
-        <v>217</v>
+        <v>403</v>
       </c>
       <c r="E203" s="39" t="s">
-        <v>1238</v>
+        <v>586</v>
       </c>
       <c r="F203" s="74" t="s">
         <v>585</v>
@@ -47577,7 +47577,7 @@
         <v>94</v>
       </c>
       <c r="D204" s="38" t="s">
-        <v>390</v>
+        <v>217</v>
       </c>
       <c r="E204" s="39" t="s">
         <v>1238</v>
@@ -47595,7 +47595,7 @@
         <v>94</v>
       </c>
       <c r="D205" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E205" s="39" t="s">
         <v>1238</v>
@@ -47613,7 +47613,7 @@
         <v>94</v>
       </c>
       <c r="D206" s="38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E206" s="39" t="s">
         <v>1238</v>
@@ -47631,7 +47631,7 @@
         <v>94</v>
       </c>
       <c r="D207" s="38" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E207" s="39" t="s">
         <v>1238</v>
@@ -47649,7 +47649,7 @@
         <v>94</v>
       </c>
       <c r="D208" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E208" s="39" t="s">
         <v>1238</v>
@@ -47667,7 +47667,7 @@
         <v>94</v>
       </c>
       <c r="D209" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E209" s="39" t="s">
         <v>1238</v>
@@ -47676,39 +47676,39 @@
         <v>585</v>
       </c>
     </row>
-    <row r="210" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
+    <row r="210" spans="1:6" ht="20" customHeight="1">
       <c r="A210" s="41">
         <v>42736</v>
       </c>
-      <c r="B210" s="52"/>
+      <c r="B210" s="35"/>
       <c r="C210" s="38" t="s">
         <v>94</v>
       </c>
       <c r="D210" s="38" t="s">
-        <v>403</v>
-      </c>
-      <c r="E210" s="42" t="s">
+        <v>401</v>
+      </c>
+      <c r="E210" s="39" t="s">
         <v>1238</v>
       </c>
-      <c r="F210" s="79" t="s">
+      <c r="F210" s="74" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="20" customHeight="1">
+    <row r="211" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
       <c r="A211" s="41">
         <v>42736</v>
       </c>
-      <c r="B211" s="35"/>
+      <c r="B211" s="52"/>
       <c r="C211" s="38" t="s">
         <v>94</v>
       </c>
       <c r="D211" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="E211" s="39" t="s">
-        <v>1237</v>
-      </c>
-      <c r="F211" s="74" t="s">
+        <v>403</v>
+      </c>
+      <c r="E211" s="42" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F211" s="79" t="s">
         <v>585</v>
       </c>
     </row>
@@ -47721,7 +47721,7 @@
         <v>94</v>
       </c>
       <c r="D212" s="38" t="s">
-        <v>390</v>
+        <v>217</v>
       </c>
       <c r="E212" s="39" t="s">
         <v>1237</v>
@@ -47739,7 +47739,7 @@
         <v>94</v>
       </c>
       <c r="D213" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E213" s="39" t="s">
         <v>1237</v>
@@ -47757,7 +47757,7 @@
         <v>94</v>
       </c>
       <c r="D214" s="38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E214" s="39" t="s">
         <v>1237</v>
@@ -47775,7 +47775,7 @@
         <v>94</v>
       </c>
       <c r="D215" s="38" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E215" s="39" t="s">
         <v>1237</v>
@@ -47793,7 +47793,7 @@
         <v>94</v>
       </c>
       <c r="D216" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E216" s="39" t="s">
         <v>1237</v>
@@ -47811,7 +47811,7 @@
         <v>94</v>
       </c>
       <c r="D217" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E217" s="39" t="s">
         <v>1237</v>
@@ -47829,7 +47829,7 @@
         <v>94</v>
       </c>
       <c r="D218" s="38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E218" s="39" t="s">
         <v>1237</v>
@@ -47847,10 +47847,10 @@
         <v>94</v>
       </c>
       <c r="D219" s="38" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="E219" s="39" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="F219" s="74" t="s">
         <v>585</v>
@@ -47865,7 +47865,7 @@
         <v>94</v>
       </c>
       <c r="D220" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E220" s="39" t="s">
         <v>1240</v>
@@ -47883,7 +47883,7 @@
         <v>94</v>
       </c>
       <c r="D221" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E221" s="39" t="s">
         <v>1240</v>
@@ -47901,7 +47901,7 @@
         <v>94</v>
       </c>
       <c r="D222" s="38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E222" s="39" t="s">
         <v>1240</v>
@@ -47919,10 +47919,10 @@
         <v>94</v>
       </c>
       <c r="D223" s="38" t="s">
-        <v>217</v>
+        <v>403</v>
       </c>
       <c r="E223" s="39" t="s">
-        <v>586</v>
+        <v>1240</v>
       </c>
       <c r="F223" s="74" t="s">
         <v>585</v>
@@ -47937,7 +47937,7 @@
         <v>94</v>
       </c>
       <c r="D224" s="38" t="s">
-        <v>390</v>
+        <v>217</v>
       </c>
       <c r="E224" s="39" t="s">
         <v>586</v>
@@ -47955,7 +47955,7 @@
         <v>94</v>
       </c>
       <c r="D225" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E225" s="39" t="s">
         <v>586</v>
@@ -47973,7 +47973,7 @@
         <v>94</v>
       </c>
       <c r="D226" s="38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E226" s="39" t="s">
         <v>586</v>
@@ -47991,7 +47991,7 @@
         <v>94</v>
       </c>
       <c r="D227" s="38" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E227" s="39" t="s">
         <v>586</v>
@@ -48009,7 +48009,7 @@
         <v>94</v>
       </c>
       <c r="D228" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E228" s="39" t="s">
         <v>586</v>
@@ -48027,7 +48027,7 @@
         <v>94</v>
       </c>
       <c r="D229" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E229" s="39" t="s">
         <v>586</v>
@@ -48045,7 +48045,7 @@
         <v>94</v>
       </c>
       <c r="D230" s="38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E230" s="39" t="s">
         <v>586</v>
@@ -48060,13 +48060,13 @@
       </c>
       <c r="B231" s="35"/>
       <c r="C231" s="38" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D231" s="38" t="s">
-        <v>217</v>
+        <v>403</v>
       </c>
       <c r="E231" s="39" t="s">
-        <v>1237</v>
+        <v>586</v>
       </c>
       <c r="F231" s="74" t="s">
         <v>585</v>
@@ -48081,7 +48081,7 @@
         <v>97</v>
       </c>
       <c r="D232" s="38" t="s">
-        <v>390</v>
+        <v>217</v>
       </c>
       <c r="E232" s="39" t="s">
         <v>1237</v>
@@ -48099,7 +48099,7 @@
         <v>97</v>
       </c>
       <c r="D233" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E233" s="39" t="s">
         <v>1237</v>
@@ -48117,7 +48117,7 @@
         <v>97</v>
       </c>
       <c r="D234" s="38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E234" s="39" t="s">
         <v>1237</v>
@@ -48135,7 +48135,7 @@
         <v>97</v>
       </c>
       <c r="D235" s="38" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E235" s="39" t="s">
         <v>1237</v>
@@ -48153,7 +48153,7 @@
         <v>97</v>
       </c>
       <c r="D236" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E236" s="39" t="s">
         <v>1237</v>
@@ -48171,7 +48171,7 @@
         <v>97</v>
       </c>
       <c r="D237" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E237" s="39" t="s">
         <v>1237</v>
@@ -48189,7 +48189,7 @@
         <v>97</v>
       </c>
       <c r="D238" s="38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E238" s="39" t="s">
         <v>1237</v>
@@ -48207,10 +48207,10 @@
         <v>97</v>
       </c>
       <c r="D239" s="38" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="E239" s="39" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="F239" s="74" t="s">
         <v>585</v>
@@ -48225,7 +48225,7 @@
         <v>97</v>
       </c>
       <c r="D240" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E240" s="39" t="s">
         <v>1240</v>
@@ -48243,7 +48243,7 @@
         <v>97</v>
       </c>
       <c r="D241" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E241" s="39" t="s">
         <v>1240</v>
@@ -48261,7 +48261,7 @@
         <v>97</v>
       </c>
       <c r="D242" s="38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E242" s="39" t="s">
         <v>1240</v>
@@ -48279,10 +48279,10 @@
         <v>97</v>
       </c>
       <c r="D243" s="38" t="s">
-        <v>217</v>
+        <v>403</v>
       </c>
       <c r="E243" s="39" t="s">
-        <v>586</v>
+        <v>1240</v>
       </c>
       <c r="F243" s="74" t="s">
         <v>585</v>
@@ -48297,7 +48297,7 @@
         <v>97</v>
       </c>
       <c r="D244" s="38" t="s">
-        <v>390</v>
+        <v>217</v>
       </c>
       <c r="E244" s="39" t="s">
         <v>586</v>
@@ -48315,7 +48315,7 @@
         <v>97</v>
       </c>
       <c r="D245" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E245" s="39" t="s">
         <v>586</v>
@@ -48333,7 +48333,7 @@
         <v>97</v>
       </c>
       <c r="D246" s="38" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E246" s="39" t="s">
         <v>586</v>
@@ -48351,7 +48351,7 @@
         <v>97</v>
       </c>
       <c r="D247" s="38" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E247" s="39" t="s">
         <v>586</v>
@@ -48369,7 +48369,7 @@
         <v>97</v>
       </c>
       <c r="D248" s="38" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E248" s="39" t="s">
         <v>586</v>
@@ -48387,7 +48387,7 @@
         <v>97</v>
       </c>
       <c r="D249" s="38" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E249" s="39" t="s">
         <v>586</v>
@@ -48405,7 +48405,7 @@
         <v>97</v>
       </c>
       <c r="D250" s="38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E250" s="39" t="s">
         <v>586</v>
@@ -48419,11 +48419,11 @@
         <v>42736</v>
       </c>
       <c r="B251" s="35"/>
-      <c r="C251" s="428" t="s">
-        <v>100</v>
-      </c>
-      <c r="D251" s="483" t="s">
-        <v>165</v>
+      <c r="C251" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D251" s="38" t="s">
+        <v>403</v>
       </c>
       <c r="E251" s="39" t="s">
         <v>586</v>
@@ -48437,11 +48437,11 @@
         <v>42736</v>
       </c>
       <c r="B252" s="35"/>
-      <c r="C252" s="38" t="s">
+      <c r="C252" s="428" t="s">
         <v>100</v>
       </c>
-      <c r="D252" s="484" t="s">
-        <v>169</v>
+      <c r="D252" s="483" t="s">
+        <v>165</v>
       </c>
       <c r="E252" s="39" t="s">
         <v>586</v>
@@ -48455,11 +48455,11 @@
         <v>42736</v>
       </c>
       <c r="B253" s="35"/>
-      <c r="C253" s="428" t="s">
+      <c r="C253" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="D253" s="483" t="s">
-        <v>172</v>
+      <c r="D253" s="484" t="s">
+        <v>169</v>
       </c>
       <c r="E253" s="39" t="s">
         <v>586</v>
@@ -48473,11 +48473,11 @@
         <v>42736</v>
       </c>
       <c r="B254" s="35"/>
-      <c r="C254" s="38" t="s">
+      <c r="C254" s="428" t="s">
         <v>100</v>
       </c>
-      <c r="D254" s="425" t="s">
-        <v>241</v>
+      <c r="D254" s="483" t="s">
+        <v>172</v>
       </c>
       <c r="E254" s="39" t="s">
         <v>586</v>
@@ -48491,11 +48491,11 @@
         <v>42736</v>
       </c>
       <c r="B255" s="35"/>
-      <c r="C255" s="428" t="s">
+      <c r="C255" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="D255" s="426" t="s">
-        <v>253</v>
+      <c r="D255" s="425" t="s">
+        <v>241</v>
       </c>
       <c r="E255" s="39" t="s">
         <v>586</v>
@@ -48509,11 +48509,11 @@
         <v>42736</v>
       </c>
       <c r="B256" s="35"/>
-      <c r="C256" s="38" t="s">
+      <c r="C256" s="428" t="s">
         <v>100</v>
       </c>
-      <c r="D256" s="36" t="s">
-        <v>181</v>
+      <c r="D256" s="426" t="s">
+        <v>253</v>
       </c>
       <c r="E256" s="39" t="s">
         <v>586</v>
@@ -48523,20 +48523,20 @@
       </c>
     </row>
     <row r="257" spans="1:6" ht="20" customHeight="1">
-      <c r="A257" s="472">
-        <v>42736</v>
-      </c>
-      <c r="B257" s="473"/>
-      <c r="C257" s="453" t="s">
-        <v>103</v>
-      </c>
-      <c r="D257" s="433" t="s">
-        <v>165</v>
-      </c>
-      <c r="E257" s="474" t="s">
+      <c r="A257" s="41">
+        <v>42736</v>
+      </c>
+      <c r="B257" s="35"/>
+      <c r="C257" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D257" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E257" s="39" t="s">
         <v>586</v>
       </c>
-      <c r="F257" s="475" t="s">
+      <c r="F257" s="74" t="s">
         <v>585</v>
       </c>
     </row>
@@ -48549,7 +48549,7 @@
         <v>103</v>
       </c>
       <c r="D258" s="433" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E258" s="474" t="s">
         <v>586</v>
@@ -48567,7 +48567,7 @@
         <v>103</v>
       </c>
       <c r="D259" s="433" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
       <c r="E259" s="474" t="s">
         <v>586</v>
@@ -48585,7 +48585,7 @@
         <v>103</v>
       </c>
       <c r="D260" s="433" t="s">
-        <v>404</v>
+        <v>210</v>
       </c>
       <c r="E260" s="474" t="s">
         <v>586</v>
@@ -48598,17 +48598,17 @@
       <c r="A261" s="472">
         <v>42736</v>
       </c>
-      <c r="B261" s="472"/>
-      <c r="C261" s="472" t="s">
+      <c r="B261" s="473"/>
+      <c r="C261" s="453" t="s">
         <v>103</v>
       </c>
-      <c r="D261" s="472" t="s">
-        <v>406</v>
-      </c>
-      <c r="E261" s="472" t="s">
+      <c r="D261" s="433" t="s">
+        <v>404</v>
+      </c>
+      <c r="E261" s="474" t="s">
         <v>586</v>
       </c>
-      <c r="F261" s="472" t="s">
+      <c r="F261" s="475" t="s">
         <v>585</v>
       </c>
     </row>
@@ -48621,7 +48621,7 @@
         <v>103</v>
       </c>
       <c r="D262" s="472" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E262" s="472" t="s">
         <v>586</v>
@@ -48630,7 +48630,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="13.25" customHeight="1">
+    <row r="263" spans="1:6" ht="20" customHeight="1">
       <c r="A263" s="472">
         <v>42736</v>
       </c>
@@ -48639,7 +48639,7 @@
         <v>103</v>
       </c>
       <c r="D263" s="472" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E263" s="472" t="s">
         <v>586</v>
@@ -48657,7 +48657,7 @@
         <v>103</v>
       </c>
       <c r="D264" s="472" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E264" s="472" t="s">
         <v>586</v>
@@ -48666,21 +48666,21 @@
         <v>585</v>
       </c>
     </row>
-    <row r="265" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
-      <c r="A265" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B265" s="35"/>
-      <c r="C265" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D265" s="36" t="s">
-        <v>165</v>
-      </c>
-      <c r="E265" s="50" t="s">
+    <row r="265" spans="1:6" ht="13.25" customHeight="1">
+      <c r="A265" s="472">
+        <v>42736</v>
+      </c>
+      <c r="B265" s="472"/>
+      <c r="C265" s="472" t="s">
+        <v>103</v>
+      </c>
+      <c r="D265" s="472" t="s">
+        <v>414</v>
+      </c>
+      <c r="E265" s="472" t="s">
         <v>586</v>
       </c>
-      <c r="F265" s="74" t="s">
+      <c r="F265" s="472" t="s">
         <v>585</v>
       </c>
     </row>
@@ -48693,13 +48693,13 @@
         <v>106</v>
       </c>
       <c r="D266" s="36" t="s">
-        <v>282</v>
+        <v>165</v>
       </c>
       <c r="E266" s="50" t="s">
         <v>586</v>
       </c>
       <c r="F266" s="74" t="s">
-        <v>1241</v>
+        <v>585</v>
       </c>
     </row>
     <row r="267" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
@@ -48711,13 +48711,13 @@
         <v>106</v>
       </c>
       <c r="D267" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E267" s="50" t="s">
         <v>586</v>
       </c>
       <c r="F267" s="74" t="s">
-        <v>587</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="268" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
@@ -48728,14 +48728,14 @@
       <c r="C268" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D268" s="38" t="s">
-        <v>286</v>
+      <c r="D268" s="36" t="s">
+        <v>284</v>
       </c>
       <c r="E268" s="50" t="s">
         <v>586</v>
       </c>
-      <c r="F268" s="188" t="s">
-        <v>585</v>
+      <c r="F268" s="74" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="269" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
@@ -48747,31 +48747,31 @@
         <v>106</v>
       </c>
       <c r="D269" s="38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E269" s="50" t="s">
         <v>586</v>
       </c>
-      <c r="F269" s="74" t="s">
+      <c r="F269" s="188" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
+      <c r="A270" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B270" s="35"/>
+      <c r="C270" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D270" s="38" t="s">
+        <v>288</v>
+      </c>
+      <c r="E270" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="F270" s="74" t="s">
         <v>587</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" s="285" customFormat="1" ht="20" customHeight="1">
-      <c r="A270" s="516">
-        <v>42736</v>
-      </c>
-      <c r="B270" s="488"/>
-      <c r="C270" s="490" t="s">
-        <v>109</v>
-      </c>
-      <c r="D270" s="490" t="s">
-        <v>165</v>
-      </c>
-      <c r="E270" s="491" t="s">
-        <v>586</v>
-      </c>
-      <c r="F270" s="493" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="271" spans="1:6" s="285" customFormat="1" ht="20" customHeight="1">
@@ -48786,27 +48786,27 @@
         <v>165</v>
       </c>
       <c r="E271" s="491" t="s">
-        <v>1237</v>
+        <v>586</v>
       </c>
       <c r="F271" s="493" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="272" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
-      <c r="A272" s="34">
-        <v>42736</v>
-      </c>
-      <c r="B272" s="35"/>
-      <c r="C272" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D272" s="36" t="s">
+    <row r="272" spans="1:6" s="285" customFormat="1" ht="20" customHeight="1">
+      <c r="A272" s="516">
+        <v>42736</v>
+      </c>
+      <c r="B272" s="488"/>
+      <c r="C272" s="490" t="s">
+        <v>109</v>
+      </c>
+      <c r="D272" s="490" t="s">
         <v>165</v>
       </c>
-      <c r="E272" s="50" t="s">
-        <v>586</v>
-      </c>
-      <c r="F272" s="74" t="s">
+      <c r="E272" s="491" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F272" s="493" t="s">
         <v>585</v>
       </c>
     </row>
@@ -48816,7 +48816,7 @@
       </c>
       <c r="B273" s="35"/>
       <c r="C273" s="38" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D273" s="36" t="s">
         <v>165</v>
@@ -48834,7 +48834,7 @@
       </c>
       <c r="B274" s="35"/>
       <c r="C274" s="38" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D274" s="36" t="s">
         <v>165</v>
@@ -48843,6 +48843,24 @@
         <v>586</v>
       </c>
       <c r="F274" s="74" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" s="290" customFormat="1" ht="20" customHeight="1">
+      <c r="A275" s="34">
+        <v>42736</v>
+      </c>
+      <c r="B275" s="35"/>
+      <c r="C275" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D275" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="E275" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="F275" s="74" t="s">
         <v>585</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding missing invalid def file and adding searchCriteria to masterCaseType
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F6A4BCC-31AA-45C9-B735-F5EF7A998EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABF05F8B-3942-4C19-AA7B-230A6D0A69EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60660" yWindow="400" windowWidth="28800" windowHeight="16440" firstSheet="25" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60660" yWindow="400" windowWidth="28800" windowHeight="16440" firstSheet="26" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10258" uniqueCount="1293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10260" uniqueCount="1293">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -6493,16 +6493,16 @@
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Explanatory Text" xfId="14" builtinId="53"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
@@ -53161,7 +53161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8940C136-71BC-4A6C-9A16-A91A0EC48C23}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
@@ -53899,9 +53899,11 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D71A9F6-41FB-48D6-A885-E8BB581EF700}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="A4:D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -53953,10 +53955,10 @@
       </c>
       <c r="B4" s="528"/>
       <c r="C4" s="530" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D4" s="530" t="s">
-        <v>238</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -53968,7 +53970,7 @@
         <v>46</v>
       </c>
       <c r="D5" s="530" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -53980,7 +53982,7 @@
         <v>46</v>
       </c>
       <c r="D6" s="530" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -53989,10 +53991,10 @@
       </c>
       <c r="B7" s="528"/>
       <c r="C7" s="530" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D7" s="530" t="s">
-        <v>1264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -54001,9 +54003,11 @@
       </c>
       <c r="B8" s="528"/>
       <c r="C8" s="530" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="530"/>
+        <v>61</v>
+      </c>
+      <c r="D8" s="530" t="s">
+        <v>1264</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="534">
@@ -54011,11 +54015,9 @@
       </c>
       <c r="B9" s="528"/>
       <c r="C9" s="530" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="530" t="s">
-        <v>12</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D9" s="530"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="534">
@@ -54023,14 +54025,23 @@
       </c>
       <c r="B10" s="528"/>
       <c r="C10" s="530" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="530" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="534">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="528"/>
+      <c r="C11" s="530" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="530" t="s">
+      <c r="D11" s="530" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" s="399"/>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="399"/>
@@ -54043,6 +54054,9 @@
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="399"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="399"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RDM-12806 ccd-test-definitions prerelease for CR&D
   [RDM-12806](https://tools.hmcts.net/jira/browse/RDM-12806)

ccd-test-definitions prerelease for CR&D.
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20334C8C-4361-AE47-BB8E-F9024349F50A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8D084F-133B-B843-ADD1-609C0B29D456}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="21380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="42740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11609" uniqueCount="1398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11609" uniqueCount="1404">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -4220,9 +4220,6 @@
     <t>updateCaseSubmitTTL</t>
   </si>
   <si>
-    <t>${TEST_STUB_SERVICE_BASE_URL:http://ccd-test-stubs-service-aat.service.core-compute-aat.internal}//callback_unmodified</t>
-  </si>
-  <si>
     <t>updateCaseSubmitSuspendedTTL</t>
   </si>
   <si>
@@ -4342,6 +4339,27 @@
   </si>
   <si>
     <t>Standard case links field</t>
+  </si>
+  <si>
+    <t>${TEST_STUB_SERVICE_BASE_URL:http://ccd-test-stubs-service-aat.service.core-compute-aat.internal}/callback_unmodified</t>
+  </si>
+  <si>
+    <t>Update a case midevent Suspended TTL</t>
+  </si>
+  <si>
+    <t>Update midevent SuspendedTTL</t>
+  </si>
+  <si>
+    <t>Update midevent SystemTTL</t>
+  </si>
+  <si>
+    <t>Update midevent OverrideTTL</t>
+  </si>
+  <si>
+    <t>Update a case midevent Override TTL</t>
+  </si>
+  <si>
+    <t>Update a case midevent System TTL</t>
   </si>
 </sst>
 </file>
@@ -19213,7 +19231,7 @@
         <v>942</v>
       </c>
       <c r="W2" s="253" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
@@ -19284,7 +19302,7 @@
         <v>668</v>
       </c>
       <c r="W3" s="349" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="4" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
@@ -19409,7 +19427,7 @@
       <c r="K6" s="144"/>
       <c r="L6" s="144"/>
       <c r="M6" s="144" t="s">
-        <v>1357</v>
+        <v>1397</v>
       </c>
       <c r="N6" s="144"/>
       <c r="O6" s="144"/>
@@ -19436,13 +19454,13 @@
         <v>41</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>958</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="G7" s="127">
         <v>1</v>
@@ -19457,7 +19475,7 @@
       <c r="K7" s="144"/>
       <c r="L7" s="144"/>
       <c r="M7" s="144" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="N7" s="144"/>
       <c r="O7" s="144"/>
@@ -19484,10 +19502,10 @@
         <v>41</v>
       </c>
       <c r="D8" s="15" t="s">
+        <v>1360</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>1361</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>1362</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>956</v>
@@ -19528,13 +19546,13 @@
         <v>41</v>
       </c>
       <c r="D9" s="15" t="s">
+        <v>1362</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>1363</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="F9" s="15" t="s">
         <v>1364</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>1365</v>
       </c>
       <c r="G9" s="127">
         <v>1</v>
@@ -19547,7 +19565,7 @@
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="144" t="s">
-        <v>1357</v>
+        <v>1397</v>
       </c>
       <c r="L9" s="144"/>
       <c r="M9" s="144"/>
@@ -19566,7 +19584,7 @@
       <c r="U9" s="15"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="10" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
@@ -19578,13 +19596,13 @@
         <v>41</v>
       </c>
       <c r="D10" s="15" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>1367</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="F10" s="15" t="s">
         <v>1368</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>1369</v>
       </c>
       <c r="G10" s="127">
         <v>1</v>
@@ -19597,7 +19615,7 @@
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="144" t="s">
-        <v>1357</v>
+        <v>1397</v>
       </c>
       <c r="L10" s="144"/>
       <c r="M10" s="144"/>
@@ -19626,13 +19644,13 @@
         <v>41</v>
       </c>
       <c r="D11" s="15" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>1370</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="F11" s="15" t="s">
         <v>1371</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>1372</v>
       </c>
       <c r="G11" s="127">
         <v>1</v>
@@ -19645,7 +19663,7 @@
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="144" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="L11" s="144"/>
       <c r="M11" s="144"/>
@@ -19664,7 +19682,7 @@
       <c r="U11" s="15"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="12" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
@@ -19676,13 +19694,13 @@
         <v>41</v>
       </c>
       <c r="D12" s="15" t="s">
+        <v>1373</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>1374</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="F12" s="15" t="s">
         <v>1375</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>1376</v>
       </c>
       <c r="G12" s="127">
         <v>1</v>
@@ -19695,7 +19713,7 @@
       </c>
       <c r="J12" s="15"/>
       <c r="K12" s="144" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="L12" s="144"/>
       <c r="M12" s="144"/>
@@ -19714,7 +19732,7 @@
       <c r="U12" s="15"/>
       <c r="V12" s="10"/>
       <c r="W12" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="13" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
@@ -19726,13 +19744,13 @@
         <v>41</v>
       </c>
       <c r="D13" s="15" t="s">
+        <v>1377</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>1378</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="F13" s="15" t="s">
         <v>1379</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>1380</v>
       </c>
       <c r="G13" s="127">
         <v>1</v>
@@ -19745,7 +19763,7 @@
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="144" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="L13" s="144"/>
       <c r="M13" s="144"/>
@@ -19764,7 +19782,7 @@
       <c r="U13" s="15"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="14" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
@@ -19776,13 +19794,13 @@
         <v>41</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>1379</v>
+        <v>1399</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>1380</v>
+        <v>1398</v>
       </c>
       <c r="G14" s="127">
         <v>1</v>
@@ -19812,7 +19830,7 @@
       <c r="U14" s="15"/>
       <c r="V14" s="10"/>
       <c r="W14" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="15" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
@@ -19824,13 +19842,13 @@
         <v>41</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>1375</v>
+        <v>1400</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>1376</v>
+        <v>1403</v>
       </c>
       <c r="G15" s="127">
         <v>1</v>
@@ -19860,7 +19878,7 @@
       <c r="U15" s="15"/>
       <c r="V15" s="10"/>
       <c r="W15" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="16" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
@@ -19872,13 +19890,13 @@
         <v>41</v>
       </c>
       <c r="D16" s="15" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>1384</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="F16" s="15" t="s">
         <v>1385</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>1386</v>
       </c>
       <c r="G16" s="127">
         <v>1</v>
@@ -19908,7 +19926,7 @@
       <c r="U16" s="15"/>
       <c r="V16" s="10"/>
       <c r="W16" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="17" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
@@ -19920,13 +19938,13 @@
         <v>41</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>1371</v>
+        <v>1401</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>1372</v>
+        <v>1402</v>
       </c>
       <c r="G17" s="127">
         <v>1</v>
@@ -19956,7 +19974,7 @@
       <c r="U17" s="15"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="18" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
@@ -19968,10 +19986,10 @@
         <v>41</v>
       </c>
       <c r="D18" s="15" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>1388</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>1389</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>956</v>
@@ -24833,7 +24851,7 @@
         <v>41</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>1351</v>
@@ -24865,7 +24883,7 @@
         <v>41</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>1351</v>
@@ -24897,7 +24915,7 @@
         <v>41</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>1351</v>
@@ -24929,7 +24947,7 @@
         <v>41</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>1351</v>
@@ -24961,7 +24979,7 @@
         <v>41</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>1351</v>
@@ -24993,7 +25011,7 @@
         <v>41</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>1351</v>
@@ -25025,7 +25043,7 @@
         <v>41</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>1351</v>
@@ -25048,7 +25066,7 @@
         <v>259</v>
       </c>
       <c r="R30" s="35" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="35" customFormat="1" ht="20" customHeight="1">
@@ -25060,7 +25078,7 @@
         <v>41</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>1351</v>
@@ -25083,7 +25101,7 @@
         <v>259</v>
       </c>
       <c r="R31" s="35" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="35" customFormat="1" ht="20" customHeight="1">
@@ -25095,7 +25113,7 @@
         <v>41</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>1351</v>
@@ -25118,7 +25136,7 @@
         <v>259</v>
       </c>
       <c r="R32" s="35" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="33" spans="1:20" s="35" customFormat="1" ht="20" customHeight="1">
@@ -25207,7 +25225,7 @@
         <v>706</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="F35" s="41">
         <v>1</v>
@@ -25238,7 +25256,7 @@
         <v>41</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>236</v>
@@ -25270,7 +25288,7 @@
         <v>41</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>271</v>
@@ -25302,10 +25320,10 @@
         <v>41</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="F38" s="41">
         <v>1</v>
@@ -43748,7 +43766,7 @@
         <v>41</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="E32" s="35" t="s">
         <v>627</v>
@@ -43766,7 +43784,7 @@
         <v>41</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="E33" s="35" t="s">
         <v>1247</v>
@@ -49766,7 +49784,7 @@
         <v>41</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="E5" s="38" t="s">
         <v>627</v>
@@ -49783,7 +49801,7 @@
         <v>41</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>1247</v>
@@ -49905,7 +49923,7 @@
         <v>41</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="E13" s="350" t="s">
         <v>627</v>
@@ -49923,7 +49941,7 @@
         <v>41</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="E14" s="350" t="s">
         <v>1247</v>
@@ -49941,7 +49959,7 @@
         <v>41</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="E15" s="350" t="s">
         <v>627</v>
@@ -49959,7 +49977,7 @@
         <v>41</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="E16" s="350" t="s">
         <v>1247</v>
@@ -49977,7 +49995,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="E17" s="350" t="s">
         <v>627</v>
@@ -49995,7 +50013,7 @@
         <v>41</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="E18" s="350" t="s">
         <v>627</v>
@@ -50013,7 +50031,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E19" s="350" t="s">
         <v>627</v>
@@ -50031,7 +50049,7 @@
         <v>41</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="E20" s="350" t="s">
         <v>627</v>
@@ -50049,7 +50067,7 @@
         <v>41</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="E21" s="350" t="s">
         <v>627</v>
@@ -50067,7 +50085,7 @@
         <v>41</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="E22" s="350" t="s">
         <v>1247</v>
@@ -50085,7 +50103,7 @@
         <v>41</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="E23" s="350" t="s">
         <v>627</v>
@@ -50103,7 +50121,7 @@
         <v>41</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="E24" s="350" t="s">
         <v>1247</v>
@@ -50121,7 +50139,7 @@
         <v>41</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="E25" s="350" t="s">
         <v>1247</v>
@@ -50139,7 +50157,7 @@
         <v>41</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="E26" s="350" t="s">
         <v>627</v>
@@ -50157,7 +50175,7 @@
         <v>41</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="E27" s="350" t="s">
         <v>1247</v>
@@ -50175,7 +50193,7 @@
         <v>41</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="E28" s="350" t="s">
         <v>627</v>
@@ -50193,7 +50211,7 @@
         <v>41</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="E29" s="350" t="s">
         <v>1247</v>
@@ -54410,7 +54428,7 @@
       </c>
       <c r="B16" s="83"/>
       <c r="C16" s="35" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="D16" s="40"/>
       <c r="E16" s="10" t="s">
@@ -55765,8 +55783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -56989,7 +57007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IO234"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -57887,10 +57905,10 @@
         <v>41</v>
       </c>
       <c r="D29" s="15" t="s">
+        <v>1395</v>
+      </c>
+      <c r="E29" s="15" t="s">
         <v>1396</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>1397</v>
       </c>
       <c r="F29" s="39"/>
       <c r="G29" s="10" t="s">

</xml_diff>

<commit_message>
CCD-2779 - Test data added for CCD-2779 FTA tests
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/BEFTA_Master_Definition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8D084F-133B-B843-ADD1-609C0B29D456}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BDE765-5B44-B14D-8BB7-580485569908}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="42740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11609" uniqueCount="1404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11618" uniqueCount="1407">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -4360,6 +4360,15 @@
   </si>
   <si>
     <t>Update a case midevent System TTL</t>
+  </si>
+  <si>
+    <t>createCaseInjectedData</t>
+  </si>
+  <si>
+    <t>An event with injected data</t>
+  </si>
+  <si>
+    <t>Create case injected data</t>
   </si>
 </sst>
 </file>
@@ -4372,7 +4381,7 @@
     <numFmt numFmtId="166" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="60">
+  <fonts count="62">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -4739,8 +4748,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4861,8 +4882,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor rgb="FFDCE6F1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -4880,6 +4907,36 @@
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4903,7 +4960,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="352">
+  <cellXfs count="360">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5870,6 +5927,30 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="60" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="60" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="61" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="60" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -11486,8 +11567,7 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:W110" totalsRowShown="0" headerRowDxfId="215" dataDxfId="213" headerRowBorderDxfId="214" tableBorderDxfId="212" totalsRowBorderDxfId="211">
-  <autoFilter ref="A3:W110" xr:uid="{3C2856EB-06E3-4E47-A9E1-F995066A5408}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:W111" totalsRowShown="0" headerRowDxfId="215" dataDxfId="213" headerRowBorderDxfId="214" tableBorderDxfId="212" totalsRowBorderDxfId="211">
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="210"/>
     <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="209"/>
@@ -13445,8 +13525,8 @@
   <dimension ref="A1:CR116"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -19098,11 +19178,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:W110"/>
+  <dimension ref="A1:W111"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F95" sqref="A95:XFD95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -19115,7 +19195,8 @@
     <col min="6" max="6" width="45.5" style="16" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" style="16" customWidth="1"/>
     <col min="8" max="8" width="22.6640625" style="16" customWidth="1"/>
-    <col min="9" max="10" width="25.6640625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" style="16" customWidth="1"/>
+    <col min="10" max="10" width="33.5" style="16" customWidth="1"/>
     <col min="11" max="11" width="61.6640625" style="16" customWidth="1"/>
     <col min="12" max="12" width="29.83203125" style="16" customWidth="1"/>
     <col min="13" max="13" width="33.83203125" style="16" customWidth="1"/>
@@ -23382,46 +23463,48 @@
       <c r="A95" s="13">
         <v>42736</v>
       </c>
-      <c r="B95" s="13"/>
-      <c r="C95" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D95" s="10" t="s">
-        <v>1012</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>956</v>
-      </c>
-      <c r="F95" s="10" t="s">
-        <v>956</v>
-      </c>
-      <c r="G95" s="127">
+      <c r="B95" s="352"/>
+      <c r="C95" s="353" t="s">
+        <v>121</v>
+      </c>
+      <c r="D95" s="353" t="s">
+        <v>1404</v>
+      </c>
+      <c r="E95" s="353" t="s">
+        <v>1406</v>
+      </c>
+      <c r="F95" s="353" t="s">
+        <v>1405</v>
+      </c>
+      <c r="G95" s="354">
         <v>1</v>
       </c>
-      <c r="H95" s="10"/>
-      <c r="I95" s="10" t="s">
+      <c r="H95" s="353"/>
+      <c r="I95" s="355" t="s">
         <v>888</v>
       </c>
-      <c r="J95" s="10"/>
-      <c r="K95" s="144"/>
-      <c r="L95" s="144"/>
-      <c r="M95" s="144"/>
-      <c r="N95" s="144"/>
-      <c r="O95" s="144"/>
-      <c r="P95" s="144"/>
-      <c r="Q95" s="10" t="s">
+      <c r="J95" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="K95" s="356"/>
+      <c r="L95" s="357"/>
+      <c r="M95" s="357"/>
+      <c r="N95" s="357"/>
+      <c r="O95" s="357"/>
+      <c r="P95" s="357"/>
+      <c r="Q95" s="355" t="s">
         <v>45</v>
       </c>
-      <c r="R95" s="10" t="s">
+      <c r="R95" s="355" t="s">
         <v>259</v>
       </c>
-      <c r="S95" s="41"/>
-      <c r="T95" s="41" t="s">
+      <c r="S95" s="358"/>
+      <c r="T95" s="358" t="s">
         <v>255</v>
       </c>
-      <c r="U95" s="10"/>
-      <c r="V95" s="10"/>
-      <c r="W95" s="10"/>
+      <c r="U95" s="355"/>
+      <c r="V95" s="355"/>
+      <c r="W95" s="359"/>
     </row>
     <row r="96" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
       <c r="A96" s="13">
@@ -23432,22 +23515,20 @@
         <v>124</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="G96" s="127">
         <v>1</v>
       </c>
-      <c r="H96" s="10" t="s">
+      <c r="H96" s="10"/>
+      <c r="I96" s="10" t="s">
         <v>888</v>
-      </c>
-      <c r="I96" s="10" t="s">
-        <v>890</v>
       </c>
       <c r="J96" s="10"/>
       <c r="K96" s="144"/>
@@ -23479,27 +23560,27 @@
         <v>124</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>1068</v>
+        <v>1015</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>1069</v>
+        <v>958</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>1069</v>
+        <v>958</v>
       </c>
       <c r="G97" s="127">
         <v>1</v>
       </c>
-      <c r="H97" s="10"/>
+      <c r="H97" s="10" t="s">
+        <v>888</v>
+      </c>
       <c r="I97" s="10" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="144"/>
       <c r="L97" s="144"/>
-      <c r="M97" s="144" t="s">
-        <v>1070</v>
-      </c>
+      <c r="M97" s="144"/>
       <c r="N97" s="144"/>
       <c r="O97" s="144"/>
       <c r="P97" s="144"/>
@@ -23517,49 +23598,52 @@
       <c r="V97" s="10"/>
       <c r="W97" s="10"/>
     </row>
-    <row r="98" spans="1:23" s="77" customFormat="1" ht="20" customHeight="1">
-      <c r="A98" s="73">
-        <v>42736</v>
-      </c>
-      <c r="B98" s="73"/>
-      <c r="C98" s="74" t="s">
-        <v>126</v>
-      </c>
-      <c r="D98" s="76" t="s">
-        <v>1012</v>
-      </c>
-      <c r="E98" s="76" t="s">
-        <v>956</v>
-      </c>
-      <c r="F98" s="76" t="s">
-        <v>956</v>
-      </c>
-      <c r="G98" s="141">
+    <row r="98" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="A98" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B98" s="13"/>
+      <c r="C98" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F98" s="10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="G98" s="127">
         <v>1</v>
       </c>
-      <c r="H98" s="76"/>
-      <c r="I98" s="76" t="s">
+      <c r="H98" s="10"/>
+      <c r="I98" s="10" t="s">
         <v>888</v>
       </c>
-      <c r="J98" s="76"/>
-      <c r="K98" s="146"/>
-      <c r="L98" s="146"/>
-      <c r="M98" s="146"/>
-      <c r="N98" s="146"/>
-      <c r="O98" s="146"/>
-      <c r="P98" s="146"/>
-      <c r="Q98" s="76" t="s">
+      <c r="J98" s="10"/>
+      <c r="K98" s="144"/>
+      <c r="L98" s="144"/>
+      <c r="M98" s="144" t="s">
+        <v>1070</v>
+      </c>
+      <c r="N98" s="144"/>
+      <c r="O98" s="144"/>
+      <c r="P98" s="144"/>
+      <c r="Q98" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="R98" s="76" t="s">
+      <c r="R98" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="T98" s="77" t="s">
+      <c r="S98" s="41"/>
+      <c r="T98" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="U98" s="76"/>
-      <c r="V98" s="76"/>
-      <c r="W98" s="76"/>
+      <c r="U98" s="10"/>
+      <c r="V98" s="10"/>
+      <c r="W98" s="10"/>
     </row>
     <row r="99" spans="1:23" s="77" customFormat="1" ht="20" customHeight="1">
       <c r="A99" s="73">
@@ -23569,23 +23653,21 @@
       <c r="C99" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="D99" s="74" t="s">
-        <v>1015</v>
-      </c>
-      <c r="E99" s="74" t="s">
-        <v>958</v>
-      </c>
-      <c r="F99" s="74" t="s">
-        <v>958</v>
+      <c r="D99" s="76" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E99" s="76" t="s">
+        <v>956</v>
+      </c>
+      <c r="F99" s="76" t="s">
+        <v>956</v>
       </c>
       <c r="G99" s="141">
         <v>1</v>
       </c>
-      <c r="H99" s="74" t="s">
-        <v>984</v>
-      </c>
-      <c r="I99" s="74" t="s">
-        <v>984</v>
+      <c r="H99" s="76"/>
+      <c r="I99" s="76" t="s">
+        <v>888</v>
       </c>
       <c r="J99" s="76"/>
       <c r="K99" s="146"/>
@@ -23613,23 +23695,25 @@
       </c>
       <c r="B100" s="73"/>
       <c r="C100" s="74" t="s">
-        <v>128</v>
-      </c>
-      <c r="D100" s="76" t="s">
-        <v>1012</v>
-      </c>
-      <c r="E100" s="76" t="s">
-        <v>956</v>
-      </c>
-      <c r="F100" s="76" t="s">
-        <v>956</v>
+        <v>126</v>
+      </c>
+      <c r="D100" s="74" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E100" s="74" t="s">
+        <v>958</v>
+      </c>
+      <c r="F100" s="74" t="s">
+        <v>958</v>
       </c>
       <c r="G100" s="141">
         <v>1</v>
       </c>
-      <c r="H100" s="76"/>
-      <c r="I100" s="76" t="s">
-        <v>888</v>
+      <c r="H100" s="74" t="s">
+        <v>984</v>
+      </c>
+      <c r="I100" s="74" t="s">
+        <v>984</v>
       </c>
       <c r="J100" s="76"/>
       <c r="K100" s="146"/>
@@ -23659,23 +23743,21 @@
       <c r="C101" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="D101" s="74" t="s">
-        <v>1015</v>
-      </c>
-      <c r="E101" s="74" t="s">
-        <v>958</v>
-      </c>
-      <c r="F101" s="74" t="s">
-        <v>958</v>
+      <c r="D101" s="76" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E101" s="76" t="s">
+        <v>956</v>
+      </c>
+      <c r="F101" s="76" t="s">
+        <v>956</v>
       </c>
       <c r="G101" s="141">
         <v>1</v>
       </c>
-      <c r="H101" s="74" t="s">
-        <v>984</v>
-      </c>
-      <c r="I101" s="74" t="s">
-        <v>984</v>
+      <c r="H101" s="76"/>
+      <c r="I101" s="76" t="s">
+        <v>888</v>
       </c>
       <c r="J101" s="76"/>
       <c r="K101" s="146"/>
@@ -23703,23 +23785,25 @@
       </c>
       <c r="B102" s="73"/>
       <c r="C102" s="74" t="s">
-        <v>129</v>
-      </c>
-      <c r="D102" s="76" t="s">
-        <v>1012</v>
-      </c>
-      <c r="E102" s="76" t="s">
-        <v>956</v>
-      </c>
-      <c r="F102" s="76" t="s">
-        <v>956</v>
+        <v>128</v>
+      </c>
+      <c r="D102" s="74" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E102" s="74" t="s">
+        <v>958</v>
+      </c>
+      <c r="F102" s="74" t="s">
+        <v>958</v>
       </c>
       <c r="G102" s="141">
         <v>1</v>
       </c>
-      <c r="H102" s="76"/>
-      <c r="I102" s="76" t="s">
-        <v>888</v>
+      <c r="H102" s="74" t="s">
+        <v>984</v>
+      </c>
+      <c r="I102" s="74" t="s">
+        <v>984</v>
       </c>
       <c r="J102" s="76"/>
       <c r="K102" s="146"/>
@@ -23749,23 +23833,21 @@
       <c r="C103" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="D103" s="74" t="s">
-        <v>1015</v>
-      </c>
-      <c r="E103" s="74" t="s">
-        <v>958</v>
-      </c>
-      <c r="F103" s="74" t="s">
-        <v>958</v>
+      <c r="D103" s="76" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E103" s="76" t="s">
+        <v>956</v>
+      </c>
+      <c r="F103" s="76" t="s">
+        <v>956</v>
       </c>
       <c r="G103" s="141">
         <v>1</v>
       </c>
-      <c r="H103" s="74" t="s">
-        <v>984</v>
-      </c>
-      <c r="I103" s="74" t="s">
-        <v>984</v>
+      <c r="H103" s="76"/>
+      <c r="I103" s="76" t="s">
+        <v>888</v>
       </c>
       <c r="J103" s="76"/>
       <c r="K103" s="146"/>
@@ -23787,72 +23869,93 @@
       <c r="V103" s="76"/>
       <c r="W103" s="76"/>
     </row>
-    <row r="104" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
-      <c r="A104" s="13">
+    <row r="104" spans="1:23" s="77" customFormat="1" ht="20" customHeight="1">
+      <c r="A104" s="73">
+        <v>42736</v>
+      </c>
+      <c r="B104" s="73"/>
+      <c r="C104" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="D104" s="74" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E104" s="74" t="s">
+        <v>958</v>
+      </c>
+      <c r="F104" s="74" t="s">
+        <v>958</v>
+      </c>
+      <c r="G104" s="141">
+        <v>1</v>
+      </c>
+      <c r="H104" s="74" t="s">
+        <v>984</v>
+      </c>
+      <c r="I104" s="74" t="s">
+        <v>984</v>
+      </c>
+      <c r="J104" s="76"/>
+      <c r="K104" s="146"/>
+      <c r="L104" s="146"/>
+      <c r="M104" s="146"/>
+      <c r="N104" s="146"/>
+      <c r="O104" s="146"/>
+      <c r="P104" s="146"/>
+      <c r="Q104" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="R104" s="76" t="s">
+        <v>259</v>
+      </c>
+      <c r="T104" s="77" t="s">
+        <v>255</v>
+      </c>
+      <c r="U104" s="76"/>
+      <c r="V104" s="76"/>
+      <c r="W104" s="76"/>
+    </row>
+    <row r="105" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="A105" s="13">
         <v>42737</v>
       </c>
-      <c r="B104" s="13"/>
-      <c r="C104" s="15" t="s">
+      <c r="B105" s="13"/>
+      <c r="C105" s="15" t="s">
         <v>1334</v>
       </c>
-      <c r="D104" s="10" t="s">
+      <c r="D105" s="10" t="s">
         <v>1012</v>
       </c>
-      <c r="E104" s="10" t="s">
+      <c r="E105" s="10" t="s">
         <v>956</v>
       </c>
-      <c r="F104" s="10" t="s">
+      <c r="F105" s="10" t="s">
         <v>956</v>
       </c>
-      <c r="G104" s="127">
+      <c r="G105" s="127">
         <v>1</v>
       </c>
-      <c r="H104" s="10"/>
-      <c r="I104" s="10" t="s">
+      <c r="H105" s="10"/>
+      <c r="I105" s="10" t="s">
         <v>888</v>
       </c>
-      <c r="J104" s="10"/>
-      <c r="K104" s="144"/>
-      <c r="L104" s="144"/>
-      <c r="M104" s="144"/>
-      <c r="N104" s="144"/>
-      <c r="O104" s="144"/>
-      <c r="P104" s="144"/>
-      <c r="Q104" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R104" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="S104" s="41"/>
-      <c r="T104" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="U104" s="10"/>
-      <c r="V104" s="10"/>
-      <c r="W104" s="10"/>
-    </row>
-    <row r="105" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
-      <c r="A105" s="13"/>
-      <c r="B105" s="13"/>
-      <c r="C105" s="15"/>
-      <c r="D105" s="10"/>
-      <c r="E105" s="10"/>
-      <c r="F105" s="10"/>
-      <c r="G105" s="127"/>
-      <c r="H105" s="10"/>
-      <c r="I105" s="10"/>
       <c r="J105" s="10"/>
-      <c r="K105" s="147"/>
+      <c r="K105" s="144"/>
       <c r="L105" s="144"/>
       <c r="M105" s="144"/>
       <c r="N105" s="144"/>
       <c r="O105" s="144"/>
       <c r="P105" s="144"/>
-      <c r="Q105" s="10"/>
-      <c r="R105" s="10"/>
+      <c r="Q105" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="R105" s="10" t="s">
+        <v>259</v>
+      </c>
       <c r="S105" s="41"/>
-      <c r="T105" s="41"/>
+      <c r="T105" s="41" t="s">
+        <v>255</v>
+      </c>
       <c r="U105" s="10"/>
       <c r="V105" s="10"/>
       <c r="W105" s="10"/>
@@ -23981,6 +24084,31 @@
       <c r="U110" s="10"/>
       <c r="V110" s="10"/>
       <c r="W110" s="10"/>
+    </row>
+    <row r="111" spans="1:23" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="A111" s="13"/>
+      <c r="B111" s="13"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="10"/>
+      <c r="G111" s="127"/>
+      <c r="H111" s="10"/>
+      <c r="I111" s="10"/>
+      <c r="J111" s="10"/>
+      <c r="K111" s="147"/>
+      <c r="L111" s="144"/>
+      <c r="M111" s="144"/>
+      <c r="N111" s="144"/>
+      <c r="O111" s="144"/>
+      <c r="P111" s="144"/>
+      <c r="Q111" s="10"/>
+      <c r="R111" s="10"/>
+      <c r="S111" s="41"/>
+      <c r="T111" s="41"/>
+      <c r="U111" s="10"/>
+      <c r="V111" s="10"/>
+      <c r="W111" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -55785,7 +55913,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -57007,9 +57135,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IO234"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P200" sqref="P200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -66215,8 +66343,8 @@
   <dimension ref="A1:T128"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="3" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>

</xml_diff>